<commit_message>
add MP2015 for retirees, w/ consistency issue
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0BA844-6761-4D9C-8783-88339EF1C497}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8564F223-5AC3-469C-AC74-52B8CB51C82F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="125">
   <si>
     <t>runname</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>scale_sal_HighYosUp</t>
+  </si>
+  <si>
+    <t>Sensitivity test parameters</t>
   </si>
 </sst>
 </file>
@@ -1125,11 +1128,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AX11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10:E11"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,9 +1182,11 @@
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
+      <c r="F3" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="30" t="s">
         <v>100</v>
       </c>
@@ -1259,13 +1264,13 @@
       <c r="E4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="23" t="s">
         <v>116</v>
       </c>
       <c r="I4" s="28" t="s">
@@ -2100,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add deterministic returns in near future years
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C85C9E-9C3A-4C48-839D-8BAC855B0189}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06846C6E-53CE-49F4-9F8E-18BA28AD989A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>runname</t>
   </si>
@@ -235,9 +235,6 @@
     <t>15 years of low returns</t>
   </si>
   <si>
-    <t>Assumption achived</t>
-  </si>
-  <si>
     <t>cd</t>
   </si>
   <si>
@@ -464,6 +461,42 @@
   </si>
   <si>
     <t>TDA assets</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
+  </si>
+  <si>
+    <t>2017-2018</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>2020-2045</t>
+  </si>
+  <si>
+    <t>internal</t>
+  </si>
+  <si>
+    <t>TDA_type</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>TDA_smooth</t>
+  </si>
+  <si>
+    <t>TDA_amort</t>
+  </si>
+  <si>
+    <t>TDA_smooth_method</t>
+  </si>
+  <si>
+    <t>w.TDA</t>
+  </si>
+  <si>
+    <t>method2</t>
   </si>
 </sst>
 </file>
@@ -1157,13 +1190,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AX11"/>
+  <dimension ref="A3:BC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="AC5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AO15" sqref="AO15"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,262 +1209,286 @@
     <col min="7" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="29.140625" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="14.28515625" customWidth="1"/>
-    <col min="19" max="21" width="19.7109375" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.85546875" customWidth="1"/>
-    <col min="25" max="25" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14" customWidth="1"/>
-    <col min="31" max="31" width="13.42578125" customWidth="1"/>
-    <col min="32" max="32" width="12.5703125" customWidth="1"/>
-    <col min="33" max="33" width="14.85546875" customWidth="1"/>
-    <col min="38" max="38" width="12" customWidth="1"/>
-    <col min="39" max="39" width="12.28515625" customWidth="1"/>
-    <col min="42" max="42" width="15.140625" customWidth="1"/>
-    <col min="43" max="44" width="16.5703125" customWidth="1"/>
-    <col min="45" max="45" width="12" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.28515625" customWidth="1"/>
-    <col min="49" max="49" width="11.42578125" customWidth="1"/>
-    <col min="50" max="50" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="14.28515625" customWidth="1"/>
+    <col min="24" max="26" width="19.7109375" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" customWidth="1"/>
+    <col min="43" max="43" width="12" customWidth="1"/>
+    <col min="44" max="44" width="12.28515625" customWidth="1"/>
+    <col min="47" max="47" width="15.140625" customWidth="1"/>
+    <col min="48" max="49" width="16.5703125" customWidth="1"/>
+    <col min="50" max="50" width="12" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="18" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.28515625" customWidth="1"/>
+    <col min="54" max="54" width="11.42578125" customWidth="1"/>
+    <col min="55" max="55" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:50" s="38" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" s="38" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
       <c r="F3" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
       <c r="I3" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" s="30"/>
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
-      <c r="O3" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="32" t="s">
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="T3" s="32"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="33" t="s">
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="33"/>
+      <c r="AE3" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG3" s="36"/>
-      <c r="AH3" s="36"/>
-      <c r="AI3" s="36"/>
-      <c r="AJ3" s="36"/>
-      <c r="AK3" s="36"/>
-      <c r="AL3" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="AM3" s="32"/>
-      <c r="AN3" s="32"/>
-      <c r="AO3" s="32"/>
-      <c r="AP3" s="32"/>
-      <c r="AQ3" s="32"/>
-      <c r="AR3" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="AS3" s="37"/>
-      <c r="AT3" s="37"/>
-      <c r="AU3" s="37"/>
-      <c r="AV3" s="37"/>
-      <c r="AW3" s="37"/>
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="34"/>
+      <c r="AH3" s="34"/>
+      <c r="AI3" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ3" s="35"/>
+      <c r="AK3" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL3" s="36"/>
+      <c r="AM3" s="36"/>
+      <c r="AN3" s="36"/>
+      <c r="AO3" s="36"/>
+      <c r="AP3" s="36"/>
+      <c r="AQ3" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR3" s="32"/>
+      <c r="AS3" s="32"/>
+      <c r="AT3" s="32"/>
+      <c r="AU3" s="32"/>
+      <c r="AV3" s="32"/>
+      <c r="AW3" s="37" t="s">
+        <v>107</v>
+      </c>
       <c r="AX3" s="37"/>
-    </row>
-    <row r="4" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37"/>
+      <c r="BA3" s="37"/>
+      <c r="BB3" s="37"/>
+      <c r="BC3" s="37"/>
+    </row>
+    <row r="4" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="M4" s="28" t="s">
         <v>106</v>
       </c>
       <c r="N4" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="O4" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="P4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q4" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="O4" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="S4" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="R4" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="S4" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="T4" s="22" t="s">
+      <c r="X4" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y4" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG4" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH4" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ4" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="U4" s="22"/>
-      <c r="V4" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="W4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="X4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z4" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA4" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="AB4" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="AC4" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="AD4" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE4" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF4" s="21" t="s">
+      <c r="AK4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="AG4" s="21" t="s">
+      <c r="AL4" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="AH4" s="21" t="s">
+      <c r="AM4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AI4" s="21" t="s">
+      <c r="AN4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="AJ4" s="21" t="s">
+      <c r="AO4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AK4" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL4" s="22" t="s">
+      <c r="AP4" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ4" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR4" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="AM4" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="AN4" s="22" t="s">
+      <c r="AS4" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AO4" s="22" t="s">
+      <c r="AT4" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AP4" s="22" t="s">
+      <c r="AU4" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="AQ4" s="22" t="s">
+      <c r="AV4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="AR4" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="AS4" s="26" t="s">
+      <c r="AW4" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AX4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AT4" s="26" t="s">
+      <c r="AY4" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AU4" s="26" t="s">
+      <c r="AZ4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AV4" s="26" t="s">
+      <c r="BA4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="AW4" s="26" t="s">
+      <c r="BB4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AX4" s="26" t="s">
+      <c r="BC4" s="26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -1443,136 +1500,151 @@
         <v>0.3</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K5" t="s">
-        <v>104</v>
-      </c>
-      <c r="L5">
+      <c r="Q5" t="s">
+        <v>103</v>
+      </c>
+      <c r="R5">
         <v>0.4</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>6</v>
-      </c>
-      <c r="O5">
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>3</v>
       </c>
-      <c r="P5">
+      <c r="U5">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q5">
+      <c r="V5">
         <v>62</v>
       </c>
-      <c r="R5">
+      <c r="W5">
         <v>5</v>
       </c>
-      <c r="S5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T5">
-        <v>0.03</v>
-      </c>
-      <c r="V5" t="s">
-        <v>57</v>
-      </c>
-      <c r="W5" t="s">
-        <v>46</v>
-      </c>
-      <c r="X5">
-        <v>14</v>
+      <c r="X5" t="s">
+        <v>86</v>
       </c>
       <c r="Y5">
         <v>0.03</v>
       </c>
-      <c r="Z5">
+      <c r="AA5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5">
+        <v>14</v>
+      </c>
+      <c r="AD5">
+        <v>0.03</v>
+      </c>
+      <c r="AE5">
         <v>6</v>
       </c>
-      <c r="AA5">
+      <c r="AF5">
         <v>1.2</v>
       </c>
-      <c r="AB5">
+      <c r="AG5">
         <v>0.8</v>
       </c>
-      <c r="AC5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL5" t="s">
         <v>21</v>
       </c>
-      <c r="AH5">
+      <c r="AM5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI5">
+      <c r="AN5">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AJ5" s="3">
+      <c r="AO5" s="3">
         <v>0.12</v>
       </c>
-      <c r="AK5" s="10">
+      <c r="AP5" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AQ5" t="s">
         <v>34</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AR5" t="s">
         <v>34</v>
       </c>
-      <c r="AN5">
+      <c r="AS5">
         <v>0.623</v>
       </c>
-      <c r="AO5">
-        <v>0.623</v>
-      </c>
-      <c r="AR5" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT5" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV5" s="19" t="s">
+      <c r="AT5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="AW5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="19">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AW5" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX5" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="BB5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC5" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>21</v>
@@ -1584,132 +1656,132 @@
         <v>0.3</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="P7">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L7">
+      <c r="Q7" t="s">
+        <v>103</v>
+      </c>
+      <c r="R7">
         <v>0.4</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>6</v>
-      </c>
-      <c r="O7">
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>3</v>
       </c>
-      <c r="P7">
+      <c r="U7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q7">
+      <c r="V7">
         <v>62</v>
       </c>
-      <c r="R7">
+      <c r="W7">
         <v>5</v>
       </c>
-      <c r="S7" t="s">
-        <v>87</v>
-      </c>
-      <c r="T7">
-        <v>0.03</v>
-      </c>
-      <c r="V7" t="s">
-        <v>57</v>
-      </c>
-      <c r="W7" t="s">
-        <v>46</v>
-      </c>
-      <c r="X7">
-        <v>14</v>
+      <c r="X7" t="s">
+        <v>86</v>
       </c>
       <c r="Y7">
         <v>0.03</v>
       </c>
-      <c r="Z7">
+      <c r="AA7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7">
+        <v>14</v>
+      </c>
+      <c r="AD7">
+        <v>0.03</v>
+      </c>
+      <c r="AE7">
         <v>6</v>
       </c>
-      <c r="AA7">
+      <c r="AF7">
         <v>1.2</v>
       </c>
-      <c r="AB7">
+      <c r="AG7">
         <v>0.8</v>
       </c>
-      <c r="AC7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="s">
+      <c r="AH7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="s">
         <v>35</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AL7" t="s">
         <v>21</v>
       </c>
-      <c r="AH7">
+      <c r="AM7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI7">
+      <c r="AN7">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AJ7" s="3">
+      <c r="AO7" s="3">
         <v>0.12</v>
       </c>
-      <c r="AK7" s="10">
+      <c r="AP7" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AQ7" t="s">
         <v>34</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AR7" t="s">
         <v>34</v>
       </c>
-      <c r="AN7">
+      <c r="AS7">
         <v>0.623</v>
       </c>
-      <c r="AO7">
+      <c r="AT7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AR7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="19" t="s">
+      <c r="AW7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ7" s="19">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AW7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX7" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="BB7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC7" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -1721,132 +1793,132 @@
         <v>0.3</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="P8">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K8" t="s">
-        <v>104</v>
-      </c>
-      <c r="L8">
+      <c r="Q8" t="s">
+        <v>103</v>
+      </c>
+      <c r="R8">
         <v>0.4</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>6</v>
-      </c>
-      <c r="O8">
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>3</v>
       </c>
-      <c r="P8">
+      <c r="U8">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q8">
+      <c r="V8">
         <v>62</v>
       </c>
-      <c r="R8">
+      <c r="W8">
         <v>5</v>
       </c>
-      <c r="S8" t="s">
-        <v>87</v>
-      </c>
-      <c r="T8">
-        <v>0.03</v>
-      </c>
-      <c r="V8" t="s">
-        <v>57</v>
-      </c>
-      <c r="W8" t="s">
-        <v>46</v>
-      </c>
-      <c r="X8">
-        <v>14</v>
+      <c r="X8" t="s">
+        <v>86</v>
       </c>
       <c r="Y8">
         <v>0.03</v>
       </c>
-      <c r="Z8">
+      <c r="AA8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC8">
+        <v>14</v>
+      </c>
+      <c r="AD8">
+        <v>0.03</v>
+      </c>
+      <c r="AE8">
         <v>6</v>
       </c>
-      <c r="AA8">
+      <c r="AF8">
         <v>1.2</v>
       </c>
-      <c r="AB8">
+      <c r="AG8">
         <v>0.8</v>
       </c>
-      <c r="AC8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF8" t="s">
+      <c r="AH8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="s">
         <v>35</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AL8" t="s">
         <v>21</v>
       </c>
-      <c r="AH8">
+      <c r="AM8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI8">
+      <c r="AN8">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AJ8" s="3">
+      <c r="AO8" s="3">
         <v>0.12</v>
       </c>
-      <c r="AK8" s="10">
+      <c r="AP8" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AQ8" t="s">
         <v>34</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AR8" t="s">
         <v>34</v>
       </c>
-      <c r="AN8">
+      <c r="AS8">
         <v>0.623</v>
       </c>
-      <c r="AO8">
+      <c r="AT8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AR8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU8" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="19" t="s">
+      <c r="AW8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ8" s="19">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AW8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX8" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="BB8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC8" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1858,132 +1930,132 @@
         <v>0.3</v>
       </c>
       <c r="G10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="P10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K10" t="s">
-        <v>104</v>
-      </c>
-      <c r="L10">
+      <c r="Q10" t="s">
+        <v>103</v>
+      </c>
+      <c r="R10">
         <v>0.4</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>6</v>
-      </c>
-      <c r="O10">
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
         <v>3</v>
       </c>
-      <c r="P10">
+      <c r="U10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q10">
+      <c r="V10">
         <v>62</v>
       </c>
-      <c r="R10">
+      <c r="W10">
         <v>5</v>
       </c>
-      <c r="S10" t="s">
-        <v>87</v>
-      </c>
-      <c r="T10">
-        <v>0.03</v>
-      </c>
-      <c r="V10" t="s">
-        <v>57</v>
-      </c>
-      <c r="W10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X10">
-        <v>14</v>
+      <c r="X10" t="s">
+        <v>86</v>
       </c>
       <c r="Y10">
         <v>0.03</v>
       </c>
-      <c r="Z10">
+      <c r="AA10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC10">
+        <v>14</v>
+      </c>
+      <c r="AD10">
+        <v>0.03</v>
+      </c>
+      <c r="AE10">
         <v>6</v>
       </c>
-      <c r="AA10">
+      <c r="AF10">
         <v>1.2</v>
       </c>
-      <c r="AB10">
+      <c r="AG10">
         <v>0.8</v>
       </c>
-      <c r="AC10" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF10" t="s">
+      <c r="AH10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="s">
         <v>35</v>
       </c>
-      <c r="AG10" t="s">
+      <c r="AL10" t="s">
         <v>21</v>
       </c>
-      <c r="AH10">
+      <c r="AM10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI10">
+      <c r="AN10">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AJ10" s="3">
+      <c r="AO10" s="3">
         <v>0.12</v>
       </c>
-      <c r="AK10" s="10">
+      <c r="AP10" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AQ10" t="s">
         <v>34</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AR10" t="s">
         <v>34</v>
       </c>
-      <c r="AN10">
+      <c r="AS10">
         <v>0.623</v>
       </c>
-      <c r="AO10">
+      <c r="AT10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AR10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU10" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="19" t="s">
+      <c r="AW10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ10" s="19">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AW10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX10" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="BB10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC10" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -1995,135 +2067,135 @@
         <v>0.3</v>
       </c>
       <c r="G11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="J11">
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="P11">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="K11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L11">
+      <c r="Q11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R11">
         <v>0.4</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>6</v>
-      </c>
-      <c r="O11">
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>3</v>
       </c>
-      <c r="P11">
+      <c r="U11">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q11">
+      <c r="V11">
         <v>62</v>
       </c>
-      <c r="R11">
+      <c r="W11">
         <v>5</v>
       </c>
-      <c r="S11" t="s">
-        <v>87</v>
-      </c>
-      <c r="T11">
-        <v>0.03</v>
-      </c>
-      <c r="V11" t="s">
-        <v>57</v>
-      </c>
-      <c r="W11" t="s">
-        <v>46</v>
-      </c>
-      <c r="X11">
-        <v>14</v>
+      <c r="X11" t="s">
+        <v>86</v>
       </c>
       <c r="Y11">
         <v>0.03</v>
       </c>
-      <c r="Z11">
+      <c r="AA11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC11">
+        <v>14</v>
+      </c>
+      <c r="AD11">
+        <v>0.03</v>
+      </c>
+      <c r="AE11">
         <v>6</v>
       </c>
-      <c r="AA11">
+      <c r="AF11">
         <v>1.2</v>
       </c>
-      <c r="AB11">
+      <c r="AG11">
         <v>0.8</v>
       </c>
-      <c r="AC11" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF11" t="s">
+      <c r="AH11" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="s">
         <v>35</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AL11" t="s">
         <v>21</v>
       </c>
-      <c r="AH11">
+      <c r="AM11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AI11">
+      <c r="AN11">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AJ11" s="3">
+      <c r="AO11" s="3">
         <v>0.12</v>
       </c>
-      <c r="AK11" s="10">
+      <c r="AP11" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AQ11" t="s">
         <v>34</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AR11" t="s">
         <v>34</v>
       </c>
-      <c r="AN11">
+      <c r="AS11">
         <v>0.623</v>
       </c>
-      <c r="AO11">
+      <c r="AT11">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AR11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AS11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AT11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AU11" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="19" t="s">
+      <c r="AW11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AZ11" s="19">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AW11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX11" s="39" t="b">
+      <c r="BB11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC11" s="39" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS5:AT8 I10:I11 AS10:AT11 E5:E8 I5:I8 E10:E11" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX5:AY8 I5:I8 AX10:AY11 E5:E8 E10:E11 I10:I11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF5:AF8 AF10:AF11" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK5:AK8 AK10:AK11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2137,7 +2209,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2220,7 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -2160,22 +2232,22 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2217,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,121 +2333,203 @@
         <v>21</v>
       </c>
       <c r="B2" s="4">
-        <v>7.9200000000000007E-2</v>
+        <v>0.13</v>
       </c>
       <c r="C2" s="3">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
-        <v>7.1999999999999995E-2</v>
+        <f>F2</f>
+        <v>0.13</v>
       </c>
       <c r="F2" s="15">
         <f>B2 - C2^2/2</f>
-        <v>7.2000000000000008E-2</v>
+        <v>0.13</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>5.7200000000000001E-2</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.128</v>
       </c>
       <c r="C3" s="3">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f>B3-C3^2/2</f>
-        <v>0.05</v>
+        <f t="shared" ref="E3:E5" si="0">F3</f>
+        <v>0.128</v>
       </c>
       <c r="F3" s="15">
         <f>B3 - C3^2/2</f>
-        <v>0.05</v>
-      </c>
-      <c r="G3" t="s">
-        <v>55</v>
+        <v>0.128</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>7.22E-2</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.05</v>
       </c>
       <c r="C4" s="3">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
-        <f>B4-C4^2/2</f>
-        <v>6.5000000000000002E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.05</v>
       </c>
       <c r="F4" s="15">
         <f>B4 - C4^2/2</f>
-        <v>6.5000000000000002E-2</v>
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>7.9200000000000007E-2</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="4">
+        <v>7.7200000000000005E-2</v>
       </c>
       <c r="C5" s="3">
         <v>0.12</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4">
-        <f>B5-C5^2/2</f>
-        <v>7.2000000000000008E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F5" s="15">
         <f>B5 - C5^2/2</f>
-        <v>7.2000000000000008E-2</v>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="9">
-        <v>8.6790000000000006E-2</v>
-      </c>
-      <c r="C6" s="10">
-        <v>0.17199999999999999</v>
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.12</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4">
         <f>B6-C6^2/2</f>
-        <v>7.1998000000000006E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F6" s="15">
         <f>B6 - C6^2/2</f>
+        <v>0.05</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>7.22E-2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4">
+        <f>B7-C7^2/2</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="F7" s="15">
+        <f>B7 - C7^2/2</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>7.9200000000000007E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4">
+        <f>B8-C8^2/2</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
+      <c r="F8" s="15">
+        <f>B8 - C8^2/2</f>
+        <v>7.2000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8.6790000000000006E-2</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4">
+        <f>B9-C9^2/2</f>
         <v>7.1998000000000006E-2</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F9" s="15">
+        <f>B9 - C9^2/2</f>
+        <v>7.1998000000000006E-2</v>
+      </c>
+      <c r="G9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f>0.07+0.12^2/2</f>
+        <v>7.7200000000000005E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2404,11 +2558,11 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2417,14 +2571,14 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="40"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>42</v>
@@ -2463,7 +2617,7 @@
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="12">
         <v>11.58</v>
@@ -2508,7 +2662,7 @@
     </row>
     <row r="10" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="12">
         <v>42.24</v>
@@ -2530,7 +2684,7 @@
     </row>
     <row r="11" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="12">
         <v>3.76</v>
@@ -2764,7 +2918,7 @@
     </row>
     <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="12">
         <v>4.343</v>
@@ -2786,7 +2940,7 @@
     </row>
     <row r="27" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="6">
         <v>13.5</v>
@@ -2806,7 +2960,7 @@
     </row>
     <row r="28" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="6">
         <v>14.28</v>
@@ -2824,7 +2978,7 @@
     </row>
     <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -2925,29 +3079,29 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
         <v>128</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
         <v>129</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>131</v>
-      </c>
-      <c r="F3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="41">
         <v>70000777</v>
@@ -2961,7 +3115,7 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="41">
         <v>73323430</v>

</xml_diff>

<commit_message>
figures for Dec 15 draft
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5099673-8EE1-4C63-9E3F-BF821A02F86C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6179D73-C37E-443E-AAFA-8972FA93B9BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="AE4" authorId="0" shapeId="0" xr:uid="{D91F68BF-928B-4B3B-9F98-4B2FFAC0BBBC}">
+    <comment ref="AF4" authorId="0" shapeId="0" xr:uid="{D91F68BF-928B-4B3B-9F98-4B2FFAC0BBBC}">
       <text>
         <r>
           <rPr>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="156">
   <si>
     <t>runname</t>
   </si>
@@ -208,9 +208,6 @@
     <t>AL_pct</t>
   </si>
   <si>
-    <t>simple</t>
-  </si>
-  <si>
     <t>diff</t>
   </si>
   <si>
@@ -569,6 +566,9 @@
   </si>
   <si>
     <t>t4a_C15dA0</t>
+  </si>
+  <si>
+    <t>sensitivity_on</t>
   </si>
 </sst>
 </file>
@@ -1276,13 +1276,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AZ20"/>
+  <dimension ref="A3:BA20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AA24" sqref="AA24"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,276 +1294,281 @@
     <col min="5" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
     <col min="8" max="8" width="29.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="23" width="19.7109375" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.85546875" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14" customWidth="1"/>
-    <col min="33" max="33" width="13.42578125" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" customWidth="1"/>
-    <col min="35" max="35" width="14.85546875" customWidth="1"/>
-    <col min="40" max="40" width="12" customWidth="1"/>
-    <col min="41" max="41" width="12.28515625" customWidth="1"/>
-    <col min="44" max="44" width="15.140625" customWidth="1"/>
-    <col min="45" max="46" width="16.5703125" customWidth="1"/>
-    <col min="47" max="47" width="12" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.28515625" customWidth="1"/>
-    <col min="51" max="51" width="11.42578125" customWidth="1"/>
-    <col min="52" max="52" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="14.28515625" customWidth="1"/>
+    <col min="22" max="24" width="19.7109375" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" customWidth="1"/>
+    <col min="28" max="28" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14" customWidth="1"/>
+    <col min="34" max="34" width="13.42578125" customWidth="1"/>
+    <col min="35" max="35" width="12.5703125" customWidth="1"/>
+    <col min="36" max="36" width="14.85546875" customWidth="1"/>
+    <col min="41" max="41" width="12" customWidth="1"/>
+    <col min="42" max="42" width="12.28515625" customWidth="1"/>
+    <col min="45" max="45" width="15.140625" customWidth="1"/>
+    <col min="46" max="47" width="16.5703125" customWidth="1"/>
+    <col min="48" max="48" width="12" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.28515625" customWidth="1"/>
+    <col min="52" max="52" width="11.42578125" customWidth="1"/>
+    <col min="53" max="53" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:52" s="38" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" s="38" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
       <c r="F3" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
-      <c r="I3" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="30"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="30" t="s">
+        <v>96</v>
+      </c>
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
       <c r="P3" s="30"/>
-      <c r="Q3" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="R3" s="31"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="31" t="s">
+        <v>77</v>
+      </c>
       <c r="S3" s="31"/>
       <c r="T3" s="31"/>
-      <c r="U3" s="32" t="s">
+      <c r="U3" s="31"/>
+      <c r="V3" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="V3" s="32"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y3" s="33"/>
       <c r="Z3" s="33"/>
       <c r="AA3" s="33"/>
-      <c r="AB3" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC3" s="34"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="34" t="s">
+        <v>86</v>
+      </c>
       <c r="AD3" s="34"/>
       <c r="AE3" s="34"/>
-      <c r="AF3" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="AI3" s="36"/>
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="35"/>
+      <c r="AI3" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="AJ3" s="36"/>
       <c r="AK3" s="36"/>
       <c r="AL3" s="36"/>
       <c r="AM3" s="36"/>
-      <c r="AN3" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="AO3" s="32"/>
+      <c r="AN3" s="36"/>
+      <c r="AO3" s="32" t="s">
+        <v>91</v>
+      </c>
       <c r="AP3" s="32"/>
       <c r="AQ3" s="32"/>
       <c r="AR3" s="32"/>
       <c r="AS3" s="32"/>
-      <c r="AT3" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU3" s="37"/>
+      <c r="AT3" s="32"/>
+      <c r="AU3" s="37" t="s">
+        <v>104</v>
+      </c>
       <c r="AV3" s="37"/>
       <c r="AW3" s="37"/>
       <c r="AX3" s="37"/>
       <c r="AY3" s="37"/>
       <c r="AZ3" s="37"/>
-    </row>
-    <row r="4" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BA3" s="37"/>
+    </row>
+    <row r="4" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="25" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="J4" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" s="28" t="s">
+      <c r="O4" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="P4" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="S4" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="V4" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="W4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF4" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH4" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM4" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="AN4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO4" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP4" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS4" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT4" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU4" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="AV4" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW4" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX4" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="AY4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="BA4" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="M4" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="N4" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="P4" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="T4" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="U4" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="V4" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="W4" s="22"/>
-      <c r="X4" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB4" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC4" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="AD4" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE4" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF4" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG4" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI4" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ4" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK4" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="AM4" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="AN4" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="AO4" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP4" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ4" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="AR4" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS4" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT4" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU4" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="AV4" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW4" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="AX4" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY4" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ4" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1572,141 +1577,144 @@
         <v>0.3</v>
       </c>
       <c r="G5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>136</v>
+      <c r="J5" t="b">
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>142</v>
-      </c>
-      <c r="L5">
+        <v>135</v>
+      </c>
+      <c r="L5" t="s">
+        <v>141</v>
+      </c>
+      <c r="M5">
         <v>6</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N5" t="s">
-        <v>101</v>
-      </c>
-      <c r="O5">
+      <c r="O5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5">
         <v>0.45</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>3</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>62</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>5</v>
       </c>
-      <c r="U5" t="s">
-        <v>84</v>
-      </c>
-      <c r="V5">
+      <c r="V5" t="s">
+        <v>83</v>
+      </c>
+      <c r="W5">
         <v>0.03</v>
       </c>
-      <c r="X5" t="s">
-        <v>55</v>
-      </c>
       <c r="Y5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z5">
+        <v>54</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA5">
         <v>14</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>0.03</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>6</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>1.2</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>0.8</v>
       </c>
-      <c r="AE5" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>134</v>
+      <c r="AF5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="b">
+        <v>0</v>
       </c>
       <c r="AI5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>21</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK5">
+      <c r="AL5">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL5" s="3">
+      <c r="AM5" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM5" s="10">
+      <c r="AN5" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>34</v>
       </c>
       <c r="AO5" t="s">
         <v>34</v>
       </c>
-      <c r="AP5">
+      <c r="AP5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ5">
         <v>0.623</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT5" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU5" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV5" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX5" s="19" t="s">
+      <c r="AW5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY5" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ5" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ5" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA5" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1715,141 +1723,144 @@
         <v>0.3</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6">
+        <v>135</v>
+      </c>
+      <c r="L6" t="s">
+        <v>141</v>
+      </c>
+      <c r="M6">
         <v>6</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N6" t="s">
-        <v>101</v>
-      </c>
-      <c r="O6">
+      <c r="O6" t="s">
+        <v>100</v>
+      </c>
+      <c r="P6">
         <v>0.45</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
       <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>62</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>5</v>
       </c>
-      <c r="U6" t="s">
-        <v>84</v>
-      </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>83</v>
+      </c>
+      <c r="W6">
         <v>0.03</v>
       </c>
-      <c r="X6" t="s">
-        <v>55</v>
-      </c>
       <c r="Y6" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z6">
+        <v>54</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA6">
         <v>14</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>0.03</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>6</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>1.2</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>0.8</v>
       </c>
-      <c r="AE6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>134</v>
+      <c r="AF6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="b">
+        <v>0</v>
       </c>
       <c r="AI6" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>21</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL6" s="3">
+      <c r="AM6" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM6" s="10">
+      <c r="AN6" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>34</v>
       </c>
       <c r="AO6" t="s">
         <v>34</v>
       </c>
-      <c r="AP6">
+      <c r="AP6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ6">
         <v>0.623</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT6" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU6" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV6" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW6" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX6" s="19" t="s">
+      <c r="AW6" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX6" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY6" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ6" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ6" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1858,152 +1869,155 @@
         <v>0.3</v>
       </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>139</v>
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>142</v>
-      </c>
-      <c r="L7">
+        <v>138</v>
+      </c>
+      <c r="L7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M7">
         <v>6</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N7" t="s">
-        <v>101</v>
-      </c>
-      <c r="O7">
+      <c r="O7" t="s">
+        <v>100</v>
+      </c>
+      <c r="P7">
         <v>0.45</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
       <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
         <v>3</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>62</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>5</v>
       </c>
-      <c r="U7" t="s">
-        <v>84</v>
-      </c>
-      <c r="V7">
+      <c r="V7" t="s">
+        <v>83</v>
+      </c>
+      <c r="W7">
         <v>0.03</v>
       </c>
-      <c r="X7" t="s">
-        <v>55</v>
-      </c>
       <c r="Y7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z7">
+        <v>54</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA7">
         <v>14</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>0.03</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>6</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>1.2</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <v>0.8</v>
       </c>
-      <c r="AE7" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>134</v>
+      <c r="AF7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="b">
+        <v>0</v>
       </c>
       <c r="AI7" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>21</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL7" s="3">
+      <c r="AM7" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM7" s="10">
+      <c r="AN7" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>34</v>
       </c>
       <c r="AO7" t="s">
         <v>34</v>
       </c>
-      <c r="AP7">
+      <c r="AP7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ7">
         <v>0.623</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT7" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU7" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV7" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW7" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="19" t="s">
+      <c r="AW7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ7" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="10"/>
-      <c r="AT8" s="19"/>
+      <c r="AZ7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA7" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="10"/>
       <c r="AU8" s="19"/>
       <c r="AV8" s="19"/>
       <c r="AW8" s="19"/>
       <c r="AX8" s="19"/>
       <c r="AY8" s="19"/>
-      <c r="AZ8" s="39"/>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ8" s="19"/>
+      <c r="BA8" s="39"/>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -2012,284 +2026,290 @@
         <v>0.3</v>
       </c>
       <c r="G9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>142</v>
-      </c>
-      <c r="L9">
+        <v>135</v>
+      </c>
+      <c r="L9" t="s">
+        <v>141</v>
+      </c>
+      <c r="M9">
         <v>6</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N9" t="s">
-        <v>101</v>
-      </c>
-      <c r="O9">
+      <c r="O9" t="s">
+        <v>100</v>
+      </c>
+      <c r="P9">
         <v>0.45</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
       <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>3</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>62</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>5</v>
       </c>
-      <c r="U9" t="s">
-        <v>84</v>
-      </c>
-      <c r="V9">
+      <c r="V9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W9">
         <v>0.03</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z9" t="s">
         <v>149</v>
       </c>
-      <c r="Y9" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>29</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>0.03</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>6</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>1.2</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>0.8</v>
       </c>
-      <c r="AE9" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>134</v>
+      <c r="AF9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="b">
+        <v>0</v>
       </c>
       <c r="AI9" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ9" t="s">
         <v>21</v>
       </c>
-      <c r="AJ9">
+      <c r="AK9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK9">
+      <c r="AL9">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL9" s="3">
+      <c r="AM9" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM9" s="10">
+      <c r="AN9" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>34</v>
       </c>
       <c r="AO9" t="s">
         <v>34</v>
       </c>
-      <c r="AP9">
+      <c r="AP9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ9">
         <v>0.623</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT9" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU9" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV9" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW9" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="19" t="s">
+      <c r="AW9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY9" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ9" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA9" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0.3</v>
       </c>
       <c r="G10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>142</v>
-      </c>
-      <c r="L10">
+        <v>135</v>
+      </c>
+      <c r="L10" t="s">
+        <v>141</v>
+      </c>
+      <c r="M10">
         <v>6</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N10" t="s">
-        <v>101</v>
-      </c>
-      <c r="O10">
+      <c r="O10" t="s">
+        <v>100</v>
+      </c>
+      <c r="P10">
         <v>0.45</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
       <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <v>3</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>62</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>5</v>
       </c>
-      <c r="U10" t="s">
-        <v>84</v>
-      </c>
-      <c r="V10">
+      <c r="V10" t="s">
+        <v>83</v>
+      </c>
+      <c r="W10">
         <v>0.03</v>
       </c>
-      <c r="X10" t="s">
-        <v>55</v>
-      </c>
       <c r="Y10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z10">
+        <v>54</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA10">
         <v>14</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>0.03</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <v>6</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>1.2</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>0.8</v>
       </c>
-      <c r="AE10" t="s">
-        <v>148</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>134</v>
+      <c r="AF10" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="b">
+        <v>0</v>
       </c>
       <c r="AI10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ10" t="s">
         <v>21</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK10">
+      <c r="AL10">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL10" s="3">
+      <c r="AM10" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM10" s="10">
+      <c r="AN10" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>34</v>
       </c>
       <c r="AO10" t="s">
         <v>34</v>
       </c>
-      <c r="AP10">
+      <c r="AP10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ10">
         <v>0.623</v>
       </c>
-      <c r="AQ10">
+      <c r="AR10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT10" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU10" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV10" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW10" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="19" t="s">
+      <c r="AW10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX10" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ10" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA10" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -2298,284 +2318,290 @@
         <v>0.3</v>
       </c>
       <c r="G11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L11">
+        <v>135</v>
+      </c>
+      <c r="L11" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11">
         <v>6</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N11" t="s">
-        <v>101</v>
-      </c>
-      <c r="O11">
+      <c r="O11" t="s">
+        <v>100</v>
+      </c>
+      <c r="P11">
         <v>0.45</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
       <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
         <v>3</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>62</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>5</v>
       </c>
-      <c r="U11" t="s">
-        <v>84</v>
-      </c>
-      <c r="V11">
+      <c r="V11" t="s">
+        <v>83</v>
+      </c>
+      <c r="W11">
         <v>0.03</v>
       </c>
-      <c r="X11" t="s">
-        <v>55</v>
-      </c>
       <c r="Y11" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z11">
+        <v>54</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA11">
         <v>14</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>0.03</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>6</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>1.2</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>0.8</v>
       </c>
-      <c r="AE11" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>134</v>
+      <c r="AF11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="b">
+        <v>0</v>
       </c>
       <c r="AI11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ11" t="s">
         <v>21</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL11" s="3">
+      <c r="AM11" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM11" s="10">
+      <c r="AN11" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>34</v>
       </c>
       <c r="AO11" t="s">
         <v>34</v>
       </c>
-      <c r="AP11">
+      <c r="AP11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ11">
         <v>0.623</v>
       </c>
-      <c r="AQ11">
+      <c r="AR11">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT11" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU11" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV11" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW11" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="19" t="s">
+      <c r="AW11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX11" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ11" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ11" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA11" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0.3</v>
       </c>
       <c r="G12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>142</v>
-      </c>
-      <c r="L12">
+        <v>135</v>
+      </c>
+      <c r="L12" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12">
         <v>6</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N12" t="s">
-        <v>101</v>
-      </c>
-      <c r="O12">
+      <c r="O12" t="s">
+        <v>100</v>
+      </c>
+      <c r="P12">
         <v>0.45</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
       <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <v>3</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>62</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>5</v>
       </c>
-      <c r="U12" t="s">
-        <v>84</v>
-      </c>
-      <c r="V12">
+      <c r="V12" t="s">
+        <v>83</v>
+      </c>
+      <c r="W12">
         <v>0.03</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z12" t="s">
         <v>149</v>
       </c>
-      <c r="Y12" t="s">
-        <v>150</v>
-      </c>
-      <c r="Z12">
+      <c r="AA12">
         <v>14</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>0.03</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>6</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>1.2</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>0.8</v>
       </c>
-      <c r="AE12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>134</v>
+      <c r="AF12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12" t="b">
+        <v>0</v>
       </c>
       <c r="AI12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>21</v>
       </c>
-      <c r="AJ12">
+      <c r="AK12">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK12">
+      <c r="AL12">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL12" s="3">
+      <c r="AM12" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM12" s="10">
+      <c r="AN12" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>34</v>
       </c>
       <c r="AO12" t="s">
         <v>34</v>
       </c>
-      <c r="AP12">
+      <c r="AP12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ12">
         <v>0.623</v>
       </c>
-      <c r="AQ12">
+      <c r="AR12">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT12" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU12" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV12" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW12" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX12" s="19" t="s">
+      <c r="AW12" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY12" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ12" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ12" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA12" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -2584,141 +2610,144 @@
         <v>0.3</v>
       </c>
       <c r="G13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>142</v>
-      </c>
-      <c r="L13">
+        <v>135</v>
+      </c>
+      <c r="L13" t="s">
+        <v>141</v>
+      </c>
+      <c r="M13">
         <v>6</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N13" t="s">
-        <v>101</v>
-      </c>
-      <c r="O13">
+      <c r="O13" t="s">
+        <v>100</v>
+      </c>
+      <c r="P13">
         <v>0.45</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
       <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <v>3</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>62</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>5</v>
       </c>
-      <c r="U13" t="s">
-        <v>84</v>
-      </c>
-      <c r="V13">
+      <c r="V13" t="s">
+        <v>83</v>
+      </c>
+      <c r="W13">
         <v>0.03</v>
       </c>
-      <c r="X13" t="s">
-        <v>55</v>
-      </c>
       <c r="Y13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z13">
+        <v>54</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA13">
         <v>29</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>0.03</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>6</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>1.2</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>0.8</v>
       </c>
-      <c r="AE13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>134</v>
+      <c r="AF13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG13">
+        <v>0</v>
+      </c>
+      <c r="AH13" t="b">
+        <v>0</v>
       </c>
       <c r="AI13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>21</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK13">
+      <c r="AL13">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL13" s="3">
+      <c r="AM13" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM13" s="10">
+      <c r="AN13" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>34</v>
       </c>
       <c r="AO13" t="s">
         <v>34</v>
       </c>
-      <c r="AP13">
+      <c r="AP13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ13">
         <v>0.623</v>
       </c>
-      <c r="AQ13">
+      <c r="AR13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT13" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU13" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV13" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW13" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX13" s="19" t="s">
+      <c r="AW13" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY13" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ13" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ13" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA13" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -2727,142 +2756,145 @@
         <v>0.3</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>136</v>
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>142</v>
-      </c>
-      <c r="L14">
+        <v>135</v>
+      </c>
+      <c r="L14" t="s">
+        <v>141</v>
+      </c>
+      <c r="M14">
         <v>6</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N14" t="s">
-        <v>101</v>
-      </c>
-      <c r="O14">
+      <c r="O14" t="s">
+        <v>100</v>
+      </c>
+      <c r="P14">
         <v>0.45</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
         <v>3</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>62</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>5</v>
       </c>
-      <c r="U14" t="s">
-        <v>84</v>
-      </c>
-      <c r="V14">
+      <c r="V14" t="s">
+        <v>83</v>
+      </c>
+      <c r="W14">
         <v>0.03</v>
       </c>
-      <c r="X14" t="s">
-        <v>149</v>
-      </c>
       <c r="Y14" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z14">
+        <v>148</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA14">
         <v>14</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>0.03</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>6</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>1.2</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>0.8</v>
       </c>
-      <c r="AE14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
-      <c r="AG14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>134</v>
+      <c r="AF14" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG14">
+        <v>0</v>
+      </c>
+      <c r="AH14" t="b">
+        <v>0</v>
       </c>
       <c r="AI14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ14" t="s">
         <v>21</v>
       </c>
-      <c r="AJ14">
+      <c r="AK14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK14">
+      <c r="AL14">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL14" s="3">
+      <c r="AM14" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM14" s="10">
+      <c r="AN14" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>34</v>
       </c>
       <c r="AO14" t="s">
         <v>34</v>
       </c>
-      <c r="AP14">
+      <c r="AP14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ14">
         <v>0.623</v>
       </c>
-      <c r="AQ14">
+      <c r="AR14">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT14" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU14" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV14" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW14" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX14" s="19" t="s">
+      <c r="AW14" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX14" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY14" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ14" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="AL15" s="3"/>
+      <c r="AZ14" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA14" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AM15" s="3"/>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AN15" s="3"/>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
@@ -2874,570 +2906,582 @@
         <v>0.3</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
       </c>
-      <c r="J16" t="s">
-        <v>136</v>
+      <c r="J16" t="b">
+        <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>142</v>
-      </c>
-      <c r="L16">
+        <v>135</v>
+      </c>
+      <c r="L16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M16">
         <v>6</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N16" t="s">
-        <v>101</v>
-      </c>
-      <c r="O16">
+      <c r="O16" t="s">
+        <v>100</v>
+      </c>
+      <c r="P16">
         <v>0.45</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
       <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
         <v>3</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>62</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>5</v>
       </c>
-      <c r="U16" t="s">
-        <v>84</v>
-      </c>
-      <c r="V16">
+      <c r="V16" t="s">
+        <v>83</v>
+      </c>
+      <c r="W16">
         <v>0.03</v>
       </c>
-      <c r="X16" t="s">
-        <v>55</v>
-      </c>
       <c r="Y16" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z16">
+        <v>54</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA16">
         <v>14</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>0.03</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>6</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>1.2</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>0.8</v>
       </c>
-      <c r="AE16" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF16">
-        <v>0</v>
-      </c>
-      <c r="AG16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>35</v>
+      <c r="AF16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16" t="b">
+        <v>0</v>
       </c>
       <c r="AI16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ16" t="s">
         <v>21</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL16" s="3">
+      <c r="AM16" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM16" s="10">
+      <c r="AN16" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>34</v>
       </c>
       <c r="AO16" t="s">
         <v>34</v>
       </c>
-      <c r="AP16">
+      <c r="AP16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ16">
         <v>0.623</v>
       </c>
-      <c r="AQ16">
+      <c r="AR16">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT16" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU16" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV16" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW16" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX16" s="19" t="s">
+      <c r="AW16" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX16" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY16" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY16" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ16" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ16" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA16" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0.3</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="J17" t="s">
-        <v>136</v>
+      <c r="J17" t="b">
+        <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>142</v>
-      </c>
-      <c r="L17">
+        <v>135</v>
+      </c>
+      <c r="L17" t="s">
+        <v>141</v>
+      </c>
+      <c r="M17">
         <v>6</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N17" t="s">
-        <v>101</v>
-      </c>
-      <c r="O17">
+      <c r="O17" t="s">
+        <v>100</v>
+      </c>
+      <c r="P17">
         <v>0.45</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
       <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
         <v>3</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>62</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>5</v>
       </c>
-      <c r="U17" t="s">
-        <v>84</v>
-      </c>
-      <c r="V17">
+      <c r="V17" t="s">
+        <v>83</v>
+      </c>
+      <c r="W17">
         <v>0.03</v>
       </c>
-      <c r="X17" t="s">
-        <v>55</v>
-      </c>
       <c r="Y17" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z17">
+        <v>54</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA17">
         <v>14</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>0.03</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>6</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>1.2</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>0.8</v>
       </c>
-      <c r="AE17" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-      <c r="AG17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>35</v>
+      <c r="AF17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17" t="b">
+        <v>0</v>
       </c>
       <c r="AI17" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>21</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL17" s="3">
+      <c r="AM17" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM17" s="10">
+      <c r="AN17" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>34</v>
       </c>
       <c r="AO17" t="s">
         <v>34</v>
       </c>
-      <c r="AP17">
+      <c r="AP17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ17">
         <v>0.623</v>
       </c>
-      <c r="AQ17">
+      <c r="AR17">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT17" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU17" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV17" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW17" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX17" s="19" t="s">
+      <c r="AW17" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX17" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY17" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ17" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ17" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA17" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0.3</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
       </c>
-      <c r="J19" t="s">
-        <v>136</v>
+      <c r="J19" t="b">
+        <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>142</v>
-      </c>
-      <c r="L19">
+        <v>135</v>
+      </c>
+      <c r="L19" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19">
         <v>6</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N19" t="s">
-        <v>101</v>
-      </c>
-      <c r="O19">
+      <c r="O19" t="s">
+        <v>100</v>
+      </c>
+      <c r="P19">
         <v>0.45</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
       <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
         <v>3</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>62</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>5</v>
       </c>
-      <c r="U19" t="s">
-        <v>84</v>
-      </c>
-      <c r="V19">
+      <c r="V19" t="s">
+        <v>83</v>
+      </c>
+      <c r="W19">
         <v>0.03</v>
       </c>
-      <c r="X19" t="s">
-        <v>55</v>
-      </c>
       <c r="Y19" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z19">
+        <v>54</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA19">
         <v>14</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>0.03</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>6</v>
       </c>
-      <c r="AC19">
+      <c r="AD19">
         <v>1.2</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>0.8</v>
       </c>
-      <c r="AE19" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF19">
-        <v>0</v>
-      </c>
-      <c r="AG19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>35</v>
+      <c r="AF19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19" t="b">
+        <v>0</v>
       </c>
       <c r="AI19" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ19" t="s">
         <v>21</v>
       </c>
-      <c r="AJ19">
+      <c r="AK19">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK19">
+      <c r="AL19">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL19" s="3">
+      <c r="AM19" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM19" s="10">
+      <c r="AN19" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN19" t="s">
-        <v>34</v>
       </c>
       <c r="AO19" t="s">
         <v>34</v>
       </c>
-      <c r="AP19">
+      <c r="AP19" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ19">
         <v>0.623</v>
       </c>
-      <c r="AQ19">
+      <c r="AR19">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT19" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU19" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV19" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW19" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX19" s="19" t="s">
+      <c r="AW19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX19" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY19" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY19" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ19" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AZ19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA19" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
         <v>21</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0.3</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="J20" t="s">
-        <v>136</v>
+      <c r="J20" t="b">
+        <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>142</v>
-      </c>
-      <c r="L20">
+        <v>135</v>
+      </c>
+      <c r="L20" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20">
         <v>6</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="N20" t="s">
-        <v>101</v>
-      </c>
-      <c r="O20">
+      <c r="O20" t="s">
+        <v>100</v>
+      </c>
+      <c r="P20">
         <v>0.45</v>
       </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
       <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
         <v>3</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>62</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>5</v>
       </c>
-      <c r="U20" t="s">
-        <v>84</v>
-      </c>
-      <c r="V20">
+      <c r="V20" t="s">
+        <v>83</v>
+      </c>
+      <c r="W20">
         <v>0.03</v>
       </c>
-      <c r="X20" t="s">
-        <v>55</v>
-      </c>
       <c r="Y20" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z20">
+        <v>54</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA20">
         <v>14</v>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <v>0.03</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <v>6</v>
       </c>
-      <c r="AC20">
+      <c r="AD20">
         <v>1.2</v>
       </c>
-      <c r="AD20">
+      <c r="AE20">
         <v>0.8</v>
       </c>
-      <c r="AE20" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF20">
-        <v>0</v>
-      </c>
-      <c r="AG20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>35</v>
+      <c r="AF20" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20" t="b">
+        <v>0</v>
       </c>
       <c r="AI20" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ20" t="s">
         <v>21</v>
       </c>
-      <c r="AJ20">
+      <c r="AK20">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AK20">
+      <c r="AL20">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AL20" s="3">
+      <c r="AM20" s="3">
         <v>0.12</v>
       </c>
-      <c r="AM20" s="10">
+      <c r="AN20" s="10">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>34</v>
       </c>
       <c r="AO20" t="s">
         <v>34</v>
       </c>
-      <c r="AP20">
+      <c r="AP20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ20">
         <v>0.623</v>
       </c>
-      <c r="AQ20">
+      <c r="AR20">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AT20" s="19" t="b">
-        <v>1</v>
-      </c>
       <c r="AU20" s="19" t="b">
         <v>1</v>
       </c>
       <c r="AV20" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="AW20" s="19">
-        <v>0</v>
-      </c>
-      <c r="AX20" s="19" t="s">
+      <c r="AW20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX20" s="19">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AY20" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="AZ20" s="39" t="b">
+      <c r="AZ20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA20" s="39" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU19:AV20 I19:I20 E19:E20 AU5:AV17 I5:I17 E5:E17" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV19:AW20 J19:J20 E5:E17 AV5:AW17 J5:J17 E19:E20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH19:AH20 AH5:AH17" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI5:AI17 AI19:AI20" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3463,7 +3507,7 @@
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -3475,22 +3519,22 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3593,7 +3637,7 @@
         <v>0.13</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3618,7 +3662,7 @@
         <v>0.128</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3643,7 +3687,7 @@
         <v>0.02</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3668,7 +3712,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3693,7 +3737,7 @@
         <v>0.05</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3762,7 +3806,7 @@
         <v>7.1998000000000006E-2</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3797,15 +3841,15 @@
   <sheetData>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3814,31 +3858,31 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="43"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="12">
         <v>40.130000000000003</v>
@@ -3860,7 +3904,7 @@
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="12">
         <v>11.58</v>
@@ -3882,7 +3926,7 @@
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="12">
         <f>C7-C8</f>
@@ -3905,7 +3949,7 @@
     </row>
     <row r="10" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="12">
         <v>42.24</v>
@@ -3927,7 +3971,7 @@
     </row>
     <row r="11" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="12">
         <v>3.76</v>
@@ -3965,7 +4009,7 @@
     </row>
     <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="12">
         <f>SUM(C9,C10,C11)</f>
@@ -3997,7 +4041,7 @@
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="12">
         <v>67.38</v>
@@ -4015,7 +4059,7 @@
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="12">
         <v>64.25</v>
@@ -4033,7 +4077,7 @@
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="12">
         <f>C14-C16</f>
@@ -4068,7 +4112,7 @@
     </row>
     <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="16">
         <f>11.582186/111.581756</f>
@@ -4091,7 +4135,7 @@
     </row>
     <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6">
         <v>1.07</v>
@@ -4113,7 +4157,7 @@
     </row>
     <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="16">
         <v>7.4999999999999997E-2</v>
@@ -4133,7 +4177,7 @@
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6">
         <v>6</v>
@@ -4161,7 +4205,7 @@
     </row>
     <row r="26" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="12">
         <v>4.343</v>
@@ -4183,7 +4227,7 @@
     </row>
     <row r="27" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6">
         <v>13.5</v>
@@ -4203,7 +4247,7 @@
     </row>
     <row r="28" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="6">
         <v>14.28</v>
@@ -4221,7 +4265,7 @@
     </row>
     <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -4322,29 +4366,29 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
         <v>125</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" t="s">
         <v>126</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>128</v>
-      </c>
-      <c r="F3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="40">
         <v>70000777</v>
@@ -4362,7 +4406,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="40">
         <v>73323430</v>

</xml_diff>

<commit_message>
modify IndivLiab for PVFEEC
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20507E7-291B-4381-AB7E-42A9F57A4463}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0815F2-033A-4ABA-B34B-127B84A52317}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,7 +1271,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1706,7 @@
         <v>139</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0.3</v>
@@ -3035,7 +3035,7 @@
         <v>21</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0.3</v>
@@ -3181,7 +3181,7 @@
         <v>21</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0.3</v>
@@ -3327,7 +3327,7 @@
         <v>21</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0.3</v>
@@ -3568,7 +3568,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix asset smoothing issue
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE867CDC-F114-457A-845C-A168DAC2384D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274CF2EF-4361-4A9F-8F2A-00CB6F41487D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="181">
   <si>
     <t>runname</t>
   </si>
@@ -640,6 +640,9 @@
   </si>
   <si>
     <t>t4a_TDAamortAS_OYLM_DF2</t>
+  </si>
+  <si>
+    <t>corridor</t>
   </si>
 </sst>
 </file>
@@ -888,10 +891,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1345,13 +1348,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:BC40"/>
+  <dimension ref="A3:BD40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N36" sqref="N36"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,23 +1386,24 @@
     <col min="32" max="32" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14" customWidth="1"/>
-    <col min="36" max="36" width="13.42578125" customWidth="1"/>
-    <col min="37" max="37" width="12.5703125" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" customWidth="1"/>
-    <col min="43" max="43" width="12" customWidth="1"/>
-    <col min="44" max="44" width="12.28515625" customWidth="1"/>
-    <col min="47" max="47" width="15.140625" customWidth="1"/>
-    <col min="48" max="49" width="16.5703125" customWidth="1"/>
-    <col min="50" max="50" width="12" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="12.28515625" customWidth="1"/>
-    <col min="54" max="54" width="11.42578125" customWidth="1"/>
-    <col min="55" max="55" width="14.28515625" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" customWidth="1"/>
+    <col min="36" max="36" width="14" customWidth="1"/>
+    <col min="37" max="37" width="13.42578125" customWidth="1"/>
+    <col min="38" max="38" width="12.5703125" customWidth="1"/>
+    <col min="39" max="39" width="14.85546875" customWidth="1"/>
+    <col min="44" max="44" width="12" customWidth="1"/>
+    <col min="45" max="45" width="12.28515625" customWidth="1"/>
+    <col min="48" max="48" width="15.140625" customWidth="1"/>
+    <col min="49" max="50" width="16.5703125" customWidth="1"/>
+    <col min="51" max="51" width="12" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="18" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.28515625" customWidth="1"/>
+    <col min="55" max="55" width="11.42578125" customWidth="1"/>
+    <col min="56" max="56" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:55" s="36" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" s="36" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="27"/>
       <c r="B3" s="27"/>
       <c r="C3" s="27"/>
@@ -1448,37 +1452,38 @@
       <c r="AF3" s="32"/>
       <c r="AG3" s="32"/>
       <c r="AH3" s="32"/>
-      <c r="AI3" s="33" t="s">
+      <c r="AI3" s="32"/>
+      <c r="AJ3" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="AJ3" s="33"/>
-      <c r="AK3" s="34" t="s">
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="AL3" s="34"/>
       <c r="AM3" s="34"/>
       <c r="AN3" s="34"/>
       <c r="AO3" s="34"/>
       <c r="AP3" s="34"/>
-      <c r="AQ3" s="30" t="s">
+      <c r="AQ3" s="34"/>
+      <c r="AR3" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="AR3" s="30"/>
       <c r="AS3" s="30"/>
       <c r="AT3" s="30"/>
       <c r="AU3" s="30"/>
       <c r="AV3" s="30"/>
-      <c r="AW3" s="35" t="s">
+      <c r="AW3" s="30"/>
+      <c r="AX3" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="AX3" s="35"/>
       <c r="AY3" s="35"/>
       <c r="AZ3" s="35"/>
       <c r="BA3" s="35"/>
       <c r="BB3" s="35"/>
       <c r="BC3" s="35"/>
-    </row>
-    <row r="4" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD3" s="35"/>
+    </row>
+    <row r="4" spans="1:56" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>0</v>
       </c>
@@ -1579,71 +1584,74 @@
       <c r="AH4" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AI4" s="25" t="s">
+      <c r="AI4" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="AJ4" s="25" t="s">
+      <c r="AK4" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="AK4" s="19" t="s">
+      <c r="AL4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AL4" s="19" t="s">
+      <c r="AM4" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AM4" s="19" t="s">
+      <c r="AN4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AN4" s="19" t="s">
+      <c r="AO4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="AO4" s="19" t="s">
+      <c r="AP4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="AP4" s="19" t="s">
+      <c r="AQ4" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="AQ4" s="20" t="s">
+      <c r="AR4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="AR4" s="20" t="s">
+      <c r="AS4" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="AS4" s="20" t="s">
+      <c r="AT4" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="AT4" s="20" t="s">
+      <c r="AU4" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="AU4" s="20" t="s">
+      <c r="AV4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AV4" s="20" t="s">
+      <c r="AW4" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="AW4" s="24" t="s">
+      <c r="AX4" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="AX4" s="24" t="s">
+      <c r="AY4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="AY4" s="24" t="s">
+      <c r="AZ4" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="AZ4" s="24" t="s">
+      <c r="BA4" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="BA4" s="24" t="s">
+      <c r="BB4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="BB4" s="24" t="s">
+      <c r="BC4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="BC4" s="24" t="s">
+      <c r="BD4" s="24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -1737,65 +1745,65 @@
       <c r="AH5" t="s">
         <v>86</v>
       </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="s">
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="s">
         <v>128</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>21</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN5">
+      <c r="AO5">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO5" s="3">
+      <c r="AP5" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP5" s="9">
+      <c r="AQ5" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>32</v>
       </c>
       <c r="AR5" t="s">
         <v>32</v>
       </c>
-      <c r="AS5">
+      <c r="AS5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT5">
         <v>0.623</v>
       </c>
-      <c r="AT5">
+      <c r="AU5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW5" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX5" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY5" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ5" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA5" s="17" t="s">
+      <c r="AZ5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA5" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB5" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC5" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC5" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD5" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -1889,76 +1897,76 @@
       <c r="AH6" t="s">
         <v>86</v>
       </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK6" t="s">
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL6" t="s">
         <v>128</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>21</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO6" s="3">
+      <c r="AP6" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP6" s="9">
+      <c r="AQ6" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>32</v>
       </c>
       <c r="AR6" t="s">
         <v>32</v>
       </c>
-      <c r="AS6">
+      <c r="AS6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT6">
         <v>0.623</v>
       </c>
-      <c r="AT6">
+      <c r="AU6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW6" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX6" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY6" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ6" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA6" s="17" t="s">
+      <c r="AZ6" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB6" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC6" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="9"/>
-      <c r="AW7" s="17"/>
+      <c r="BC6" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD6" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="9"/>
       <c r="AX7" s="17"/>
       <c r="AY7" s="17"/>
       <c r="AZ7" s="17"/>
       <c r="BA7" s="17"/>
       <c r="BB7" s="17"/>
-      <c r="BC7" s="37"/>
-    </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC7" s="17"/>
+      <c r="BD7" s="37"/>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>160</v>
       </c>
@@ -2052,65 +2060,65 @@
       <c r="AH8" t="s">
         <v>86</v>
       </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK8" t="s">
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL8" t="s">
         <v>128</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AM8" t="s">
         <v>21</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN8">
+      <c r="AO8">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO8" s="3">
+      <c r="AP8" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP8" s="9">
+      <c r="AQ8" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>32</v>
       </c>
       <c r="AR8" t="s">
         <v>32</v>
       </c>
-      <c r="AS8">
+      <c r="AS8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT8">
         <v>0.623</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW8" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX8" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY8" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ8" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="17" t="s">
+      <c r="AZ8" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA8" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB8" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC8" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC8" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD8" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -2204,76 +2212,76 @@
       <c r="AH9" t="s">
         <v>86</v>
       </c>
-      <c r="AI9">
-        <v>0</v>
-      </c>
-      <c r="AJ9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="s">
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL9" t="s">
         <v>128</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="AM9" t="s">
         <v>21</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO9" s="3">
+      <c r="AP9" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP9" s="9">
+      <c r="AQ9" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>32</v>
       </c>
       <c r="AR9" t="s">
         <v>32</v>
       </c>
-      <c r="AS9">
+      <c r="AS9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT9">
         <v>0.623</v>
       </c>
-      <c r="AT9">
+      <c r="AU9">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW9" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX9" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY9" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ9" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="17" t="s">
+      <c r="AZ9" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA9" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB9" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC9" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="9"/>
-      <c r="AW10" s="17"/>
+      <c r="BC9" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD9" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="9"/>
       <c r="AX10" s="17"/>
       <c r="AY10" s="17"/>
       <c r="AZ10" s="17"/>
       <c r="BA10" s="17"/>
       <c r="BB10" s="17"/>
-      <c r="BC10" s="37"/>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC10" s="17"/>
+      <c r="BD10" s="37"/>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -2283,7 +2291,7 @@
       <c r="D11" t="s">
         <v>139</v>
       </c>
-      <c r="F11" t="b">
+      <c r="F11" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G11">
@@ -2367,65 +2375,65 @@
       <c r="AH11" t="s">
         <v>86</v>
       </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK11" t="s">
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL11" t="s">
         <v>128</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AM11" t="s">
         <v>21</v>
       </c>
-      <c r="AM11">
+      <c r="AN11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN11">
+      <c r="AO11">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO11" s="3">
+      <c r="AP11" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP11" s="9">
+      <c r="AQ11" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>32</v>
       </c>
       <c r="AR11" t="s">
         <v>32</v>
       </c>
-      <c r="AS11">
+      <c r="AS11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT11">
         <v>0.623</v>
       </c>
-      <c r="AT11">
+      <c r="AU11">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW11" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX11" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY11" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ11" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA11" s="17" t="s">
+      <c r="AZ11" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA11" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB11" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC11" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC11" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD11" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -2435,7 +2443,7 @@
       <c r="D12" t="s">
         <v>139</v>
       </c>
-      <c r="F12" t="b">
+      <c r="F12" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G12">
@@ -2519,65 +2527,65 @@
       <c r="AH12" t="s">
         <v>142</v>
       </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK12" t="s">
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL12" t="s">
         <v>128</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="AM12" t="s">
         <v>21</v>
       </c>
-      <c r="AM12">
+      <c r="AN12">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN12">
+      <c r="AO12">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO12" s="3">
+      <c r="AP12" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP12" s="9">
+      <c r="AQ12" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>32</v>
       </c>
       <c r="AR12" t="s">
         <v>32</v>
       </c>
-      <c r="AS12">
+      <c r="AS12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT12">
         <v>0.623</v>
       </c>
-      <c r="AT12">
+      <c r="AU12">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW12" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX12" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY12" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ12" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA12" s="17" t="s">
+      <c r="AZ12" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA12" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB12" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC12" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC12" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD12" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -2587,7 +2595,7 @@
       <c r="D13" t="s">
         <v>139</v>
       </c>
-      <c r="F13" t="b">
+      <c r="F13" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G13">
@@ -2671,65 +2679,65 @@
       <c r="AH13" t="s">
         <v>86</v>
       </c>
-      <c r="AI13">
-        <v>0</v>
-      </c>
-      <c r="AJ13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK13" t="s">
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL13" t="s">
         <v>128</v>
       </c>
-      <c r="AL13" t="s">
+      <c r="AM13" t="s">
         <v>21</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN13">
+      <c r="AO13">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO13" s="3">
+      <c r="AP13" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP13" s="9">
+      <c r="AQ13" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ13" t="s">
-        <v>32</v>
       </c>
       <c r="AR13" t="s">
         <v>32</v>
       </c>
-      <c r="AS13">
+      <c r="AS13" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT13">
         <v>0.623</v>
       </c>
-      <c r="AT13">
+      <c r="AU13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW13" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX13" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY13" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ13" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA13" s="17" t="s">
+      <c r="AZ13" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA13" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB13" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB13" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC13" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC13" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD13" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -2739,7 +2747,7 @@
       <c r="D14" t="s">
         <v>139</v>
       </c>
-      <c r="F14" t="b">
+      <c r="F14" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G14">
@@ -2823,65 +2831,65 @@
       <c r="AH14" t="s">
         <v>86</v>
       </c>
-      <c r="AI14">
-        <v>0</v>
-      </c>
-      <c r="AJ14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK14" t="s">
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL14" t="s">
         <v>128</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AM14" t="s">
         <v>21</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN14">
+      <c r="AO14">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO14" s="3">
+      <c r="AP14" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP14" s="9">
+      <c r="AQ14" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>32</v>
       </c>
       <c r="AR14" t="s">
         <v>32</v>
       </c>
-      <c r="AS14">
+      <c r="AS14" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT14">
         <v>0.623</v>
       </c>
-      <c r="AT14">
+      <c r="AU14">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW14" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX14" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY14" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ14" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA14" s="17" t="s">
+      <c r="AZ14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA14" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB14" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC14" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC14" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD14" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>146</v>
       </c>
@@ -2891,7 +2899,7 @@
       <c r="D15" t="s">
         <v>139</v>
       </c>
-      <c r="F15" t="b">
+      <c r="F15" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G15">
@@ -2975,65 +2983,65 @@
       <c r="AH15" t="s">
         <v>86</v>
       </c>
-      <c r="AI15">
-        <v>0</v>
-      </c>
-      <c r="AJ15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK15" t="s">
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL15" t="s">
         <v>128</v>
       </c>
-      <c r="AL15" t="s">
+      <c r="AM15" t="s">
         <v>21</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN15">
+      <c r="AO15">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO15" s="3">
+      <c r="AP15" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP15" s="9">
+      <c r="AQ15" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>32</v>
       </c>
       <c r="AR15" t="s">
         <v>32</v>
       </c>
-      <c r="AS15">
+      <c r="AS15" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT15">
         <v>0.623</v>
       </c>
-      <c r="AT15">
+      <c r="AU15">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW15" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX15" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY15" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ15" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA15" s="17" t="s">
+      <c r="AZ15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA15" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB15" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB15" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC15" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC15" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD15" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -3043,7 +3051,7 @@
       <c r="D16" t="s">
         <v>139</v>
       </c>
-      <c r="F16" t="b">
+      <c r="F16" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G16">
@@ -3127,69 +3135,69 @@
       <c r="AH16" t="s">
         <v>86</v>
       </c>
-      <c r="AI16">
-        <v>0</v>
-      </c>
-      <c r="AJ16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK16" t="s">
+      <c r="AJ16">
+        <v>0</v>
+      </c>
+      <c r="AK16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL16" t="s">
         <v>128</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="AM16" t="s">
         <v>21</v>
       </c>
-      <c r="AM16">
+      <c r="AN16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN16">
+      <c r="AO16">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO16" s="3">
+      <c r="AP16" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP16" s="9">
+      <c r="AQ16" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ16" t="s">
-        <v>32</v>
       </c>
       <c r="AR16" t="s">
         <v>32</v>
       </c>
-      <c r="AS16">
+      <c r="AS16" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT16">
         <v>0.623</v>
       </c>
-      <c r="AT16">
+      <c r="AU16">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW16" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX16" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY16" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ16" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA16" s="17" t="s">
+      <c r="AZ16" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA16" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB16" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC16" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AO17" s="3"/>
+      <c r="BC16" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD16" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AP17" s="3"/>
-    </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AQ17" s="3"/>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>166</v>
       </c>
@@ -3283,65 +3291,65 @@
       <c r="AH18" t="s">
         <v>86</v>
       </c>
-      <c r="AI18">
-        <v>0</v>
-      </c>
-      <c r="AJ18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK18" t="s">
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL18" t="s">
         <v>128</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AM18" t="s">
         <v>151</v>
       </c>
-      <c r="AM18">
+      <c r="AN18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN18">
+      <c r="AO18">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO18" s="3">
+      <c r="AP18" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP18" s="9">
+      <c r="AQ18" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ18" t="s">
-        <v>32</v>
       </c>
       <c r="AR18" t="s">
         <v>32</v>
       </c>
-      <c r="AS18">
+      <c r="AS18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT18">
         <v>0.623</v>
       </c>
-      <c r="AT18">
+      <c r="AU18">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW18" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX18" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY18" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ18" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA18" s="17" t="s">
+      <c r="AZ18" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA18" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB18" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC18" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC18" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD18" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>167</v>
       </c>
@@ -3435,65 +3443,65 @@
       <c r="AH19" t="s">
         <v>86</v>
       </c>
-      <c r="AI19">
-        <v>0</v>
-      </c>
-      <c r="AJ19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK19" t="s">
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL19" t="s">
         <v>128</v>
       </c>
-      <c r="AL19" t="s">
+      <c r="AM19" t="s">
         <v>151</v>
       </c>
-      <c r="AM19">
+      <c r="AN19">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN19">
+      <c r="AO19">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO19" s="3">
+      <c r="AP19" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP19" s="9">
+      <c r="AQ19" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ19" t="s">
-        <v>32</v>
       </c>
       <c r="AR19" t="s">
         <v>32</v>
       </c>
-      <c r="AS19">
+      <c r="AS19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT19">
         <v>0.623</v>
       </c>
-      <c r="AT19">
+      <c r="AU19">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW19" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX19" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY19" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ19" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA19" s="17" t="s">
+      <c r="AZ19" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA19" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB19" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC19" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC19" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD19" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -3503,8 +3511,8 @@
       <c r="D21" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="43" t="b">
-        <v>0</v>
+      <c r="F21" s="42" t="b">
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0.3</v>
@@ -3587,65 +3595,65 @@
       <c r="AH21" t="s">
         <v>86</v>
       </c>
-      <c r="AI21">
-        <v>0</v>
-      </c>
-      <c r="AJ21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK21" t="s">
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL21" t="s">
         <v>128</v>
       </c>
-      <c r="AL21" t="s">
+      <c r="AM21" t="s">
         <v>154</v>
       </c>
-      <c r="AM21">
+      <c r="AN21">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN21">
+      <c r="AO21">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO21" s="3">
+      <c r="AP21" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP21" s="9">
+      <c r="AQ21" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ21" t="s">
-        <v>32</v>
       </c>
       <c r="AR21" t="s">
         <v>32</v>
       </c>
-      <c r="AS21">
+      <c r="AS21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT21">
         <v>0.623</v>
       </c>
-      <c r="AT21">
+      <c r="AU21">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW21" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX21" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY21" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ21" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA21" s="17" t="s">
+      <c r="AZ21" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA21" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB21" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB21" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC21" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC21" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD21" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -3655,8 +3663,8 @@
       <c r="D22" t="s">
         <v>161</v>
       </c>
-      <c r="F22" s="43" t="b">
-        <v>0</v>
+      <c r="F22" s="42" t="b">
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0.3</v>
@@ -3739,69 +3747,69 @@
       <c r="AH22" t="s">
         <v>86</v>
       </c>
-      <c r="AI22">
-        <v>0</v>
-      </c>
-      <c r="AJ22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK22" t="s">
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL22" t="s">
         <v>128</v>
       </c>
-      <c r="AL22" t="s">
+      <c r="AM22" t="s">
         <v>154</v>
       </c>
-      <c r="AM22">
+      <c r="AN22">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN22">
+      <c r="AO22">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO22" s="3">
+      <c r="AP22" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP22" s="9">
+      <c r="AQ22" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ22" t="s">
-        <v>32</v>
       </c>
       <c r="AR22" t="s">
         <v>32</v>
       </c>
-      <c r="AS22">
+      <c r="AS22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT22">
         <v>0.623</v>
       </c>
-      <c r="AT22">
+      <c r="AU22">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW22" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX22" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY22" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ22" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA22" s="17" t="s">
+      <c r="AZ22" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA22" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB22" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB22" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC22" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AO23" s="3"/>
+      <c r="BC22" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD22" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AP23" s="3"/>
-    </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AQ23" s="3"/>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>176</v>
       </c>
@@ -3895,65 +3903,65 @@
       <c r="AH24" t="s">
         <v>86</v>
       </c>
-      <c r="AI24">
-        <v>0</v>
-      </c>
-      <c r="AJ24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK24" t="s">
+      <c r="AJ24">
+        <v>0</v>
+      </c>
+      <c r="AK24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL24" t="s">
         <v>128</v>
       </c>
-      <c r="AL24" t="s">
+      <c r="AM24" t="s">
         <v>174</v>
       </c>
-      <c r="AM24">
+      <c r="AN24">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN24">
+      <c r="AO24">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO24" s="3">
+      <c r="AP24" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP24" s="9">
+      <c r="AQ24" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ24" t="s">
-        <v>32</v>
       </c>
       <c r="AR24" t="s">
         <v>32</v>
       </c>
-      <c r="AS24">
+      <c r="AS24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT24">
         <v>0.623</v>
       </c>
-      <c r="AT24">
+      <c r="AU24">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW24" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX24" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY24" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ24" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA24" s="17" t="s">
+      <c r="AZ24" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA24" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB24" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB24" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC24" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC24" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD24" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>177</v>
       </c>
@@ -4047,65 +4055,65 @@
       <c r="AH25" t="s">
         <v>86</v>
       </c>
-      <c r="AI25">
-        <v>0</v>
-      </c>
-      <c r="AJ25" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK25" t="s">
+      <c r="AJ25">
+        <v>0</v>
+      </c>
+      <c r="AK25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL25" t="s">
         <v>128</v>
       </c>
-      <c r="AL25" t="s">
+      <c r="AM25" t="s">
         <v>174</v>
       </c>
-      <c r="AM25">
+      <c r="AN25">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN25">
+      <c r="AO25">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO25" s="3">
+      <c r="AP25" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP25" s="9">
+      <c r="AQ25" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ25" t="s">
-        <v>32</v>
       </c>
       <c r="AR25" t="s">
         <v>32</v>
       </c>
-      <c r="AS25">
+      <c r="AS25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT25">
         <v>0.623</v>
       </c>
-      <c r="AT25">
+      <c r="AU25">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW25" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX25" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY25" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ25" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA25" s="17" t="s">
+      <c r="AZ25" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA25" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB25" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB25" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC25" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC25" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD25" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>178</v>
       </c>
@@ -4115,7 +4123,7 @@
       <c r="D26" t="s">
         <v>138</v>
       </c>
-      <c r="F26" t="b">
+      <c r="F26" s="42" t="b">
         <v>1</v>
       </c>
       <c r="G26">
@@ -4199,65 +4207,65 @@
       <c r="AH26" t="s">
         <v>86</v>
       </c>
-      <c r="AI26">
-        <v>0</v>
-      </c>
-      <c r="AJ26" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK26" t="s">
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL26" t="s">
         <v>128</v>
       </c>
-      <c r="AL26" t="s">
+      <c r="AM26" t="s">
         <v>175</v>
       </c>
-      <c r="AM26">
+      <c r="AN26">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN26">
+      <c r="AO26">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO26" s="3">
+      <c r="AP26" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP26" s="9">
+      <c r="AQ26" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ26" t="s">
-        <v>32</v>
       </c>
       <c r="AR26" t="s">
         <v>32</v>
       </c>
-      <c r="AS26">
+      <c r="AS26" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT26">
         <v>0.623</v>
       </c>
-      <c r="AT26">
+      <c r="AU26">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW26" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX26" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY26" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ26" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA26" s="17" t="s">
+      <c r="AZ26" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA26" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB26" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB26" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC26" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC26" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD26" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>179</v>
       </c>
@@ -4267,7 +4275,7 @@
       <c r="D27" t="s">
         <v>161</v>
       </c>
-      <c r="F27" t="b">
+      <c r="F27" s="42" t="b">
         <v>1</v>
       </c>
       <c r="G27">
@@ -4351,80 +4359,80 @@
       <c r="AH27" t="s">
         <v>86</v>
       </c>
-      <c r="AI27">
-        <v>0</v>
-      </c>
-      <c r="AJ27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK27" t="s">
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL27" t="s">
         <v>128</v>
       </c>
-      <c r="AL27" t="s">
+      <c r="AM27" t="s">
         <v>175</v>
       </c>
-      <c r="AM27">
+      <c r="AN27">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN27">
+      <c r="AO27">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO27" s="3">
+      <c r="AP27" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP27" s="9">
+      <c r="AQ27" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ27" t="s">
-        <v>32</v>
       </c>
       <c r="AR27" t="s">
         <v>32</v>
       </c>
-      <c r="AS27">
+      <c r="AS27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT27">
         <v>0.623</v>
       </c>
-      <c r="AT27">
+      <c r="AU27">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW27" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX27" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY27" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ27" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA27" s="17" t="s">
+      <c r="AZ27" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA27" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB27" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB27" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC27" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AO28" s="3"/>
-      <c r="AP28" s="9"/>
-      <c r="AW28" s="17"/>
+      <c r="BC27" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD27" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AP28" s="3"/>
+      <c r="AQ28" s="9"/>
       <c r="AX28" s="17"/>
       <c r="AY28" s="17"/>
       <c r="AZ28" s="17"/>
       <c r="BA28" s="17"/>
       <c r="BB28" s="17"/>
-      <c r="BC28" s="37"/>
-    </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AO29" s="3"/>
+      <c r="BC28" s="17"/>
+      <c r="BD28" s="37"/>
+    </row>
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="AP29" s="3"/>
-    </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AQ29" s="3"/>
+    </row>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -4434,7 +4442,7 @@
       <c r="D30" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="43" t="b">
+      <c r="F30" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G30">
@@ -4518,65 +4526,65 @@
       <c r="AH30" t="s">
         <v>86</v>
       </c>
-      <c r="AI30">
-        <v>0</v>
-      </c>
-      <c r="AJ30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK30" t="s">
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL30" t="s">
         <v>128</v>
       </c>
-      <c r="AL30" t="s">
+      <c r="AM30" t="s">
         <v>21</v>
       </c>
-      <c r="AM30">
+      <c r="AN30">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN30">
+      <c r="AO30">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO30" s="3">
+      <c r="AP30" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP30" s="9">
+      <c r="AQ30" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ30" t="s">
-        <v>32</v>
       </c>
       <c r="AR30" t="s">
         <v>32</v>
       </c>
-      <c r="AS30">
+      <c r="AS30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT30">
         <v>0.623</v>
       </c>
-      <c r="AT30">
+      <c r="AU30">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW30" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX30" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY30" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ30" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA30" s="17" t="s">
+      <c r="AZ30" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA30" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB30" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB30" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC30" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC30" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD30" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -4586,7 +4594,7 @@
       <c r="D31" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="43" t="b">
+      <c r="F31" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G31">
@@ -4670,65 +4678,65 @@
       <c r="AH31" t="s">
         <v>86</v>
       </c>
-      <c r="AI31">
-        <v>0</v>
-      </c>
-      <c r="AJ31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK31" t="s">
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL31" t="s">
         <v>128</v>
       </c>
-      <c r="AL31" t="s">
+      <c r="AM31" t="s">
         <v>21</v>
       </c>
-      <c r="AM31">
+      <c r="AN31">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN31">
+      <c r="AO31">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO31" s="3">
+      <c r="AP31" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP31" s="9">
+      <c r="AQ31" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ31" t="s">
-        <v>32</v>
       </c>
       <c r="AR31" t="s">
         <v>32</v>
       </c>
-      <c r="AS31">
+      <c r="AS31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT31">
         <v>0.623</v>
       </c>
-      <c r="AT31">
+      <c r="AU31">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW31" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX31" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY31" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ31" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA31" s="17" t="s">
+      <c r="AZ31" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA31" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB31" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC31" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC31" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD31" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>105</v>
       </c>
@@ -4738,7 +4746,7 @@
       <c r="D33" t="s">
         <v>21</v>
       </c>
-      <c r="F33" s="43" t="b">
+      <c r="F33" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G33">
@@ -4822,65 +4830,65 @@
       <c r="AH33" t="s">
         <v>86</v>
       </c>
-      <c r="AI33">
-        <v>0</v>
-      </c>
-      <c r="AJ33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK33" t="s">
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL33" t="s">
         <v>128</v>
       </c>
-      <c r="AL33" t="s">
+      <c r="AM33" t="s">
         <v>21</v>
       </c>
-      <c r="AM33">
+      <c r="AN33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN33">
+      <c r="AO33">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO33" s="3">
+      <c r="AP33" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP33" s="9">
+      <c r="AQ33" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ33" t="s">
-        <v>32</v>
       </c>
       <c r="AR33" t="s">
         <v>32</v>
       </c>
-      <c r="AS33">
+      <c r="AS33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT33">
         <v>0.623</v>
       </c>
-      <c r="AT33">
+      <c r="AU33">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW33" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX33" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY33" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ33" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA33" s="17" t="s">
+      <c r="AZ33" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA33" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB33" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB33" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC33" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC33" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD33" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -4890,7 +4898,7 @@
       <c r="D34" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="43" t="b">
+      <c r="F34" s="42" t="b">
         <v>0</v>
       </c>
       <c r="G34">
@@ -4974,65 +4982,65 @@
       <c r="AH34" t="s">
         <v>86</v>
       </c>
-      <c r="AI34">
-        <v>0</v>
-      </c>
-      <c r="AJ34" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK34" t="s">
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL34" t="s">
         <v>128</v>
       </c>
-      <c r="AL34" t="s">
+      <c r="AM34" t="s">
         <v>21</v>
       </c>
-      <c r="AM34">
+      <c r="AN34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN34">
+      <c r="AO34">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO34" s="3">
+      <c r="AP34" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP34" s="9">
+      <c r="AQ34" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ34" t="s">
-        <v>32</v>
       </c>
       <c r="AR34" t="s">
         <v>32</v>
       </c>
-      <c r="AS34">
+      <c r="AS34" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT34">
         <v>0.623</v>
       </c>
-      <c r="AT34">
+      <c r="AU34">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW34" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX34" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY34" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ34" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA34" s="17" t="s">
+      <c r="AZ34" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA34" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB34" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB34" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC34" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC34" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD34" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
         <v>135</v>
       </c>
@@ -5126,65 +5134,65 @@
       <c r="AH38" t="s">
         <v>86</v>
       </c>
-      <c r="AI38">
-        <v>0</v>
-      </c>
-      <c r="AJ38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK38" t="s">
+      <c r="AJ38">
+        <v>0</v>
+      </c>
+      <c r="AK38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL38" t="s">
         <v>128</v>
       </c>
-      <c r="AL38" t="s">
+      <c r="AM38" t="s">
         <v>21</v>
       </c>
-      <c r="AM38">
+      <c r="AN38">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN38">
+      <c r="AO38">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO38" s="3">
+      <c r="AP38" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP38" s="9">
+      <c r="AQ38" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ38" t="s">
-        <v>32</v>
       </c>
       <c r="AR38" t="s">
         <v>32</v>
       </c>
-      <c r="AS38">
+      <c r="AS38" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT38">
         <v>0.623</v>
       </c>
-      <c r="AT38">
+      <c r="AU38">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW38" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX38" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY38" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ38" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA38" s="17" t="s">
+      <c r="AZ38" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA38" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB38" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB38" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC38" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC38" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD38" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>165</v>
       </c>
@@ -5278,65 +5286,65 @@
       <c r="AH39" t="s">
         <v>86</v>
       </c>
-      <c r="AI39">
-        <v>0</v>
-      </c>
-      <c r="AJ39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK39" t="s">
+      <c r="AJ39">
+        <v>0</v>
+      </c>
+      <c r="AK39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL39" t="s">
         <v>128</v>
       </c>
-      <c r="AL39" t="s">
+      <c r="AM39" t="s">
         <v>21</v>
       </c>
-      <c r="AM39">
+      <c r="AN39">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN39">
+      <c r="AO39">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO39" s="3">
+      <c r="AP39" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP39" s="9">
+      <c r="AQ39" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ39" t="s">
-        <v>32</v>
       </c>
       <c r="AR39" t="s">
         <v>32</v>
       </c>
-      <c r="AS39">
+      <c r="AS39" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT39">
         <v>0.623</v>
       </c>
-      <c r="AT39">
+      <c r="AU39">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW39" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX39" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY39" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ39" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA39" s="17" t="s">
+      <c r="AZ39" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA39" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB39" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB39" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC39" s="37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BC39" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD39" s="37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>134</v>
       </c>
@@ -5430,70 +5438,70 @@
       <c r="AH40" t="s">
         <v>86</v>
       </c>
-      <c r="AI40">
-        <v>0</v>
-      </c>
-      <c r="AJ40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AK40" t="s">
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+      <c r="AK40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL40" t="s">
         <v>128</v>
       </c>
-      <c r="AL40" t="s">
+      <c r="AM40" t="s">
         <v>21</v>
       </c>
-      <c r="AM40">
+      <c r="AN40">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AN40">
+      <c r="AO40">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AO40" s="3">
+      <c r="AP40" s="3">
         <v>0.12</v>
       </c>
-      <c r="AP40" s="9">
+      <c r="AQ40" s="9">
         <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AQ40" t="s">
-        <v>32</v>
       </c>
       <c r="AR40" t="s">
         <v>32</v>
       </c>
-      <c r="AS40">
+      <c r="AS40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT40">
         <v>0.623</v>
       </c>
-      <c r="AT40">
+      <c r="AU40">
         <v>0.57999999999999996</v>
       </c>
-      <c r="AW40" s="17" t="b">
-        <v>1</v>
-      </c>
       <c r="AX40" s="17" t="b">
         <v>1</v>
       </c>
       <c r="AY40" s="17" t="b">
         <v>1</v>
       </c>
-      <c r="AZ40" s="17">
-        <v>0</v>
-      </c>
-      <c r="BA40" s="17" t="s">
+      <c r="AZ40" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA40" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB40" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="BB40" s="17" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC40" s="37" t="b">
+      <c r="BC40" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD40" s="37" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX33:AY34 L33:L34 F5:F31 F38:F40 AX38:AY40 K38:L40 K26:K34 L26:L31 AX5:AY31 K5:L28 F33:F34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY33:AZ34 L33:L34 F5:F31 F38:F40 AY38:AZ40 K38:L40 K26:K34 L26:L31 AY5:AZ31 K5:L28 F33:F34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK33:AK34 AK38:AK40 AK5:AK31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL33:AL34 AL38:AL40 AL5:AL31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6441,10 +6449,10 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="42"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>

</xml_diff>

<commit_message>
update with AV2016 data
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41110D-0FD9-42A8-A711-C935D994F452}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82882B18-D6A4-45DC-A4EF-6DCC7FB80AB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -1352,7 +1352,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1362,8 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="7" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
     <col min="9" max="9" width="29.140625" customWidth="1"/>
     <col min="10" max="11" width="18.28515625" customWidth="1"/>
@@ -1660,7 +1661,7 @@
         <v>138</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0.3</v>
@@ -1812,7 +1813,7 @@
         <v>138</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0.3</v>
@@ -1969,7 +1970,7 @@
         <v>161</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0.3</v>
@@ -2278,7 +2279,7 @@
         <v>139</v>
       </c>
       <c r="F11" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0.3</v>
@@ -2430,7 +2431,7 @@
         <v>139</v>
       </c>
       <c r="F12" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0.3</v>
@@ -2582,7 +2583,7 @@
         <v>139</v>
       </c>
       <c r="F13" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0.3</v>
@@ -2734,7 +2735,7 @@
         <v>139</v>
       </c>
       <c r="F14" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>0.3</v>
@@ -2886,7 +2887,7 @@
         <v>139</v>
       </c>
       <c r="F15" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>0.3</v>
@@ -3038,7 +3039,7 @@
         <v>139</v>
       </c>
       <c r="F16" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>0.3</v>
@@ -3180,6 +3181,7 @@
       </c>
     </row>
     <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F17" s="40"/>
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3"/>
     </row>
@@ -3193,8 +3195,8 @@
       <c r="D18" t="s">
         <v>138</v>
       </c>
-      <c r="F18" t="b">
-        <v>0</v>
+      <c r="F18" s="40" t="b">
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0.3</v>
@@ -3345,8 +3347,8 @@
       <c r="D19" t="s">
         <v>161</v>
       </c>
-      <c r="F19" t="b">
-        <v>0</v>
+      <c r="F19" s="40" t="b">
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0.3</v>
@@ -3486,6 +3488,9 @@
       <c r="BD19" s="35" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -3498,7 +3503,7 @@
         <v>138</v>
       </c>
       <c r="F21" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0.3</v>
@@ -3650,7 +3655,7 @@
         <v>161</v>
       </c>
       <c r="F22" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0.3</v>
@@ -3792,6 +3797,7 @@
       </c>
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F23" s="40"/>
       <c r="AP23" s="3"/>
       <c r="AQ23" s="3"/>
     </row>
@@ -3805,8 +3811,8 @@
       <c r="D24" t="s">
         <v>138</v>
       </c>
-      <c r="F24" t="b">
-        <v>0</v>
+      <c r="F24" s="40" t="b">
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0.3</v>
@@ -3957,8 +3963,8 @@
       <c r="D25" t="s">
         <v>161</v>
       </c>
-      <c r="F25" t="b">
-        <v>0</v>
+      <c r="F25" s="40" t="b">
+        <v>1</v>
       </c>
       <c r="G25">
         <v>0.3</v>
@@ -4110,7 +4116,7 @@
         <v>138</v>
       </c>
       <c r="F26" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>0.3</v>
@@ -4262,7 +4268,7 @@
         <v>161</v>
       </c>
       <c r="F27" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>0.3</v>
@@ -4404,11 +4410,13 @@
       </c>
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F28" s="40"/>
       <c r="AP28" s="3"/>
       <c r="AQ28" s="9"/>
       <c r="BD28" s="35"/>
     </row>
     <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F29" s="40"/>
       <c r="AP29" s="3"/>
       <c r="AQ29" s="3"/>
     </row>
@@ -4423,7 +4431,7 @@
         <v>21</v>
       </c>
       <c r="F30" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>0.3</v>
@@ -4575,7 +4583,7 @@
         <v>21</v>
       </c>
       <c r="F31" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>0.3</v>
@@ -4715,6 +4723,9 @@
       <c r="BD31" s="35" t="b">
         <v>1</v>
       </c>
+    </row>
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F32" s="40"/>
     </row>
     <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -4727,7 +4738,7 @@
         <v>21</v>
       </c>
       <c r="F33" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>0.3</v>
@@ -4879,7 +4890,7 @@
         <v>21</v>
       </c>
       <c r="F34" s="40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>0.3</v>
@@ -5478,7 +5489,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY33:AZ34 L33:L34 F5:F31 F38:F40 AY38:AZ40 K38:L40 K26:K34 L26:L31 AY5:AZ31 K5:L28 F33:F34" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY33:AZ34 L33:L34 K5:L28 F38:F40 AY38:AZ40 K38:L40 K26:K34 L26:L31 AY5:AZ31 F5:F34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL33:AL34 AL38:AL40 AL5:AL31" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>

<commit_message>
final version of single tier model
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A1DE19-0AFF-40A5-B8F0-673ED460A1CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6BFA98-EF50-4033-B508-BA1482AA768F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1471,7 +1471,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,7 +2261,7 @@
         <v>161</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0.3</v>
@@ -3535,7 +3535,7 @@
         <v>138</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0.3</v>

</xml_diff>

<commit_message>
multiTier demographics, with inconsistency issues
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF9F61D-596F-4F98-866E-D28F1908DBEF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07974A8-8FF8-45AA-BC6A-94DD54E87149}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="193">
   <si>
     <t>runname</t>
   </si>
@@ -770,10 +770,13 @@
     <t>singleTier_select</t>
   </si>
   <si>
-    <t>singleTier</t>
-  </si>
-  <si>
     <t>t4a</t>
+  </si>
+  <si>
+    <t>multiTier</t>
+  </si>
+  <si>
+    <t>simple</t>
   </si>
 </sst>
 </file>
@@ -1504,13 +1507,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:BG44"/>
+  <dimension ref="A3:BG46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="AI5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="AP8" sqref="AP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,13 +1831,13 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0.3</v>
@@ -1848,20 +1851,26 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
+      <c r="J5" t="s">
+        <v>191</v>
+      </c>
+      <c r="K5" t="s">
+        <v>190</v>
+      </c>
       <c r="L5" t="b">
         <v>0</v>
       </c>
       <c r="M5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" t="s">
         <v>130</v>
       </c>
       <c r="P5" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="Q5">
         <v>6</v>
@@ -1933,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="AO5" t="s">
-        <v>128</v>
+        <v>192</v>
       </c>
       <c r="AP5" t="s">
         <v>21</v>
@@ -1985,174 +1994,174 @@
       </c>
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="9"/>
+      <c r="BG6" s="35"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="s">
         <v>138</v>
       </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>0.3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>110</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>107</v>
       </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
         <v>130</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P7" t="s">
         <v>136</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <v>6</v>
       </c>
-      <c r="R6">
+      <c r="R7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S7" t="s">
         <v>96</v>
       </c>
-      <c r="T6">
+      <c r="T7">
         <v>0.46500000000000002</v>
       </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>0.15</v>
       </c>
-      <c r="W6">
+      <c r="W7">
         <v>3</v>
       </c>
-      <c r="X6">
+      <c r="X7">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y6">
+      <c r="Y7">
         <v>62</v>
       </c>
-      <c r="Z6">
+      <c r="Z7">
         <v>5</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA7" t="s">
         <v>184</v>
       </c>
-      <c r="AB6">
+      <c r="AB7">
         <v>0.03</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AD7" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE7" t="s">
         <v>43</v>
       </c>
-      <c r="AF6">
+      <c r="AF7">
         <v>15</v>
       </c>
-      <c r="AG6">
+      <c r="AG7">
         <v>0.03</v>
       </c>
-      <c r="AH6">
+      <c r="AH7">
         <v>6</v>
       </c>
-      <c r="AI6">
+      <c r="AI7">
         <v>1.2</v>
       </c>
-      <c r="AJ6">
+      <c r="AJ7">
         <v>0.8</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AK7" t="s">
         <v>86</v>
       </c>
-      <c r="AL6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO6" t="s">
+      <c r="AL7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="s">
         <v>128</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AP7" t="s">
         <v>21</v>
       </c>
-      <c r="AQ6">
+      <c r="AQ7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR6">
+      <c r="AR7">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS6" s="3">
+      <c r="AS7" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT6" s="9">
+      <c r="AT7" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AU7" t="s">
         <v>32</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AV7" t="s">
         <v>32</v>
       </c>
-      <c r="AW6">
+      <c r="AW7">
         <v>0.623</v>
       </c>
-      <c r="AX6">
+      <c r="AX7">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD6">
-        <v>0</v>
-      </c>
-      <c r="BE6" t="s">
+      <c r="BA7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD7">
+        <v>0</v>
+      </c>
+      <c r="BE7" t="s">
         <v>4</v>
       </c>
-      <c r="BF6" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG6" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="9"/>
-      <c r="BG7" s="35"/>
+      <c r="BF7" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG7" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -2173,16 +2182,16 @@
         <v>0</v>
       </c>
       <c r="M8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" t="s">
         <v>130</v>
       </c>
       <c r="P8" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="Q8">
         <v>6</v>
@@ -2306,180 +2315,174 @@
       </c>
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>164</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="AS9" s="3"/>
+      <c r="AT9" s="9"/>
+      <c r="BG9" s="35"/>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" t="s">
         <v>161</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9">
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>0.3</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>110</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>107</v>
       </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>190</v>
-      </c>
-      <c r="K9" t="s">
-        <v>191</v>
-      </c>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
         <v>130</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P10" t="s">
         <v>162</v>
       </c>
-      <c r="Q9">
+      <c r="Q10">
         <v>6</v>
       </c>
-      <c r="R9">
+      <c r="R10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S10" t="s">
         <v>96</v>
       </c>
-      <c r="T9">
+      <c r="T10">
         <v>0.46500000000000002</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
         <v>0.15</v>
       </c>
-      <c r="W9">
+      <c r="W10">
         <v>3</v>
       </c>
-      <c r="X9">
+      <c r="X10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y9">
+      <c r="Y10">
         <v>62</v>
       </c>
-      <c r="Z9">
+      <c r="Z10">
         <v>5</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA10" t="s">
         <v>184</v>
       </c>
-      <c r="AB9">
+      <c r="AB10">
         <v>0.03</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AD10" t="s">
         <v>50</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AE10" t="s">
         <v>43</v>
       </c>
-      <c r="AF9">
+      <c r="AF10">
         <v>15</v>
       </c>
-      <c r="AG9">
+      <c r="AG10">
         <v>0.03</v>
       </c>
-      <c r="AH9">
+      <c r="AH10">
         <v>6</v>
       </c>
-      <c r="AI9">
+      <c r="AI10">
         <v>1.2</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ10">
         <v>0.8</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AK10" t="s">
         <v>86</v>
       </c>
-      <c r="AL9" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM9">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO9" t="s">
+      <c r="AL10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO10" t="s">
         <v>128</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AP10" t="s">
         <v>21</v>
       </c>
-      <c r="AQ9">
+      <c r="AQ10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR9">
+      <c r="AR10">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS9" s="3">
+      <c r="AS10" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT9" s="9">
+      <c r="AT10" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU9" t="s">
+      <c r="AU10" t="s">
         <v>32</v>
       </c>
-      <c r="AV9" t="s">
+      <c r="AV10" t="s">
         <v>32</v>
       </c>
-      <c r="AW9">
+      <c r="AW10">
         <v>0.623</v>
       </c>
-      <c r="AX9">
+      <c r="AX10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA9" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB9" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC9" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD9">
-        <v>0</v>
-      </c>
-      <c r="BE9" t="s">
+      <c r="BA10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD10">
+        <v>0</v>
+      </c>
+      <c r="BE10" t="s">
         <v>4</v>
       </c>
-      <c r="BF9" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG9" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="9"/>
-      <c r="BG10" s="35"/>
+      <c r="BF10" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG10" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -2496,6 +2499,12 @@
       <c r="I11" t="b">
         <v>0</v>
       </c>
+      <c r="J11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K11" t="s">
+        <v>190</v>
+      </c>
       <c r="L11" t="b">
         <v>0</v>
       </c>
@@ -2503,13 +2512,13 @@
         <v>1</v>
       </c>
       <c r="N11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" t="s">
         <v>130</v>
       </c>
       <c r="P11" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="Q11">
         <v>6</v>
@@ -2554,7 +2563,7 @@
         <v>43</v>
       </c>
       <c r="AF11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AG11">
         <v>0.03</v>
@@ -2584,7 +2593,7 @@
         <v>128</v>
       </c>
       <c r="AP11" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="AQ11">
         <v>7.0000000000000007E-2</v>
@@ -2633,174 +2642,174 @@
       </c>
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="AS12" s="3"/>
+      <c r="AT12" s="9"/>
+      <c r="BG12" s="35"/>
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>0.3</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>110</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>107</v>
       </c>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" t="b">
-        <v>1</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
         <v>130</v>
       </c>
-      <c r="P12" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q12">
+      <c r="P13" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q13">
         <v>6</v>
       </c>
-      <c r="R12">
+      <c r="R13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S13" t="s">
         <v>96</v>
       </c>
-      <c r="T12">
+      <c r="T13">
         <v>0.46500000000000002</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
         <v>0.15</v>
       </c>
-      <c r="W12">
+      <c r="W13">
         <v>3</v>
       </c>
-      <c r="X12">
+      <c r="X13">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y12">
+      <c r="Y13">
         <v>62</v>
       </c>
-      <c r="Z12">
+      <c r="Z13">
         <v>5</v>
       </c>
-      <c r="AA12" t="s">
+      <c r="AA13" t="s">
         <v>184</v>
       </c>
-      <c r="AB12">
+      <c r="AB13">
         <v>0.03</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AD13" t="s">
         <v>50</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AE13" t="s">
         <v>43</v>
       </c>
-      <c r="AF12">
+      <c r="AF13">
         <v>14</v>
       </c>
-      <c r="AG12">
+      <c r="AG13">
         <v>0.03</v>
       </c>
-      <c r="AH12">
+      <c r="AH13">
         <v>6</v>
       </c>
-      <c r="AI12">
+      <c r="AI13">
         <v>1.2</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ13">
         <v>0.8</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AK13" t="s">
         <v>86</v>
       </c>
-      <c r="AL12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM12">
-        <v>0</v>
-      </c>
-      <c r="AN12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO12" t="s">
+      <c r="AL13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO13" t="s">
         <v>128</v>
       </c>
-      <c r="AP12" t="s">
+      <c r="AP13" t="s">
         <v>151</v>
       </c>
-      <c r="AQ12">
+      <c r="AQ13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR12">
+      <c r="AR13">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS12" s="3">
+      <c r="AS13" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT12" s="9">
+      <c r="AT13" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU12" t="s">
+      <c r="AU13" t="s">
         <v>32</v>
       </c>
-      <c r="AV12" t="s">
+      <c r="AV13" t="s">
         <v>32</v>
       </c>
-      <c r="AW12">
+      <c r="AW13">
         <v>0.623</v>
       </c>
-      <c r="AX12">
+      <c r="AX13">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD12">
-        <v>0</v>
-      </c>
-      <c r="BE12" t="s">
+      <c r="BA13" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB13" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC13" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD13">
+        <v>0</v>
+      </c>
+      <c r="BE13" t="s">
         <v>4</v>
       </c>
-      <c r="BF12" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG12" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS13" s="3"/>
-      <c r="AT13" s="9"/>
-      <c r="BG13" s="35"/>
+      <c r="BF13" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG13" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -2875,7 +2884,7 @@
         <v>43</v>
       </c>
       <c r="AF14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AG14">
         <v>0.03</v>
@@ -2890,7 +2899,7 @@
         <v>0.8</v>
       </c>
       <c r="AK14" t="s">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="AL14" t="b">
         <v>1</v>
@@ -2905,7 +2914,7 @@
         <v>128</v>
       </c>
       <c r="AP14" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="AQ14">
         <v>7.0000000000000007E-2</v>
@@ -2923,7 +2932,7 @@
         <v>32</v>
       </c>
       <c r="AV14" t="s">
-        <v>185</v>
+        <v>32</v>
       </c>
       <c r="AW14">
         <v>0.623</v>
@@ -2953,167 +2962,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0.3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>110</v>
-      </c>
-      <c r="H15" t="s">
-        <v>107</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" t="b">
-        <v>1</v>
-      </c>
-      <c r="N15" t="b">
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
-        <v>130</v>
-      </c>
-      <c r="P15" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q15">
-        <v>6</v>
-      </c>
-      <c r="R15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S15" t="s">
-        <v>96</v>
-      </c>
-      <c r="T15">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="U15">
-        <v>0</v>
-      </c>
-      <c r="V15">
-        <v>0.15</v>
-      </c>
-      <c r="W15">
-        <v>3</v>
-      </c>
-      <c r="X15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="Y15">
-        <v>62</v>
-      </c>
-      <c r="Z15">
-        <v>5</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB15">
-        <v>0.03</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF15">
-        <v>15</v>
-      </c>
-      <c r="AG15">
-        <v>0.03</v>
-      </c>
-      <c r="AH15">
-        <v>6</v>
-      </c>
-      <c r="AI15">
-        <v>1.2</v>
-      </c>
-      <c r="AJ15">
-        <v>0.8</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM15">
-        <v>0</v>
-      </c>
-      <c r="AN15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AR15">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AS15" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AT15" s="9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW15">
-        <v>0.623</v>
-      </c>
-      <c r="AX15">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="BA15" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB15" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC15" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD15">
-        <v>0</v>
-      </c>
-      <c r="BE15" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF15" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG15" s="35" t="b">
-        <v>1</v>
-      </c>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AS15" s="3"/>
+      <c r="AT15" s="9"/>
+      <c r="BG15" s="35"/>
     </row>
     <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
         <v>139</v>
@@ -3188,7 +3044,7 @@
         <v>50</v>
       </c>
       <c r="AE16" t="s">
-        <v>144</v>
+        <v>43</v>
       </c>
       <c r="AF16">
         <v>15</v>
@@ -3206,7 +3062,7 @@
         <v>0.8</v>
       </c>
       <c r="AK16" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="AL16" t="b">
         <v>1</v>
@@ -3239,7 +3095,7 @@
         <v>32</v>
       </c>
       <c r="AV16" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="AW16">
         <v>0.623</v>
@@ -3269,9 +3125,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="C17" t="s">
         <v>139</v>
@@ -3343,10 +3199,10 @@
         <v>0.03</v>
       </c>
       <c r="AD17" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="AE17" t="s">
-        <v>144</v>
+        <v>43</v>
       </c>
       <c r="AF17">
         <v>15</v>
@@ -3367,7 +3223,7 @@
         <v>86</v>
       </c>
       <c r="AL17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM17">
         <v>0</v>
@@ -3429,7 +3285,7 @@
     </row>
     <row r="18" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
         <v>139</v>
@@ -3501,13 +3357,13 @@
         <v>0.03</v>
       </c>
       <c r="AD18" t="s">
-        <v>143</v>
+        <v>50</v>
       </c>
       <c r="AE18" t="s">
         <v>144</v>
       </c>
       <c r="AF18">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AG18">
         <v>0.03</v>
@@ -3587,10 +3443,10 @@
     </row>
     <row r="19" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -3614,13 +3470,13 @@
         <v>1</v>
       </c>
       <c r="N19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" t="s">
         <v>130</v>
       </c>
       <c r="P19" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="Q19">
         <v>6</v>
@@ -3665,7 +3521,7 @@
         <v>144</v>
       </c>
       <c r="AF19">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AG19">
         <v>0.03</v>
@@ -3744,12 +3600,166 @@
       </c>
     </row>
     <row r="20" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS20" s="3"/>
-      <c r="AT20" s="3"/>
+      <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20" t="s">
+        <v>130</v>
+      </c>
+      <c r="P20" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S20" t="s">
+        <v>96</v>
+      </c>
+      <c r="T20">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0.15</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="X20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y20">
+        <v>62</v>
+      </c>
+      <c r="Z20">
+        <v>5</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB20">
+        <v>0.03</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF20">
+        <v>30</v>
+      </c>
+      <c r="AG20">
+        <v>0.03</v>
+      </c>
+      <c r="AH20">
+        <v>6</v>
+      </c>
+      <c r="AI20">
+        <v>1.2</v>
+      </c>
+      <c r="AJ20">
+        <v>0.8</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL20" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO20" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ20">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AR20">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AS20" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AT20" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AU20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW20">
+        <v>0.623</v>
+      </c>
+      <c r="AX20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="BA20" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB20" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC20" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD20">
+        <v>0</v>
+      </c>
+      <c r="BE20" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF20" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG20" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C21" t="s">
         <v>138</v>
@@ -3782,7 +3792,7 @@
         <v>130</v>
       </c>
       <c r="P21" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="Q21">
         <v>6</v>
@@ -3821,13 +3831,13 @@
         <v>0.03</v>
       </c>
       <c r="AD21" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="AE21" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="AF21">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="AG21">
         <v>0.03</v>
@@ -3857,7 +3867,7 @@
         <v>128</v>
       </c>
       <c r="AP21" t="s">
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="AQ21">
         <v>7.0000000000000007E-2</v>
@@ -3906,174 +3916,173 @@
       </c>
     </row>
     <row r="22" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>177</v>
-      </c>
-      <c r="C22" t="s">
-        <v>161</v>
-      </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="AS22" s="3"/>
+      <c r="AT22" s="3"/>
+    </row>
+    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>0.3</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>110</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>107</v>
       </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22" t="b">
-        <v>1</v>
-      </c>
-      <c r="N22" t="b">
-        <v>1</v>
-      </c>
-      <c r="O22" t="s">
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+      <c r="N23" t="b">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
         <v>130</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P23" t="s">
         <v>162</v>
       </c>
-      <c r="Q22">
+      <c r="Q23">
         <v>6</v>
       </c>
-      <c r="R22">
+      <c r="R23">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S23" t="s">
         <v>96</v>
       </c>
-      <c r="T22">
+      <c r="T23">
         <v>0.46500000000000002</v>
       </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
         <v>0.15</v>
       </c>
-      <c r="W22">
+      <c r="W23">
         <v>3</v>
       </c>
-      <c r="X22">
+      <c r="X23">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y22">
+      <c r="Y23">
         <v>62</v>
       </c>
-      <c r="Z22">
+      <c r="Z23">
         <v>5</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AA23" t="s">
         <v>184</v>
       </c>
-      <c r="AB22">
+      <c r="AB23">
         <v>0.03</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AD23" t="s">
         <v>50</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AE23" t="s">
         <v>43</v>
       </c>
-      <c r="AF22">
+      <c r="AF23">
         <v>14</v>
       </c>
-      <c r="AG22">
+      <c r="AG23">
         <v>0.03</v>
       </c>
-      <c r="AH22">
+      <c r="AH23">
         <v>6</v>
       </c>
-      <c r="AI22">
+      <c r="AI23">
         <v>1.2</v>
       </c>
-      <c r="AJ22">
+      <c r="AJ23">
         <v>0.8</v>
       </c>
-      <c r="AK22" t="s">
+      <c r="AK23" t="s">
         <v>86</v>
       </c>
-      <c r="AL22" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM22">
-        <v>0</v>
-      </c>
-      <c r="AN22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO22" t="s">
+      <c r="AL23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO23" t="s">
         <v>128</v>
       </c>
-      <c r="AP22" t="s">
+      <c r="AP23" t="s">
         <v>174</v>
       </c>
-      <c r="AQ22">
+      <c r="AQ23">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR22">
+      <c r="AR23">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS22" s="3">
+      <c r="AS23" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT22" s="9">
+      <c r="AT23" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU22" t="s">
+      <c r="AU23" t="s">
         <v>32</v>
       </c>
-      <c r="AV22" t="s">
+      <c r="AV23" t="s">
         <v>32</v>
       </c>
-      <c r="AW22">
+      <c r="AW23">
         <v>0.623</v>
       </c>
-      <c r="AX22">
+      <c r="AX23">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA22" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB22" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC22" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD22">
-        <v>0</v>
-      </c>
-      <c r="BE22" t="s">
+      <c r="BA23" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB23" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC23" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD23">
+        <v>0</v>
+      </c>
+      <c r="BE23" t="s">
         <v>4</v>
       </c>
-      <c r="BF22" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG22" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS23" s="3"/>
-      <c r="AT23" s="9"/>
-      <c r="BG23" s="35"/>
+      <c r="BF23" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG23" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -4148,7 +4157,7 @@
         <v>43</v>
       </c>
       <c r="AF24">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="AG24">
         <v>0.03</v>
@@ -4178,7 +4187,7 @@
         <v>128</v>
       </c>
       <c r="AP24" t="s">
-        <v>21</v>
+        <v>174</v>
       </c>
       <c r="AQ24">
         <v>7.0000000000000007E-2</v>
@@ -4227,174 +4236,174 @@
       </c>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="AS25" s="3"/>
+      <c r="AT25" s="9"/>
+      <c r="BG25" s="35"/>
+    </row>
+    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" t="s">
         <v>139</v>
       </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25">
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>0.3</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
         <v>110</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H26" t="s">
         <v>107</v>
       </c>
-      <c r="I25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M25" t="b">
-        <v>1</v>
-      </c>
-      <c r="N25" t="b">
-        <v>1</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N26" t="b">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
         <v>130</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P26" t="s">
         <v>162</v>
       </c>
-      <c r="Q25">
+      <c r="Q26">
         <v>6</v>
       </c>
-      <c r="R25">
+      <c r="R26">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S26" t="s">
         <v>96</v>
       </c>
-      <c r="T25">
+      <c r="T26">
         <v>0.46500000000000002</v>
       </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
-      <c r="V25">
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
         <v>0.15</v>
       </c>
-      <c r="W25">
+      <c r="W26">
         <v>3</v>
       </c>
-      <c r="X25">
+      <c r="X26">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y25">
+      <c r="Y26">
         <v>62</v>
       </c>
-      <c r="Z25">
+      <c r="Z26">
         <v>5</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AA26" t="s">
         <v>184</v>
       </c>
-      <c r="AB25">
+      <c r="AB26">
         <v>0.03</v>
       </c>
-      <c r="AD25" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE25" t="s">
+      <c r="AD26" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE26" t="s">
         <v>43</v>
       </c>
-      <c r="AF25">
-        <v>15</v>
-      </c>
-      <c r="AG25">
+      <c r="AF26">
+        <v>30</v>
+      </c>
+      <c r="AG26">
         <v>0.03</v>
       </c>
-      <c r="AH25">
+      <c r="AH26">
         <v>6</v>
       </c>
-      <c r="AI25">
+      <c r="AI26">
         <v>1.2</v>
       </c>
-      <c r="AJ25">
+      <c r="AJ26">
         <v>0.8</v>
       </c>
-      <c r="AK25" t="s">
+      <c r="AK26" t="s">
         <v>86</v>
       </c>
-      <c r="AL25" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM25">
-        <v>0</v>
-      </c>
-      <c r="AN25" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO25" t="s">
+      <c r="AL26" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM26">
+        <v>0</v>
+      </c>
+      <c r="AN26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO26" t="s">
         <v>128</v>
       </c>
-      <c r="AP25" t="s">
+      <c r="AP26" t="s">
         <v>21</v>
       </c>
-      <c r="AQ25">
+      <c r="AQ26">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR25">
+      <c r="AR26">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS25" s="3">
+      <c r="AS26" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT25" s="9">
+      <c r="AT26" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU25" t="s">
+      <c r="AU26" t="s">
         <v>32</v>
       </c>
-      <c r="AV25" t="s">
+      <c r="AV26" t="s">
         <v>32</v>
       </c>
-      <c r="AW25">
+      <c r="AW26">
         <v>0.623</v>
       </c>
-      <c r="AX25">
+      <c r="AX26">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA25" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB25" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC25" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD25">
-        <v>0</v>
-      </c>
-      <c r="BE25" t="s">
+      <c r="BA26" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB26" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC26" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+      <c r="BE26" t="s">
         <v>4</v>
       </c>
-      <c r="BF25" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG25" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS26" s="3"/>
-      <c r="AT26" s="9"/>
-      <c r="BG26" s="35"/>
+      <c r="BF26" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG26" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -4418,13 +4427,13 @@
         <v>1</v>
       </c>
       <c r="N27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27" t="s">
         <v>130</v>
       </c>
       <c r="P27" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="Q27">
         <v>6</v>
@@ -4463,13 +4472,13 @@
         <v>0.03</v>
       </c>
       <c r="AD27" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="AE27" t="s">
         <v>43</v>
       </c>
       <c r="AF27">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AG27">
         <v>0.03</v>
@@ -4499,7 +4508,7 @@
         <v>128</v>
       </c>
       <c r="AP27" t="s">
-        <v>154</v>
+        <v>21</v>
       </c>
       <c r="AQ27">
         <v>7.0000000000000007E-2</v>
@@ -4548,784 +4557,795 @@
       </c>
     </row>
     <row r="28" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="AS28" s="3"/>
+      <c r="AT28" s="9"/>
+      <c r="BG28" s="35"/>
+    </row>
+    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" t="s">
+        <v>107</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+      <c r="N29" t="b">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>130</v>
+      </c>
+      <c r="P29" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q29">
+        <v>6</v>
+      </c>
+      <c r="R29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S29" t="s">
+        <v>96</v>
+      </c>
+      <c r="T29">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0.15</v>
+      </c>
+      <c r="W29">
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y29">
+        <v>62</v>
+      </c>
+      <c r="Z29">
+        <v>5</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB29">
+        <v>0.03</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF29">
+        <v>14</v>
+      </c>
+      <c r="AG29">
+        <v>0.03</v>
+      </c>
+      <c r="AH29">
+        <v>6</v>
+      </c>
+      <c r="AI29">
+        <v>1.2</v>
+      </c>
+      <c r="AJ29">
+        <v>0.8</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL29" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM29">
+        <v>0</v>
+      </c>
+      <c r="AN29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO29" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP29" t="s">
+        <v>154</v>
+      </c>
+      <c r="AQ29">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AR29">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AS29" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AT29" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW29">
+        <v>0.623</v>
+      </c>
+      <c r="AX29">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="BA29" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB29" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC29" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD29">
+        <v>0</v>
+      </c>
+      <c r="BE29" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF29" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG29" s="35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>169</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
         <v>161</v>
       </c>
-      <c r="E28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28">
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>0.3</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>110</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H30" t="s">
         <v>107</v>
       </c>
-      <c r="I28" t="b">
-        <v>0</v>
-      </c>
-      <c r="L28" t="b">
-        <v>0</v>
-      </c>
-      <c r="M28" t="b">
-        <v>1</v>
-      </c>
-      <c r="N28" t="b">
-        <v>1</v>
-      </c>
-      <c r="O28" t="s">
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
+      <c r="N30" t="b">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
         <v>130</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P30" t="s">
         <v>162</v>
       </c>
-      <c r="Q28">
+      <c r="Q30">
         <v>6</v>
       </c>
-      <c r="R28">
+      <c r="R30">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S28" t="s">
+      <c r="S30" t="s">
         <v>96</v>
       </c>
-      <c r="T28">
+      <c r="T30">
         <v>0.46500000000000002</v>
       </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
-      <c r="V28">
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
         <v>0.15</v>
       </c>
-      <c r="W28">
+      <c r="W30">
         <v>3</v>
       </c>
-      <c r="X28">
+      <c r="X30">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y28">
+      <c r="Y30">
         <v>62</v>
       </c>
-      <c r="Z28">
+      <c r="Z30">
         <v>5</v>
       </c>
-      <c r="AA28" t="s">
+      <c r="AA30" t="s">
         <v>184</v>
       </c>
-      <c r="AB28">
+      <c r="AB30">
         <v>0.03</v>
       </c>
-      <c r="AD28" t="s">
+      <c r="AD30" t="s">
         <v>50</v>
       </c>
-      <c r="AE28" t="s">
+      <c r="AE30" t="s">
         <v>43</v>
       </c>
-      <c r="AF28">
+      <c r="AF30">
         <v>14</v>
       </c>
-      <c r="AG28">
+      <c r="AG30">
         <v>0.03</v>
       </c>
-      <c r="AH28">
+      <c r="AH30">
         <v>6</v>
       </c>
-      <c r="AI28">
+      <c r="AI30">
         <v>1.2</v>
       </c>
-      <c r="AJ28">
+      <c r="AJ30">
         <v>0.8</v>
       </c>
-      <c r="AK28" t="s">
+      <c r="AK30" t="s">
         <v>86</v>
       </c>
-      <c r="AL28" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM28">
-        <v>0</v>
-      </c>
-      <c r="AN28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO28" t="s">
+      <c r="AL30" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM30">
+        <v>0</v>
+      </c>
+      <c r="AN30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO30" t="s">
         <v>128</v>
       </c>
-      <c r="AP28" t="s">
+      <c r="AP30" t="s">
         <v>154</v>
       </c>
-      <c r="AQ28">
+      <c r="AQ30">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR28">
+      <c r="AR30">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS28" s="3">
+      <c r="AS30" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT28" s="9">
+      <c r="AT30" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU28" t="s">
+      <c r="AU30" t="s">
         <v>32</v>
       </c>
-      <c r="AV28" t="s">
+      <c r="AV30" t="s">
         <v>32</v>
       </c>
-      <c r="AW28">
+      <c r="AW30">
         <v>0.623</v>
       </c>
-      <c r="AX28">
+      <c r="AX30">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA28" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB28" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC28" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD28">
-        <v>0</v>
-      </c>
-      <c r="BE28" t="s">
+      <c r="BA30" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB30" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC30" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD30">
+        <v>0</v>
+      </c>
+      <c r="BE30" t="s">
         <v>4</v>
       </c>
-      <c r="BF28" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG28" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS29" s="3"/>
-      <c r="AT29" s="9"/>
-      <c r="BG29" s="35"/>
-    </row>
-    <row r="30" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS30" s="3"/>
-      <c r="AT30" s="9"/>
-      <c r="BG30" s="35"/>
+      <c r="BF30" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG30" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="s">
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="9"/>
+      <c r="BG31" s="35"/>
+    </row>
+    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="9"/>
+      <c r="BG32" s="35"/>
+    </row>
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>138</v>
       </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F31">
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33">
         <v>0.3</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G33" t="s">
         <v>110</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H33" t="s">
         <v>107</v>
       </c>
-      <c r="I31" t="b">
-        <v>0</v>
-      </c>
-      <c r="L31" t="b">
-        <v>1</v>
-      </c>
-      <c r="N31" t="b">
-        <v>0</v>
-      </c>
-      <c r="O31" t="s">
+      <c r="I33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+      <c r="N33" t="b">
+        <v>0</v>
+      </c>
+      <c r="O33" t="s">
         <v>130</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P33" t="s">
         <v>162</v>
       </c>
-      <c r="Q31">
+      <c r="Q33">
         <v>6</v>
       </c>
-      <c r="R31">
+      <c r="R33">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="S31" t="s">
+      <c r="S33" t="s">
         <v>96</v>
       </c>
-      <c r="T31">
+      <c r="T33">
         <v>0.45</v>
       </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-      <c r="W31">
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="W33">
         <v>3</v>
       </c>
-      <c r="X31">
+      <c r="X33">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y31">
+      <c r="Y33">
         <v>62</v>
       </c>
-      <c r="Z31">
+      <c r="Z33">
         <v>5</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AA33" t="s">
         <v>79</v>
       </c>
-      <c r="AB31">
+      <c r="AB33">
         <v>0.03</v>
       </c>
-      <c r="AD31" t="s">
+      <c r="AD33" t="s">
         <v>50</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AE33" t="s">
         <v>43</v>
       </c>
-      <c r="AF31">
+      <c r="AF33">
         <v>14</v>
       </c>
-      <c r="AG31">
+      <c r="AG33">
         <v>0.03</v>
       </c>
-      <c r="AH31">
+      <c r="AH33">
         <v>6</v>
       </c>
-      <c r="AI31">
+      <c r="AI33">
         <v>1.2</v>
       </c>
-      <c r="AJ31">
+      <c r="AJ33">
         <v>0.8</v>
       </c>
-      <c r="AK31" t="s">
+      <c r="AK33" t="s">
         <v>86</v>
       </c>
-      <c r="AM31">
-        <v>0</v>
-      </c>
-      <c r="AN31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO31" t="s">
+      <c r="AM33">
+        <v>0</v>
+      </c>
+      <c r="AN33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO33" t="s">
         <v>128</v>
       </c>
-      <c r="AP31" t="s">
+      <c r="AP33" t="s">
         <v>175</v>
       </c>
-      <c r="AQ31">
+      <c r="AQ33">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR31">
+      <c r="AR33">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS31" s="3">
+      <c r="AS33" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT31" s="9">
+      <c r="AT33" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU31" t="s">
+      <c r="AU33" t="s">
         <v>32</v>
       </c>
-      <c r="AV31" t="s">
+      <c r="AV33" t="s">
         <v>32</v>
       </c>
-      <c r="AW31">
+      <c r="AW33">
         <v>0.623</v>
       </c>
-      <c r="AX31">
+      <c r="AX33">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA31" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB31" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC31" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD31">
-        <v>0</v>
-      </c>
-      <c r="BE31" t="s">
+      <c r="BA33" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB33" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC33" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD33">
+        <v>0</v>
+      </c>
+      <c r="BE33" t="s">
         <v>4</v>
       </c>
-      <c r="BF31" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG31" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
+      <c r="BF33" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG33" s="35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A34" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>161</v>
       </c>
-      <c r="E32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32">
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34">
         <v>0.3</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G34" t="s">
         <v>110</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H34" t="s">
         <v>107</v>
       </c>
-      <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="L32" t="b">
-        <v>1</v>
-      </c>
-      <c r="N32" t="b">
-        <v>1</v>
-      </c>
-      <c r="O32" t="s">
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
+      <c r="N34" t="b">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
         <v>130</v>
       </c>
-      <c r="P32" t="s">
+      <c r="P34" t="s">
         <v>162</v>
       </c>
-      <c r="Q32">
+      <c r="Q34">
         <v>6</v>
       </c>
-      <c r="R32">
+      <c r="R34">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="S32" t="s">
+      <c r="S34" t="s">
         <v>96</v>
       </c>
-      <c r="T32">
+      <c r="T34">
         <v>0.45</v>
       </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-      <c r="W32">
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="W34">
         <v>3</v>
       </c>
-      <c r="X32">
+      <c r="X34">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y32">
+      <c r="Y34">
         <v>62</v>
       </c>
-      <c r="Z32">
+      <c r="Z34">
         <v>5</v>
       </c>
-      <c r="AA32" t="s">
+      <c r="AA34" t="s">
         <v>79</v>
       </c>
-      <c r="AB32">
+      <c r="AB34">
         <v>0.03</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AD34" t="s">
         <v>50</v>
       </c>
-      <c r="AE32" t="s">
+      <c r="AE34" t="s">
         <v>43</v>
       </c>
-      <c r="AF32">
+      <c r="AF34">
         <v>14</v>
       </c>
-      <c r="AG32">
+      <c r="AG34">
         <v>0.03</v>
       </c>
-      <c r="AH32">
+      <c r="AH34">
         <v>6</v>
       </c>
-      <c r="AI32">
+      <c r="AI34">
         <v>1.2</v>
       </c>
-      <c r="AJ32">
+      <c r="AJ34">
         <v>0.8</v>
       </c>
-      <c r="AK32" t="s">
+      <c r="AK34" t="s">
         <v>86</v>
       </c>
-      <c r="AM32">
-        <v>0</v>
-      </c>
-      <c r="AN32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO32" t="s">
+      <c r="AM34">
+        <v>0</v>
+      </c>
+      <c r="AN34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO34" t="s">
         <v>128</v>
       </c>
-      <c r="AP32" t="s">
+      <c r="AP34" t="s">
         <v>175</v>
       </c>
-      <c r="AQ32">
+      <c r="AQ34">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR32">
+      <c r="AR34">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS32" s="3">
+      <c r="AS34" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT32" s="9">
+      <c r="AT34" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU32" t="s">
+      <c r="AU34" t="s">
         <v>32</v>
       </c>
-      <c r="AV32" t="s">
+      <c r="AV34" t="s">
         <v>32</v>
       </c>
-      <c r="AW32">
+      <c r="AW34">
         <v>0.623</v>
       </c>
-      <c r="AX32">
+      <c r="AX34">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA32" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB32" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC32" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD32">
-        <v>0</v>
-      </c>
-      <c r="BE32" t="s">
+      <c r="BA34" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB34" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC34" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD34">
+        <v>0</v>
+      </c>
+      <c r="BE34" t="s">
         <v>4</v>
       </c>
-      <c r="BF32" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG32" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS33" s="3"/>
-      <c r="AT33" s="9"/>
-      <c r="BG33" s="35"/>
-    </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AS34" s="3"/>
-      <c r="AT34" s="3"/>
+      <c r="BF34" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG34" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A35" s="40" t="s">
+      <c r="AS35" s="3"/>
+      <c r="AT35" s="9"/>
+      <c r="BG35" s="35"/>
+    </row>
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AS36" s="3"/>
+      <c r="AT36" s="3"/>
+    </row>
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>21</v>
       </c>
-      <c r="E35" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35">
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37">
         <v>0.3</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G37" t="s">
         <v>110</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H37" t="s">
         <v>112</v>
       </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="L35" t="b">
-        <v>1</v>
-      </c>
-      <c r="N35" t="b">
-        <v>1</v>
-      </c>
-      <c r="O35" t="s">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+      <c r="N37" t="b">
+        <v>1</v>
+      </c>
+      <c r="O37" t="s">
         <v>130</v>
       </c>
-      <c r="P35" t="s">
+      <c r="P37" t="s">
         <v>162</v>
       </c>
-      <c r="Q35">
+      <c r="Q37">
         <v>6</v>
       </c>
-      <c r="R35">
+      <c r="R37">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="S35" t="s">
+      <c r="S37" t="s">
         <v>96</v>
       </c>
-      <c r="T35">
+      <c r="T37">
         <v>0.45</v>
       </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-      <c r="W35">
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="W37">
         <v>3</v>
       </c>
-      <c r="X35">
+      <c r="X37">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y35">
+      <c r="Y37">
         <v>62</v>
       </c>
-      <c r="Z35">
+      <c r="Z37">
         <v>5</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AA37" t="s">
         <v>79</v>
       </c>
-      <c r="AB35">
+      <c r="AB37">
         <v>0.03</v>
       </c>
-      <c r="AD35" t="s">
+      <c r="AD37" t="s">
         <v>50</v>
       </c>
-      <c r="AE35" t="s">
+      <c r="AE37" t="s">
         <v>43</v>
       </c>
-      <c r="AF35">
+      <c r="AF37">
         <v>14</v>
       </c>
-      <c r="AG35">
+      <c r="AG37">
         <v>0.03</v>
       </c>
-      <c r="AH35">
+      <c r="AH37">
         <v>6</v>
       </c>
-      <c r="AI35">
+      <c r="AI37">
         <v>1.2</v>
       </c>
-      <c r="AJ35">
+      <c r="AJ37">
         <v>0.8</v>
       </c>
-      <c r="AK35" t="s">
+      <c r="AK37" t="s">
         <v>86</v>
       </c>
-      <c r="AM35">
-        <v>0</v>
-      </c>
-      <c r="AN35" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO35" t="s">
+      <c r="AM37">
+        <v>0</v>
+      </c>
+      <c r="AN37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO37" t="s">
         <v>128</v>
       </c>
-      <c r="AP35" t="s">
+      <c r="AP37" t="s">
         <v>21</v>
       </c>
-      <c r="AQ35">
+      <c r="AQ37">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR35">
+      <c r="AR37">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS35" s="3">
+      <c r="AS37" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT35" s="9">
+      <c r="AT37" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU35" t="s">
+      <c r="AU37" t="s">
         <v>32</v>
       </c>
-      <c r="AV35" t="s">
+      <c r="AV37" t="s">
         <v>32</v>
       </c>
-      <c r="AW35">
+      <c r="AW37">
         <v>0.623</v>
       </c>
-      <c r="AX35">
+      <c r="AX37">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA35" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB35" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC35" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD35">
-        <v>0</v>
-      </c>
-      <c r="BE35" t="s">
+      <c r="BA37" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB37" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC37" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD37">
+        <v>0</v>
+      </c>
+      <c r="BE37" t="s">
         <v>4</v>
       </c>
-      <c r="BF35" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG35" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0.3</v>
-      </c>
-      <c r="G36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" t="s">
-        <v>113</v>
-      </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="L36" t="b">
-        <v>1</v>
-      </c>
-      <c r="N36" t="b">
-        <v>1</v>
-      </c>
-      <c r="O36" t="s">
-        <v>130</v>
-      </c>
-      <c r="P36" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q36">
-        <v>6</v>
-      </c>
-      <c r="R36">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="S36" t="s">
-        <v>96</v>
-      </c>
-      <c r="T36">
-        <v>0.45</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-      <c r="W36">
-        <v>3</v>
-      </c>
-      <c r="X36">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="Y36">
-        <v>62</v>
-      </c>
-      <c r="Z36">
-        <v>5</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB36">
-        <v>0.03</v>
-      </c>
-      <c r="AD36" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE36" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF36">
-        <v>14</v>
-      </c>
-      <c r="AG36">
-        <v>0.03</v>
-      </c>
-      <c r="AH36">
-        <v>6</v>
-      </c>
-      <c r="AI36">
-        <v>1.2</v>
-      </c>
-      <c r="AJ36">
-        <v>0.8</v>
-      </c>
-      <c r="AK36" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM36">
-        <v>0</v>
-      </c>
-      <c r="AN36" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO36" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP36" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ36">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AR36">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AS36" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AT36" s="9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AU36" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV36" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW36">
-        <v>0.623</v>
-      </c>
-      <c r="AX36">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="BA36" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB36" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC36" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD36">
-        <v>0</v>
-      </c>
-      <c r="BE36" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF36" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG36" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
+      <c r="BF37" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG37" s="35" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
@@ -5337,10 +5357,10 @@
         <v>0.3</v>
       </c>
       <c r="G38" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H38" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -5473,458 +5493,312 @@
       </c>
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="41"/>
+    </row>
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A40" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="b">
+        <v>1</v>
+      </c>
+      <c r="N40" t="b">
+        <v>1</v>
+      </c>
+      <c r="O40" t="s">
+        <v>130</v>
+      </c>
+      <c r="P40" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q40">
+        <v>6</v>
+      </c>
+      <c r="R40">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="S40" t="s">
+        <v>96</v>
+      </c>
+      <c r="T40">
+        <v>0.45</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>3</v>
+      </c>
+      <c r="X40">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y40">
+        <v>62</v>
+      </c>
+      <c r="Z40">
+        <v>5</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB40">
+        <v>0.03</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF40">
+        <v>14</v>
+      </c>
+      <c r="AG40">
+        <v>0.03</v>
+      </c>
+      <c r="AH40">
+        <v>6</v>
+      </c>
+      <c r="AI40">
+        <v>1.2</v>
+      </c>
+      <c r="AJ40">
+        <v>0.8</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM40">
+        <v>0</v>
+      </c>
+      <c r="AN40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO40" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ40">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AR40">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AS40" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AT40" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AU40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV40" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW40">
+        <v>0.623</v>
+      </c>
+      <c r="AX40">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="BA40" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB40" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC40" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD40">
+        <v>0</v>
+      </c>
+      <c r="BE40" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF40" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG40" s="35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A41" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C41" t="s">
         <v>21</v>
       </c>
-      <c r="E39" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39">
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41">
         <v>0.3</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G41" t="s">
         <v>115</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H41" t="s">
         <v>107</v>
       </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="L39" t="b">
-        <v>1</v>
-      </c>
-      <c r="N39" t="b">
-        <v>1</v>
-      </c>
-      <c r="O39" t="s">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+      <c r="N41" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" t="s">
         <v>130</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P41" t="s">
         <v>162</v>
       </c>
-      <c r="Q39">
+      <c r="Q41">
         <v>6</v>
       </c>
-      <c r="R39">
+      <c r="R41">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="S39" t="s">
+      <c r="S41" t="s">
         <v>96</v>
       </c>
-      <c r="T39">
+      <c r="T41">
         <v>0.45</v>
       </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
-      <c r="W39">
+      <c r="U41">
+        <v>0</v>
+      </c>
+      <c r="W41">
         <v>3</v>
       </c>
-      <c r="X39">
+      <c r="X41">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Y39">
+      <c r="Y41">
         <v>62</v>
       </c>
-      <c r="Z39">
+      <c r="Z41">
         <v>5</v>
       </c>
-      <c r="AA39" t="s">
+      <c r="AA41" t="s">
         <v>79</v>
       </c>
-      <c r="AB39">
+      <c r="AB41">
         <v>0.03</v>
       </c>
-      <c r="AD39" t="s">
+      <c r="AD41" t="s">
         <v>50</v>
       </c>
-      <c r="AE39" t="s">
+      <c r="AE41" t="s">
         <v>43</v>
       </c>
-      <c r="AF39">
+      <c r="AF41">
         <v>14</v>
       </c>
-      <c r="AG39">
+      <c r="AG41">
         <v>0.03</v>
       </c>
-      <c r="AH39">
+      <c r="AH41">
         <v>6</v>
       </c>
-      <c r="AI39">
+      <c r="AI41">
         <v>1.2</v>
       </c>
-      <c r="AJ39">
+      <c r="AJ41">
         <v>0.8</v>
       </c>
-      <c r="AK39" t="s">
+      <c r="AK41" t="s">
         <v>86</v>
       </c>
-      <c r="AM39">
-        <v>0</v>
-      </c>
-      <c r="AN39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO39" t="s">
+      <c r="AM41">
+        <v>0</v>
+      </c>
+      <c r="AN41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO41" t="s">
         <v>128</v>
       </c>
-      <c r="AP39" t="s">
+      <c r="AP41" t="s">
         <v>21</v>
       </c>
-      <c r="AQ39">
+      <c r="AQ41">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AR39">
+      <c r="AR41">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="AS39" s="3">
+      <c r="AS41" s="3">
         <v>0.12</v>
       </c>
-      <c r="AT39" s="9">
+      <c r="AT41" s="9">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AU39" t="s">
+      <c r="AU41" t="s">
         <v>32</v>
       </c>
-      <c r="AV39" t="s">
+      <c r="AV41" t="s">
         <v>32</v>
       </c>
-      <c r="AW39">
+      <c r="AW41">
         <v>0.623</v>
       </c>
-      <c r="AX39">
+      <c r="AX41">
         <v>0.57999999999999996</v>
       </c>
-      <c r="BA39" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB39" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC39" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD39">
-        <v>0</v>
-      </c>
-      <c r="BE39" t="s">
+      <c r="BA41" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB41" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC41" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD41">
+        <v>0</v>
+      </c>
+      <c r="BE41" t="s">
         <v>4</v>
       </c>
-      <c r="BF39" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG39" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" t="s">
-        <v>139</v>
-      </c>
-      <c r="E42" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0.3</v>
-      </c>
-      <c r="G42" t="s">
-        <v>110</v>
-      </c>
-      <c r="H42" t="s">
-        <v>107</v>
-      </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="L42" t="b">
-        <v>0</v>
-      </c>
-      <c r="N42" t="b">
-        <v>1</v>
-      </c>
-      <c r="O42" t="s">
-        <v>130</v>
-      </c>
-      <c r="P42" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q42">
-        <v>6</v>
-      </c>
-      <c r="R42">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="S42" t="s">
-        <v>96</v>
-      </c>
-      <c r="T42">
-        <v>0.45</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-      <c r="W42">
-        <v>3</v>
-      </c>
-      <c r="X42">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="Y42">
-        <v>62</v>
-      </c>
-      <c r="Z42">
-        <v>5</v>
-      </c>
-      <c r="AA42" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB42">
-        <v>0.03</v>
-      </c>
-      <c r="AD42" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE42" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF42">
-        <v>14</v>
-      </c>
-      <c r="AG42">
-        <v>0.03</v>
-      </c>
-      <c r="AH42">
-        <v>6</v>
-      </c>
-      <c r="AI42">
-        <v>1.2</v>
-      </c>
-      <c r="AJ42">
-        <v>0.8</v>
-      </c>
-      <c r="AK42" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM42">
-        <v>0</v>
-      </c>
-      <c r="AN42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO42" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP42" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ42">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AR42">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AS42" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AT42" s="9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AU42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV42" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW42">
-        <v>0.623</v>
-      </c>
-      <c r="AX42">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="BA42" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB42" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC42" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD42">
-        <v>0</v>
-      </c>
-      <c r="BE42" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF42" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG42" s="35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="C43" t="s">
-        <v>139</v>
-      </c>
-      <c r="E43" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0.3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>110</v>
-      </c>
-      <c r="H43" t="s">
-        <v>107</v>
-      </c>
-      <c r="I43" t="b">
-        <v>0</v>
-      </c>
-      <c r="L43" t="b">
-        <v>1</v>
-      </c>
-      <c r="N43" t="b">
-        <v>1</v>
-      </c>
-      <c r="O43" t="s">
-        <v>130</v>
-      </c>
-      <c r="P43" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q43">
-        <v>6</v>
-      </c>
-      <c r="R43">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="S43" t="s">
-        <v>96</v>
-      </c>
-      <c r="T43">
-        <v>0.45</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-      <c r="W43">
-        <v>3</v>
-      </c>
-      <c r="X43">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="Y43">
-        <v>62</v>
-      </c>
-      <c r="Z43">
-        <v>5</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB43">
-        <v>0.03</v>
-      </c>
-      <c r="AD43" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE43" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF43">
-        <v>14</v>
-      </c>
-      <c r="AG43">
-        <v>0.03</v>
-      </c>
-      <c r="AH43">
-        <v>6</v>
-      </c>
-      <c r="AI43">
-        <v>1.2</v>
-      </c>
-      <c r="AJ43">
-        <v>0.8</v>
-      </c>
-      <c r="AK43" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM43">
-        <v>0</v>
-      </c>
-      <c r="AN43" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO43" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP43" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ43">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="AR43">
-        <v>7.7200000000000005E-2</v>
-      </c>
-      <c r="AS43" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="AT43" s="9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="AU43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW43">
-        <v>0.623</v>
-      </c>
-      <c r="AX43">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="BA43" t="b">
-        <v>1</v>
-      </c>
-      <c r="BB43" t="b">
-        <v>1</v>
-      </c>
-      <c r="BC43" t="b">
-        <v>1</v>
-      </c>
-      <c r="BD43">
-        <v>0</v>
-      </c>
-      <c r="BE43" t="s">
-        <v>4</v>
-      </c>
-      <c r="BF43" t="b">
-        <v>1</v>
-      </c>
-      <c r="BG43" s="35" t="b">
+      <c r="BF41" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG41" s="35" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -5948,7 +5822,7 @@
         <v>1</v>
       </c>
       <c r="O44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="P44" t="s">
         <v>136</v>
@@ -6068,12 +5942,310 @@
         <v>1</v>
       </c>
     </row>
+    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A45" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0.3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>110</v>
+      </c>
+      <c r="H45" t="s">
+        <v>107</v>
+      </c>
+      <c r="I45" t="b">
+        <v>0</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+      <c r="N45" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45" t="s">
+        <v>130</v>
+      </c>
+      <c r="P45" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q45">
+        <v>6</v>
+      </c>
+      <c r="R45">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="S45" t="s">
+        <v>96</v>
+      </c>
+      <c r="T45">
+        <v>0.45</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>3</v>
+      </c>
+      <c r="X45">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y45">
+        <v>62</v>
+      </c>
+      <c r="Z45">
+        <v>5</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB45">
+        <v>0.03</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF45">
+        <v>14</v>
+      </c>
+      <c r="AG45">
+        <v>0.03</v>
+      </c>
+      <c r="AH45">
+        <v>6</v>
+      </c>
+      <c r="AI45">
+        <v>1.2</v>
+      </c>
+      <c r="AJ45">
+        <v>0.8</v>
+      </c>
+      <c r="AK45" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM45">
+        <v>0</v>
+      </c>
+      <c r="AN45" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO45" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP45" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AR45">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AS45" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AT45" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AU45" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV45" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW45">
+        <v>0.623</v>
+      </c>
+      <c r="AX45">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="BA45" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB45" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC45" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD45">
+        <v>0</v>
+      </c>
+      <c r="BE45" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF45" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG45" s="35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A46" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0.3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" t="b">
+        <v>0</v>
+      </c>
+      <c r="N46" t="b">
+        <v>1</v>
+      </c>
+      <c r="O46" t="s">
+        <v>133</v>
+      </c>
+      <c r="P46" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q46">
+        <v>6</v>
+      </c>
+      <c r="R46">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="S46" t="s">
+        <v>96</v>
+      </c>
+      <c r="T46">
+        <v>0.45</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>3</v>
+      </c>
+      <c r="X46">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y46">
+        <v>62</v>
+      </c>
+      <c r="Z46">
+        <v>5</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB46">
+        <v>0.03</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF46">
+        <v>14</v>
+      </c>
+      <c r="AG46">
+        <v>0.03</v>
+      </c>
+      <c r="AH46">
+        <v>6</v>
+      </c>
+      <c r="AI46">
+        <v>1.2</v>
+      </c>
+      <c r="AJ46">
+        <v>0.8</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM46">
+        <v>0</v>
+      </c>
+      <c r="AN46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO46" t="s">
+        <v>128</v>
+      </c>
+      <c r="AP46" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AR46">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="AS46" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AT46" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AU46" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>32</v>
+      </c>
+      <c r="AW46">
+        <v>0.623</v>
+      </c>
+      <c r="AX46">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="BA46" t="b">
+        <v>1</v>
+      </c>
+      <c r="BB46" t="b">
+        <v>1</v>
+      </c>
+      <c r="BC46" t="b">
+        <v>1</v>
+      </c>
+      <c r="BD46">
+        <v>0</v>
+      </c>
+      <c r="BE46" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF46" t="b">
+        <v>1</v>
+      </c>
+      <c r="BG46" s="35" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB38:BC39 N38:N39 E42:E44 BB42:BC44 L42:N44 L31:M39 N31:N36 BB5:BC36 L5:N33 E5:E39" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB40:BC41 N40:N41 E44:E46 BB44:BC46 L44:N46 L33:M41 N33:N38 BB7:BC38 L7:N35 E7:E41 BB5:BC6 L5:N6 E5:E6" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO38:AO39 AO42:AO44 AO5:AO36" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO40:AO41 AO44:AO46 AO7:AO38 AO5:AO6" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6088,7 +6260,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
complete first internally consistent version
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07974A8-8FF8-45AA-BC6A-94DD54E87149}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4C45C0-D389-4DA0-96B6-D418F6614A69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="524" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="193">
   <si>
     <t>runname</t>
   </si>
@@ -1509,11 +1509,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:BG46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="AI5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AP8" sqref="AP8"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,7 +1837,7 @@
         <v>161</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0.3</v>
@@ -2006,7 +2006,7 @@
         <v>138</v>
       </c>
       <c r="E7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0.3</v>
@@ -2019,6 +2019,12 @@
       </c>
       <c r="I7" t="b">
         <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>191</v>
+      </c>
+      <c r="K7" t="s">
+        <v>190</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -2164,7 +2170,7 @@
         <v>138</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>0.3</v>
@@ -2177,6 +2183,12 @@
       </c>
       <c r="I8" t="b">
         <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>191</v>
+      </c>
+      <c r="K8" t="s">
+        <v>190</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
@@ -2327,7 +2339,7 @@
         <v>161</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>0.3</v>
@@ -2340,6 +2352,12 @@
       </c>
       <c r="I10" t="b">
         <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" t="s">
+        <v>190</v>
       </c>
       <c r="L10" t="b">
         <v>0</v>
@@ -2485,7 +2503,7 @@
         <v>161</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0.3</v>
@@ -2654,7 +2672,7 @@
         <v>138</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>0.3</v>
@@ -2667,6 +2685,12 @@
       </c>
       <c r="I13" t="b">
         <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" t="s">
+        <v>190</v>
       </c>
       <c r="L13" t="b">
         <v>0</v>
@@ -2812,7 +2836,7 @@
         <v>161</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0.3</v>
@@ -2825,6 +2849,12 @@
       </c>
       <c r="I14" t="b">
         <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" t="s">
+        <v>190</v>
       </c>
       <c r="L14" t="b">
         <v>0</v>
@@ -6242,10 +6272,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB40:BC41 N40:N41 E44:E46 BB44:BC46 L44:N46 L33:M41 N33:N38 BB7:BC38 L7:N35 E7:E41 BB5:BC6 L5:N6 E5:E6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB40:BC41 N40:N41 E44:E46 BB44:BC46 L44:N46 L33:M41 N33:N38 BB5:BC38 L5:N35 E5:E41" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO40:AO41 AO44:AO46 AO7:AO38 AO5:AO6" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO40:AO41 AO44:AO46 AO5:AO38" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6259,8 +6289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6306,10 +6336,10 @@
         <v>2016</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -6343,7 +6373,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
calibration, before adding variable annuity
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1749E4-FDE8-4B1D-A196-D0D46595BBEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1926FD-9D54-4763-BE10-92C262244AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1530" windowWidth="16440" windowHeight="28440" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,11 @@
     <sheet name="Calibration_AV2016lag (2)" sheetId="15" r:id="rId5"/>
     <sheet name="PVB 1" sheetId="12" r:id="rId6"/>
     <sheet name="PVB 2" sheetId="13" r:id="rId7"/>
-    <sheet name="First3Years" sheetId="14" r:id="rId8"/>
-    <sheet name="DetectiveWork" sheetId="11" r:id="rId9"/>
+    <sheet name="PVB 1 (2)" sheetId="16" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId9"/>
+    <sheet name="First3Years" sheetId="14" r:id="rId10"/>
+    <sheet name="DetectiveWork" sheetId="11" r:id="rId11"/>
+    <sheet name="Variable fund" sheetId="18" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -330,8 +333,42 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{873586C9-0526-4EF8-8986-7703F1DD56A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+adj because using tier results not obl results</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="322">
   <si>
     <t>runname</t>
   </si>
@@ -1223,17 +1260,132 @@
     <t>Model ($B)</t>
   </si>
   <si>
-    <t>PVFB_inactives+terminated</t>
-  </si>
-  <si>
     <t>EEC (received in FY2016)</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Max Allowance at age 60</t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>COLA Increase</t>
+  </si>
+  <si>
+    <t>accumlative COLA</t>
+  </si>
+  <si>
+    <t>PV at 60</t>
+  </si>
+  <si>
+    <t>Diff in PV</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>PVFB_actives1_term estimated</t>
+  </si>
+  <si>
+    <t>calibrated benefit downward to match the target</t>
+  </si>
+  <si>
+    <t>Diversified Equity fund</t>
+  </si>
+  <si>
+    <t>short-term investment</t>
+  </si>
+  <si>
+    <t>Equity Securities</t>
+  </si>
+  <si>
+    <t>Debt Securities</t>
+  </si>
+  <si>
+    <t>Corporate bonds</t>
+  </si>
+  <si>
+    <t>Short-term investments</t>
+  </si>
+  <si>
+    <t>Equity Security</t>
+  </si>
+  <si>
+    <t>International equity</t>
+  </si>
+  <si>
+    <t>Collateral form Securities lending</t>
+  </si>
+  <si>
+    <t>Balanced fund</t>
+  </si>
+  <si>
+    <t>International Equity</t>
+  </si>
+  <si>
+    <t>Inflation Protected</t>
+  </si>
+  <si>
+    <t>Socially Responsible Equity Fund</t>
+  </si>
+  <si>
+    <t>Fixed Return Fund</t>
+  </si>
+  <si>
+    <t>commercial paper</t>
+  </si>
+  <si>
+    <t>short-term investment fund</t>
+  </si>
+  <si>
+    <t>Discount notes</t>
+  </si>
+  <si>
+    <t>Debt securities</t>
+  </si>
+  <si>
+    <t>U.S. Government</t>
+  </si>
+  <si>
+    <t>Corportate and Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equtiy security </t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>Collective Trust Funds</t>
+  </si>
+  <si>
+    <t>Mortgage debt security</t>
+  </si>
+  <si>
+    <t>TIPS</t>
+  </si>
+  <si>
+    <t>Fixed Income</t>
+  </si>
+  <si>
+    <t>Collateral from Security lending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="14">
+  <numFmts count="15">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1249,7 +1401,7 @@
     <numFmt numFmtId="173" formatCode="0.0"/>
     <numFmt numFmtId="174" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1409,8 +1561,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1513,6 +1671,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1590,7 +1754,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1827,22 +1991,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1861,6 +2009,113 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="37" fontId="6" fillId="4" borderId="1" xfId="4" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="1" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="7" fillId="18" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="37" fontId="7" fillId="18" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="7" fillId="18" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="18" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="37" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2198,11 +2453,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:BG46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AY16" sqref="AY16"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3192,7 +3447,7 @@
         <v>130</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0.3</v>
@@ -3694,7 +3949,7 @@
         <v>115</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0.3</v>
@@ -3858,7 +4113,7 @@
         <v>115</v>
       </c>
       <c r="E17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0.3</v>
@@ -4022,7 +4277,7 @@
         <v>115</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0.3</v>
@@ -4186,7 +4441,7 @@
         <v>115</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0.3</v>
@@ -4350,7 +4605,7 @@
         <v>115</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0.3</v>
@@ -4514,7 +4769,7 @@
         <v>114</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0.3</v>
@@ -4682,7 +4937,7 @@
         <v>114</v>
       </c>
       <c r="E23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0.3</v>
@@ -4846,7 +5101,7 @@
         <v>130</v>
       </c>
       <c r="E24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>0.3</v>
@@ -7019,6 +7274,828 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12C2C70-1D38-4C9C-8A29-A9ED22FEC02C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4FDDF8-106A-47EA-BD4C-5B4A1371B873}">
+  <dimension ref="B2:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="27">
+        <v>70000777</v>
+      </c>
+      <c r="D4" s="27">
+        <v>43629545</v>
+      </c>
+      <c r="G4">
+        <v>20292733</v>
+      </c>
+      <c r="I4" s="29">
+        <f>G4/D4</f>
+        <v>0.46511447689862456</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="27">
+        <v>73323430</v>
+      </c>
+      <c r="D5" s="27">
+        <v>50095723</v>
+      </c>
+      <c r="G5">
+        <v>22004183</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="C6" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587985C1-19B7-4168-A948-80D126BFDABB}">
+  <dimension ref="B2:I57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="9" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="D2" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2015</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2014</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="C4" t="s">
+        <v>296</v>
+      </c>
+      <c r="D4" s="27">
+        <v>135558</v>
+      </c>
+      <c r="E4" s="27">
+        <v>65825</v>
+      </c>
+      <c r="F4" s="27">
+        <v>29570</v>
+      </c>
+      <c r="G4" s="27">
+        <v>33499</v>
+      </c>
+      <c r="H4" s="27">
+        <v>37417</v>
+      </c>
+      <c r="I4" s="27">
+        <v>30565</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="C5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D5" s="27">
+        <v>6125780</v>
+      </c>
+      <c r="E5" s="27">
+        <v>6031258</v>
+      </c>
+      <c r="F5" s="27">
+        <v>2206416</v>
+      </c>
+      <c r="G5" s="27">
+        <v>2798742</v>
+      </c>
+      <c r="H5" s="27">
+        <v>3257181</v>
+      </c>
+      <c r="I5" s="27">
+        <v>3104060</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="C6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" s="27">
+        <v>127150</v>
+      </c>
+      <c r="E6" s="27">
+        <v>106307</v>
+      </c>
+      <c r="F6" s="27">
+        <v>50541</v>
+      </c>
+      <c r="G6" s="27">
+        <v>62026</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="C7" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0</v>
+      </c>
+      <c r="H7" s="27">
+        <v>72911</v>
+      </c>
+      <c r="I7" s="27">
+        <v>134980</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="C10" t="s">
+        <v>300</v>
+      </c>
+      <c r="D10" s="27">
+        <v>849</v>
+      </c>
+      <c r="E10" s="27">
+        <v>3576</v>
+      </c>
+      <c r="F10" s="27">
+        <v>432</v>
+      </c>
+      <c r="G10" s="27">
+        <v>673</v>
+      </c>
+      <c r="H10" s="27">
+        <v>1011</v>
+      </c>
+      <c r="I10" s="27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="C11" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" s="27">
+        <v>70562</v>
+      </c>
+      <c r="E11" s="27">
+        <v>83333</v>
+      </c>
+      <c r="F11" s="27">
+        <v>24393</v>
+      </c>
+      <c r="G11" s="27">
+        <v>35113</v>
+      </c>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="C12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0</v>
+      </c>
+      <c r="H12" s="27">
+        <v>50232</v>
+      </c>
+      <c r="I12" s="27">
+        <v>66118</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="C13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="C16" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="27">
+        <v>80</v>
+      </c>
+      <c r="E16" s="27">
+        <v>53</v>
+      </c>
+      <c r="F16" s="27">
+        <v>75</v>
+      </c>
+      <c r="G16" s="27">
+        <v>124</v>
+      </c>
+      <c r="H16" s="27">
+        <v>139</v>
+      </c>
+      <c r="I16" s="27">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="C17" t="s">
+        <v>302</v>
+      </c>
+      <c r="D17" s="27">
+        <v>12076</v>
+      </c>
+      <c r="E17" s="27">
+        <v>12436</v>
+      </c>
+      <c r="F17" s="27">
+        <v>8012</v>
+      </c>
+      <c r="G17" s="27">
+        <v>10669</v>
+      </c>
+      <c r="H17" s="27">
+        <v>12639</v>
+      </c>
+      <c r="I17" s="27">
+        <v>11895</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="C20" t="s">
+        <v>300</v>
+      </c>
+      <c r="D20" s="27">
+        <v>3</v>
+      </c>
+      <c r="E20" s="27">
+        <v>23</v>
+      </c>
+      <c r="F20" s="27">
+        <v>12</v>
+      </c>
+      <c r="G20" s="27">
+        <v>10</v>
+      </c>
+      <c r="H20" s="27">
+        <v>11</v>
+      </c>
+      <c r="I20" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="C21" t="s">
+        <v>301</v>
+      </c>
+      <c r="D21" s="27">
+        <v>4596</v>
+      </c>
+      <c r="E21" s="27">
+        <v>4761</v>
+      </c>
+      <c r="F21" s="27">
+        <v>3960</v>
+      </c>
+      <c r="G21" s="27">
+        <v>4791</v>
+      </c>
+      <c r="H21" s="27">
+        <v>5723</v>
+      </c>
+      <c r="I21" s="27">
+        <v>5923</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="C24" t="s">
+        <v>300</v>
+      </c>
+      <c r="D24" s="27">
+        <v>453</v>
+      </c>
+      <c r="E24" s="27">
+        <v>662</v>
+      </c>
+      <c r="F24" s="27">
+        <v>24</v>
+      </c>
+      <c r="G24" s="27">
+        <v>461</v>
+      </c>
+      <c r="H24" s="27">
+        <v>532</v>
+      </c>
+      <c r="I24" s="27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="C25" t="s">
+        <v>301</v>
+      </c>
+      <c r="D25" s="27">
+        <v>11654</v>
+      </c>
+      <c r="E25" s="27">
+        <v>11320</v>
+      </c>
+      <c r="F25" s="27">
+        <v>7650</v>
+      </c>
+      <c r="G25" s="27">
+        <v>7576</v>
+      </c>
+      <c r="H25" s="27">
+        <v>7413</v>
+      </c>
+      <c r="I25" s="27">
+        <v>6268</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="C26" t="s">
+        <v>302</v>
+      </c>
+      <c r="D26" s="27">
+        <v>717</v>
+      </c>
+      <c r="E26" s="27">
+        <v>516</v>
+      </c>
+      <c r="F26" s="27">
+        <v>158</v>
+      </c>
+      <c r="G26" s="27">
+        <v>233</v>
+      </c>
+      <c r="H26" s="27">
+        <v>301</v>
+      </c>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D27" s="27">
+        <v>69204</v>
+      </c>
+      <c r="E27" s="27">
+        <v>80011</v>
+      </c>
+      <c r="F27" s="27">
+        <v>84226</v>
+      </c>
+      <c r="G27" s="27">
+        <v>200212</v>
+      </c>
+      <c r="H27" s="27">
+        <v>138606</v>
+      </c>
+      <c r="I27" s="27">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" s="27">
+        <f t="shared" ref="D29:I29" si="0">SUM(D4:D27)</f>
+        <v>6558682</v>
+      </c>
+      <c r="E29" s="163">
+        <f t="shared" si="0"/>
+        <v>6400081</v>
+      </c>
+      <c r="F29" s="163">
+        <f t="shared" si="0"/>
+        <v>2415469</v>
+      </c>
+      <c r="G29" s="163">
+        <f t="shared" si="0"/>
+        <v>3154129</v>
+      </c>
+      <c r="H29" s="163">
+        <f t="shared" si="0"/>
+        <v>3584116</v>
+      </c>
+      <c r="I29" s="163">
+        <f t="shared" si="0"/>
+        <v>3361415</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="D30" s="27"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="D31" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E31" s="1">
+        <v>2017</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2015</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2014</v>
+      </c>
+      <c r="I31" s="1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D32" s="27"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C33" t="s">
+        <v>309</v>
+      </c>
+      <c r="E33" s="27">
+        <v>230093</v>
+      </c>
+      <c r="F33" s="27">
+        <v>1070574</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="C34" t="s">
+        <v>310</v>
+      </c>
+      <c r="E34" s="27">
+        <v>557945</v>
+      </c>
+      <c r="F34" s="27">
+        <v>1025446</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="C35" t="s">
+        <v>311</v>
+      </c>
+      <c r="E35" s="27">
+        <v>282248</v>
+      </c>
+      <c r="F35" s="27">
+        <v>83294</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C37" t="s">
+        <v>313</v>
+      </c>
+      <c r="E37" s="27">
+        <v>7947669</v>
+      </c>
+      <c r="F37" s="27">
+        <v>5924318</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="C38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E38" s="27">
+        <v>7753224</v>
+      </c>
+      <c r="F38" s="27">
+        <v>8730691</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E40" s="27">
+        <v>21086002</v>
+      </c>
+      <c r="F40" s="27">
+        <v>22284583</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="E41" s="27"/>
+      <c r="F41" s="27"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E42" s="27">
+        <v>7523885</v>
+      </c>
+      <c r="F42" s="27">
+        <v>6872850</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C44" t="s">
+        <v>302</v>
+      </c>
+      <c r="E44" s="27">
+        <v>15734149</v>
+      </c>
+      <c r="F44" s="27">
+        <v>11507149</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="C45" t="s">
+        <v>318</v>
+      </c>
+      <c r="E45" s="27">
+        <v>495540</v>
+      </c>
+      <c r="F45" s="27">
+        <v>485191</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="C46" t="s">
+        <v>319</v>
+      </c>
+      <c r="E46" s="27">
+        <v>2682432</v>
+      </c>
+      <c r="F46" s="27">
+        <v>2399270</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="C47" t="s">
+        <v>320</v>
+      </c>
+      <c r="E47" s="27">
+        <v>1791033</v>
+      </c>
+      <c r="F47" s="27">
+        <v>1691577</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E49" s="27">
+        <v>1530310</v>
+      </c>
+      <c r="F49" s="27">
+        <v>1774456</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" s="28">
+        <f>SUM(E33:E49)</f>
+        <v>67614530</v>
+      </c>
+      <c r="F50" s="28">
+        <f>SUM(F33:F49)</f>
+        <v>63849399</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="E51" s="164">
+        <f>E50/F50-1</f>
+        <v>5.8968934069371537E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="E53" s="27">
+        <v>50095723</v>
+      </c>
+      <c r="F53" s="27">
+        <v>43629545</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="E54">
+        <f>E53/F53</f>
+        <v>1.148206404627873</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="E57">
+        <f>82961/74494</f>
+        <v>1.1136601605498428</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -7160,11 +8237,11 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <f>F2</f>
+        <f t="shared" ref="E2:E25" si="0">F2</f>
         <v>0.13</v>
       </c>
       <c r="F2" s="6">
-        <f t="shared" ref="F2:F5" si="0">B2 - C2^2/2</f>
+        <f t="shared" ref="F2:F10" si="1">B2 - C2^2/2</f>
         <v>0.13</v>
       </c>
       <c r="G2" t="s">
@@ -7185,11 +8262,11 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E5" si="1">F3</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
       <c r="G3" t="s">
@@ -7210,11 +8287,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="6">
         <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-      <c r="F4" s="6">
-        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="G4" t="s">
@@ -7235,11 +8312,11 @@
         <v>30</v>
       </c>
       <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F5" s="6">
         <f t="shared" si="1"/>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F5" s="6">
-        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G5" t="s">
@@ -7260,11 +8337,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="4">
-        <f>F6</f>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" ref="F6:F9" si="2">B6 - C6^2/2</f>
+        <f t="shared" si="1"/>
         <v>0.13</v>
       </c>
       <c r="G6" t="s">
@@ -7285,11 +8362,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" ref="E7:E9" si="3">F7</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
       <c r="G7" t="s">
@@ -7310,11 +8387,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="G8" t="s">
@@ -7335,11 +8412,11 @@
         <v>10</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G9" t="s">
@@ -7360,11 +8437,11 @@
         <v>5</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" ref="E10" si="4">F10</f>
+        <f t="shared" si="0"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" ref="F10" si="5">B10 - C10^2/2</f>
+        <f t="shared" si="1"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G10" t="s">
@@ -7385,11 +8462,11 @@
         <v>15</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11" si="6">F11</f>
+        <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" ref="F11:F20" si="7">B11 - C11^2/2</f>
+        <f t="shared" ref="F11:F20" si="2">B11 - C11^2/2</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G11" t="s">
@@ -7410,11 +8487,11 @@
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <f>F12</f>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.13</v>
       </c>
       <c r="G12" t="s">
@@ -7435,11 +8512,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" ref="E13:E16" si="8">F13</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.128</v>
       </c>
       <c r="G13" t="s">
@@ -7460,11 +8537,11 @@
         <v>1</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="G14" t="s">
@@ -7485,11 +8562,11 @@
         <v>10</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="G15" t="s">
@@ -7510,11 +8587,11 @@
         <v>20</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="0"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G16" t="s">
@@ -7535,11 +8612,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="4">
-        <f>F17</f>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.13</v>
       </c>
       <c r="G17" t="s">
@@ -7560,11 +8637,11 @@
         <v>1</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" ref="E18:E20" si="9">F18</f>
+        <f t="shared" si="0"/>
         <v>0.128</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.128</v>
       </c>
       <c r="G18" t="s">
@@ -7585,11 +8662,11 @@
         <v>1</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="G19" t="s">
@@ -7610,11 +8687,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="0"/>
         <v>-0.24</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="2"/>
         <v>-0.24</v>
       </c>
       <c r="G20" t="s">
@@ -7635,11 +8712,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" ref="E21:E24" si="10">F21</f>
+        <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="F21" s="6">
-        <f t="shared" ref="F21:F28" si="11">B21 - C21^2/2</f>
+        <f t="shared" ref="F21:F28" si="3">B21 - C21^2/2</f>
         <v>0.12</v>
       </c>
       <c r="G21" t="s">
@@ -7660,11 +8737,11 @@
         <v>1</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.13</v>
       </c>
       <c r="G22" t="s">
@@ -7685,11 +8762,11 @@
         <v>1</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.11</v>
       </c>
       <c r="G23" t="s">
@@ -7710,11 +8787,11 @@
         <v>26</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="G24" t="s">
@@ -7735,11 +8812,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f>F25</f>
+        <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.13</v>
       </c>
       <c r="G25" t="s">
@@ -7760,11 +8837,11 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" ref="E26:E32" si="12">F26</f>
+        <f t="shared" ref="E26:E32" si="4">F26</f>
         <v>0.128</v>
       </c>
       <c r="F26" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.128</v>
       </c>
       <c r="G26" t="s">
@@ -7785,11 +8862,11 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
       <c r="F27" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="G27" t="s">
@@ -7810,11 +8887,11 @@
         <v>1</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>-0.24</v>
       </c>
       <c r="F28" s="6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="3"/>
         <v>-0.24</v>
       </c>
       <c r="G28" t="s">
@@ -7835,11 +8912,11 @@
         <v>1</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>0.12</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" ref="F29:F32" si="13">B29 - C29^2/2</f>
+        <f>B29 - C29^2/2</f>
         <v>0.12</v>
       </c>
       <c r="G29" t="s">
@@ -7860,11 +8937,11 @@
         <v>1</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>0.13</v>
       </c>
       <c r="F30" s="6">
-        <f t="shared" si="13"/>
+        <f>B30 - C30^2/2</f>
         <v>0.13</v>
       </c>
       <c r="G30" t="s">
@@ -7885,11 +8962,11 @@
         <v>1</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
       <c r="F31" s="6">
-        <f t="shared" si="13"/>
+        <f>B31 - C31^2/2</f>
         <v>0.11</v>
       </c>
       <c r="G31" t="s">
@@ -7910,11 +8987,11 @@
         <v>26</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="12"/>
+        <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F32" s="6">
-        <f t="shared" si="13"/>
+        <f>B32 - C32^2/2</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G32" t="s">
@@ -8376,20 +9453,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6BF394-4CD7-4BCB-B328-ED95773294C9}">
-  <dimension ref="B2:H43"/>
+  <dimension ref="B2:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.28515625" style="105" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="105" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="106" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="106" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="106" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="106" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" style="106" customWidth="1"/>
-    <col min="7" max="7" width="36" style="105" customWidth="1"/>
+    <col min="7" max="7" width="45.140625" style="105" customWidth="1"/>
     <col min="8" max="8" width="28.85546875" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -8409,7 +9486,7 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="116" t="s">
         <v>233</v>
       </c>
       <c r="C3" s="107">
@@ -8422,27 +9499,27 @@
       <c r="E3" s="114">
         <v>37.090000000000003</v>
       </c>
-      <c r="F3" s="122">
+      <c r="F3" s="117">
         <f>E3/D3 -1</f>
         <v>-1.5322684213789239E-2</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="116" t="s">
         <v>234</v>
       </c>
       <c r="C4" s="108">
         <v>1062059552</v>
       </c>
       <c r="D4" s="114">
-        <f t="shared" ref="D4:D39" si="0">C4/1000000000</f>
+        <f t="shared" ref="D4:D40" si="0">C4/1000000000</f>
         <v>1.062059552</v>
       </c>
-      <c r="E4" s="126">
+      <c r="E4" s="121">
         <v>0.98</v>
       </c>
-      <c r="F4" s="127">
-        <f t="shared" ref="F4:F39" si="1">E4/D4 -1</f>
+      <c r="F4" s="122">
+        <f t="shared" ref="F4:F40" si="1">E4/D4 -1</f>
         <v>-7.7264548720898829E-2</v>
       </c>
       <c r="G4" s="105" t="s">
@@ -8450,7 +9527,7 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="116" t="s">
         <v>235</v>
       </c>
       <c r="C5" s="109">
@@ -8463,559 +9540,581 @@
       <c r="E5" s="114">
         <v>0.41</v>
       </c>
-      <c r="F5" s="122">
+      <c r="F5" s="117">
         <f t="shared" si="1"/>
         <v>1.0109735020278343E-2</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B6" s="105" t="s">
-        <v>236</v>
+      <c r="B6" s="116" t="s">
+        <v>293</v>
       </c>
       <c r="C6" s="109">
-        <v>2190015114</v>
+        <f>C7+C8-C14</f>
+        <v>1343967236</v>
       </c>
       <c r="D6" s="114">
         <f t="shared" si="0"/>
-        <v>2.1900151139999999</v>
+        <v>1.3439672359999999</v>
       </c>
       <c r="E6" s="114"/>
-      <c r="F6" s="122"/>
-      <c r="H6" s="28">
-        <f>C6+C7-C11-C12</f>
-        <v>808097004</v>
+      <c r="F6" s="117"/>
+      <c r="G6" s="105" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="20.25" customHeight="1">
       <c r="B7" s="105" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C7" s="109">
-        <v>125975786</v>
+        <v>2190015114</v>
       </c>
       <c r="D7" s="114">
         <f t="shared" si="0"/>
-        <v>0.12597578600000001</v>
+        <v>2.1900151139999999</v>
       </c>
       <c r="E7" s="114"/>
-      <c r="F7" s="122"/>
+      <c r="F7" s="117"/>
+      <c r="H7" s="28">
+        <f>C7+C8-C13-C14</f>
+        <v>808097004</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="20.25" customHeight="1">
       <c r="B8" s="105" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C8" s="109">
-        <v>2659607405</v>
+        <v>125975786</v>
       </c>
       <c r="D8" s="114">
         <f t="shared" si="0"/>
+        <v>0.12597578600000001</v>
+      </c>
+      <c r="E8" s="114"/>
+      <c r="F8" s="117"/>
+    </row>
+    <row r="9" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B9" s="105" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="109">
+        <v>2659607405</v>
+      </c>
+      <c r="D9" s="114">
+        <f t="shared" si="0"/>
         <v>2.659607405</v>
       </c>
-      <c r="E8" s="114"/>
-      <c r="F8" s="122"/>
-    </row>
-    <row r="9" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D9" s="114"/>
       <c r="E9" s="114"/>
-      <c r="F9" s="122"/>
+      <c r="F9" s="117"/>
     </row>
     <row r="10" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B10" s="121" t="s">
+      <c r="C10" s="162"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="117"/>
+    </row>
+    <row r="11" spans="2:8" ht="20.25" customHeight="1">
+      <c r="D11" s="114"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="117"/>
+    </row>
+    <row r="12" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B12" s="116" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="106">
+      <c r="C12" s="106">
         <v>39535995292</v>
       </c>
-      <c r="D10" s="114">
+      <c r="D12" s="114">
         <f t="shared" si="0"/>
         <v>39.535995292000003</v>
       </c>
-      <c r="E10" s="114">
+      <c r="E12" s="114">
         <v>39.200000000000003</v>
       </c>
-      <c r="F10" s="122">
+      <c r="F12" s="117">
         <f t="shared" si="1"/>
         <v>-8.4984655000701625E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B11" s="105" t="s">
+    <row r="13" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B13" s="105" t="s">
         <v>241</v>
       </c>
-      <c r="C11" s="111">
+      <c r="C13" s="111">
         <v>535870232</v>
       </c>
-      <c r="D11" s="114">
+      <c r="D13" s="114">
         <f t="shared" si="0"/>
         <v>0.53587023199999995</v>
       </c>
-      <c r="E11" s="114"/>
-      <c r="F11" s="122"/>
-      <c r="H11" s="28"/>
-    </row>
-    <row r="12" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B12" s="105" t="s">
+      <c r="E13" s="114"/>
+      <c r="F13" s="117"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B14" s="105" t="s">
         <v>242</v>
       </c>
-      <c r="C12" s="110">
+      <c r="C14" s="110">
         <v>972023664</v>
       </c>
-      <c r="D12" s="114">
+      <c r="D14" s="114">
         <f t="shared" si="0"/>
         <v>0.97202366399999995</v>
       </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="122"/>
-    </row>
-    <row r="13" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B13" s="121" t="s">
-        <v>282</v>
-      </c>
-      <c r="C13" s="110">
-        <f>SUM(C11:C12)</f>
-        <v>1507893896</v>
-      </c>
-      <c r="D13" s="114"/>
-      <c r="E13" s="114"/>
-      <c r="F13" s="122"/>
-    </row>
-    <row r="14" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B14" s="125" t="s">
+      <c r="E14" s="114"/>
+      <c r="F14" s="117"/>
+    </row>
+    <row r="15" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B15" s="120" t="s">
         <v>243</v>
       </c>
-      <c r="C14" s="110">
+      <c r="C15" s="110">
         <v>3066827192</v>
       </c>
-      <c r="D14" s="114">
+      <c r="D15" s="114">
         <f t="shared" si="0"/>
         <v>3.0668271919999999</v>
       </c>
-      <c r="E14" s="114"/>
-      <c r="F14" s="122"/>
-    </row>
-    <row r="15" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D15" s="114"/>
       <c r="E15" s="114"/>
-      <c r="F15" s="122"/>
+      <c r="F15" s="117"/>
     </row>
     <row r="16" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B16" s="105" t="s">
+      <c r="D16" s="114"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="117"/>
+    </row>
+    <row r="17" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B17" s="105" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="106">
+      <c r="C17" s="106">
         <v>37988259515</v>
       </c>
-      <c r="D16" s="114">
+      <c r="D17" s="114">
         <f t="shared" si="0"/>
         <v>37.988259515000003</v>
       </c>
-      <c r="E16" s="114"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="105" t="s">
+      <c r="E17" s="114"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="105" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B17" s="105" t="s">
+    <row r="18" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B18" s="105" t="s">
         <v>155</v>
       </c>
-      <c r="C17" s="106">
+      <c r="C18" s="106">
         <v>2813575411</v>
       </c>
-      <c r="D17" s="114">
+      <c r="D18" s="114">
         <f t="shared" si="0"/>
         <v>2.813575411</v>
       </c>
-      <c r="E17" s="114"/>
-      <c r="F17" s="122"/>
-      <c r="G17" s="105" t="s">
+      <c r="E18" s="114"/>
+      <c r="F18" s="117"/>
+      <c r="G18" s="105" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B18" s="121" t="s">
+    <row r="19" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B19" s="116" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="106">
+      <c r="C19" s="106">
         <v>849689324</v>
       </c>
-      <c r="D18" s="114">
-        <f>C18/1000000000</f>
+      <c r="D19" s="114">
+        <f>C19/1000000000</f>
         <v>0.84968932399999997</v>
       </c>
-      <c r="E18" s="114">
+      <c r="E19" s="114">
         <v>1.03</v>
       </c>
-      <c r="F18" s="127">
+      <c r="F19" s="122">
         <f t="shared" si="1"/>
         <v>0.21220776924814011</v>
       </c>
-      <c r="G18" s="105" t="s">
+      <c r="G19" s="105" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B19" s="121" t="s">
+    <row r="20" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B20" s="116" t="s">
         <v>279</v>
       </c>
-      <c r="C19" s="106">
-        <f>C17+C16</f>
+      <c r="C20" s="106">
+        <f>C18+C17</f>
         <v>40801834926</v>
       </c>
-      <c r="D19" s="114">
-        <f>C19/1000000000</f>
+      <c r="D20" s="114">
+        <f>C20/1000000000</f>
         <v>40.801834925999998</v>
       </c>
-      <c r="E19" s="114">
+      <c r="E20" s="114">
         <v>41.6</v>
       </c>
-      <c r="F19" s="122">
+      <c r="F20" s="117">
         <f t="shared" si="1"/>
         <v>1.9561989686189163E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D20" s="114"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="122"/>
-    </row>
     <row r="21" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B21" s="121" t="s">
+      <c r="D21" s="114"/>
+      <c r="E21" s="114"/>
+      <c r="F21" s="117"/>
+    </row>
+    <row r="22" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B22" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="C21" s="106">
-        <f>SUM(C10,C11,C12,C14)</f>
+      <c r="C22" s="106">
+        <f>SUM(C12,C13,C14,C15)</f>
         <v>44110716380</v>
       </c>
-      <c r="D21" s="114">
+      <c r="D22" s="114">
         <f t="shared" si="0"/>
         <v>44.11071638</v>
       </c>
-      <c r="E21" s="114">
+      <c r="E22" s="114">
         <v>43.86</v>
       </c>
-      <c r="F21" s="122">
+      <c r="F22" s="117">
         <f t="shared" si="1"/>
         <v>-5.6837975117011164E-3</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B22" s="121" t="s">
+    <row r="23" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B23" s="116" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="112">
-        <f>SUM(C16,C17,C18)</f>
+      <c r="C23" s="112">
+        <f>SUM(C17,C18,C19)</f>
         <v>41651524250</v>
       </c>
-      <c r="D22" s="114">
+      <c r="D23" s="114">
         <f t="shared" si="0"/>
         <v>41.651524250000001</v>
       </c>
-      <c r="E22" s="114">
+      <c r="E23" s="114">
         <v>42.6</v>
       </c>
-      <c r="F22" s="122">
+      <c r="F23" s="117">
         <f t="shared" si="1"/>
         <v>2.2771693643360402E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D23" s="114"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="122"/>
-    </row>
     <row r="24" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B24" s="121" t="s">
+      <c r="D24" s="114"/>
+      <c r="E24" s="114"/>
+      <c r="F24" s="117"/>
+    </row>
+    <row r="25" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B25" s="116" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="106">
-        <f>SUM(C21:C22)</f>
+      <c r="C25" s="106">
+        <f>SUM(C22:C23)</f>
         <v>85762240630</v>
       </c>
-      <c r="D24" s="114">
+      <c r="D25" s="114">
         <f t="shared" si="0"/>
         <v>85.762240629999994</v>
       </c>
-      <c r="E24" s="114">
+      <c r="E25" s="114">
         <v>86.5</v>
       </c>
-      <c r="F24" s="122">
+      <c r="F25" s="117">
         <f t="shared" si="1"/>
         <v>8.6023798419969655E-3</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D25" s="114"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="122"/>
-    </row>
     <row r="26" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B26" s="125" t="s">
+      <c r="D26" s="114"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="117"/>
+    </row>
+    <row r="27" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B27" s="120" t="s">
         <v>154</v>
       </c>
-      <c r="C26" s="110">
+      <c r="C27" s="110">
         <v>23738166660</v>
       </c>
-      <c r="D26" s="114">
+      <c r="D27" s="114">
         <f t="shared" si="0"/>
         <v>23.738166660000001</v>
       </c>
-      <c r="E26" s="114">
+      <c r="E27" s="114">
         <v>21.5</v>
       </c>
-      <c r="F26" s="127">
+      <c r="F27" s="122">
         <f t="shared" si="1"/>
         <v>-9.4285573610510709E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B27" s="121" t="s">
+    <row r="28" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B28" s="116" t="s">
         <v>244</v>
       </c>
-      <c r="C27" s="113">
-        <f>SUM(C26,C11,C12,C14,C22)</f>
+      <c r="C28" s="113">
+        <f>SUM(C27,C13,C14,C15,C23)</f>
         <v>69964411998</v>
       </c>
-      <c r="D27" s="114">
+      <c r="D28" s="114">
         <f t="shared" si="0"/>
         <v>69.964411998000003</v>
       </c>
-      <c r="E27" s="114">
+      <c r="E28" s="114">
         <v>68.7</v>
       </c>
-      <c r="F27" s="122">
+      <c r="F28" s="117">
         <f t="shared" si="1"/>
         <v>-1.807221645822088E-2</v>
       </c>
-      <c r="G27" s="105" t="s">
+      <c r="G28" s="105" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D28" s="114"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="122"/>
-    </row>
     <row r="29" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B29" s="121" t="s">
+      <c r="D29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="117"/>
+    </row>
+    <row r="30" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B30" s="116" t="s">
         <v>249</v>
       </c>
-      <c r="C29" s="106">
+      <c r="C30" s="106">
         <v>3954653723</v>
       </c>
-      <c r="D29" s="114">
+      <c r="D30" s="114">
         <f t="shared" si="0"/>
         <v>3.9546537229999998</v>
       </c>
-      <c r="E29" s="114">
+      <c r="E30" s="114">
         <v>3.95</v>
       </c>
-      <c r="F29" s="122">
+      <c r="F30" s="117">
         <f t="shared" si="1"/>
         <v>-1.1767712993261403E-3</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D30" s="114"/>
-      <c r="F30" s="122"/>
-    </row>
     <row r="31" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B31" s="121" t="s">
-        <v>283</v>
-      </c>
-      <c r="C31" s="106">
+      <c r="D31" s="114"/>
+      <c r="F31" s="117"/>
+    </row>
+    <row r="32" spans="2:8" ht="20.25" customHeight="1">
+      <c r="B32" s="116" t="s">
+        <v>282</v>
+      </c>
+      <c r="C32" s="106">
         <v>173696000</v>
       </c>
-      <c r="D31" s="128">
-        <f>C31/1000000000</f>
+      <c r="D32" s="123">
+        <f>C32/1000000000</f>
         <v>0.17369599999999999</v>
       </c>
-      <c r="E31" s="124">
+      <c r="E32" s="119">
         <v>0.19</v>
       </c>
-      <c r="F31" s="122">
+      <c r="F32" s="117">
         <f t="shared" si="1"/>
         <v>9.3865143699336961E-2</v>
       </c>
-      <c r="G31" s="105" t="s">
+      <c r="G32" s="105" t="s">
         <v>257</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B32" s="121" t="s">
+    <row r="33" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B33" s="116" t="s">
         <v>247</v>
       </c>
-      <c r="C32" s="106">
+      <c r="C33" s="106">
         <v>1172161054</v>
       </c>
-      <c r="D32" s="114">
+      <c r="D33" s="114">
         <f t="shared" si="0"/>
         <v>1.172161054</v>
       </c>
-      <c r="E32" s="124">
+      <c r="E33" s="119">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F32" s="122">
+      <c r="F33" s="117">
         <f t="shared" si="1"/>
         <v>-1.8906151099608248E-2</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H33" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B33" s="121" t="s">
+      <c r="K33">
+        <v>13.5</v>
+      </c>
+      <c r="L33">
+        <v>12.8</v>
+      </c>
+      <c r="M33">
+        <f>L33/K33</f>
+        <v>0.94814814814814818</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B34" s="116" t="s">
         <v>248</v>
       </c>
-      <c r="C33" s="106">
+      <c r="C34" s="106">
         <v>2663071096</v>
       </c>
-      <c r="D33" s="114">
+      <c r="D34" s="114">
         <f t="shared" si="0"/>
         <v>2.6630710959999999</v>
       </c>
-      <c r="E33" s="106">
+      <c r="E34" s="106">
         <v>2.67</v>
       </c>
-      <c r="F33" s="122">
+      <c r="F34" s="117">
         <f t="shared" si="1"/>
         <v>2.6018471720141712E-3</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B34" s="121" t="s">
+    <row r="35" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B35" s="116" t="s">
         <v>276</v>
       </c>
-      <c r="C34" s="106">
+      <c r="C35" s="106">
         <v>3889709927</v>
       </c>
-      <c r="D34" s="114">
+      <c r="D35" s="114">
         <f t="shared" si="0"/>
         <v>3.8897099270000002</v>
       </c>
-      <c r="E34" s="123">
+      <c r="E35" s="118">
         <v>3.82</v>
       </c>
-      <c r="F34" s="122">
+      <c r="F35" s="117">
         <f t="shared" si="1"/>
         <v>-1.7921626113072464E-2</v>
       </c>
-      <c r="G34" s="105" t="s">
+      <c r="G35" s="105" t="s">
         <v>252</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D35" s="114"/>
-      <c r="F35" s="122"/>
-    </row>
-    <row r="36" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B36" s="121" t="s">
+    <row r="36" spans="2:13" ht="20.25" customHeight="1">
+      <c r="D36" s="114"/>
+      <c r="F36" s="117"/>
+    </row>
+    <row r="37" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B37" s="116" t="s">
         <v>251</v>
       </c>
-      <c r="C36" s="106">
+      <c r="C37" s="106">
         <v>9224267647</v>
       </c>
-      <c r="D36" s="114">
+      <c r="D37" s="114">
         <f t="shared" si="0"/>
         <v>9.2242676469999996</v>
       </c>
-      <c r="E36" s="123">
+      <c r="E37" s="118">
         <v>9.14</v>
       </c>
-      <c r="F36" s="122">
+      <c r="F37" s="117">
         <f t="shared" si="1"/>
         <v>-9.1354295240343442E-3</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H37" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="20.25" customHeight="1">
-      <c r="D37" s="114"/>
-      <c r="F37" s="122"/>
-    </row>
-    <row r="38" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B38" s="121" t="s">
+    <row r="38" spans="2:13" ht="20.25" customHeight="1">
+      <c r="D38" s="114"/>
+      <c r="F38" s="117"/>
+    </row>
+    <row r="39" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B39" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="106">
+      <c r="C39" s="106">
         <v>43629545000</v>
       </c>
-      <c r="D38" s="114">
+      <c r="D39" s="114">
         <f t="shared" si="0"/>
         <v>43.629545</v>
       </c>
-      <c r="E38" s="106">
+      <c r="E39" s="106">
         <v>42.8</v>
       </c>
-      <c r="F38" s="122">
+      <c r="F39" s="117">
         <f t="shared" si="1"/>
         <v>-1.901337728825736E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B39" s="121" t="s">
+    <row r="40" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B40" s="116" t="s">
         <v>250</v>
       </c>
-      <c r="C39" s="106">
+      <c r="C40" s="106">
         <v>41015087000</v>
       </c>
-      <c r="D39" s="114">
+      <c r="D40" s="114">
         <f t="shared" si="0"/>
         <v>41.015087000000001</v>
       </c>
-      <c r="E39" s="106">
+      <c r="E40" s="106">
         <v>39.799999999999997</v>
       </c>
-      <c r="F39" s="122">
+      <c r="F40" s="117">
         <f t="shared" si="1"/>
         <v>-2.9625366880240978E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B40" s="105" t="s">
+    <row r="41" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B41" s="105" t="s">
         <v>255</v>
       </c>
-      <c r="C40" s="115">
-        <f>C38/C27</f>
+      <c r="C41" s="115">
+        <f>C39/C28</f>
         <v>0.62359625063735535</v>
       </c>
-      <c r="F40" s="122"/>
-    </row>
-    <row r="41" spans="2:8" ht="20.25" customHeight="1">
-      <c r="B41" s="105" t="s">
+      <c r="F41" s="117"/>
+    </row>
+    <row r="42" spans="2:13" ht="20.25" customHeight="1">
+      <c r="B42" s="105" t="s">
         <v>254</v>
       </c>
-      <c r="C41" s="115">
-        <f>C39/C27</f>
+      <c r="C42" s="115">
+        <f>C40/C28</f>
         <v>0.58622785254269638</v>
       </c>
-      <c r="F41" s="122"/>
-    </row>
-    <row r="42" spans="2:8" ht="20.25" customHeight="1">
-      <c r="F42" s="122"/>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="121" t="s">
+      <c r="F42" s="117"/>
+    </row>
+    <row r="43" spans="2:13" ht="20.25" customHeight="1">
+      <c r="F43" s="117"/>
+    </row>
+    <row r="44" spans="2:13">
+      <c r="B44" s="116" t="s">
         <v>277</v>
       </c>
-      <c r="C43" s="115">
-        <f>C34/C36</f>
+      <c r="C44" s="115">
+        <f>C35/C37</f>
         <v>0.42168224902548734</v>
       </c>
-      <c r="F43" s="122"/>
+      <c r="F44" s="117"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -9033,7 +10132,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9553,18 +10652,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="14.25">
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
     </row>
     <row r="2" spans="2:11" ht="14.25">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="166" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
     </row>
     <row r="3" spans="2:11" ht="25.5">
       <c r="C3" s="36">
@@ -9835,8 +10934,8 @@
         <f>D24+D26</f>
         <v>37988259515</v>
       </c>
-      <c r="H24" s="118"/>
-      <c r="I24" s="119"/>
+      <c r="H24" s="167"/>
+      <c r="I24" s="168"/>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="39" t="s">
@@ -10079,7 +11178,7 @@
   <dimension ref="A1:K165"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48:D50"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10665,36 +11764,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="169" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
+      <c r="B1" s="169"/>
+      <c r="C1" s="169"/>
+      <c r="D1" s="169"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="169" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
+      <c r="B2" s="169"/>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="169" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="169"/>
     </row>
     <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="120" t="s">
+      <c r="A4" s="169" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
+      <c r="B4" s="169"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="169"/>
     </row>
     <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="64"/>
@@ -10965,7 +12064,7 @@
         <v>870729599</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:6">
       <c r="B33" s="74" t="s">
         <v>204</v>
       </c>
@@ -10976,7 +12075,7 @@
         <v>60496.741402070453</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="B34" s="74" t="s">
         <v>206</v>
       </c>
@@ -10987,7 +12086,7 @@
         <v>47.63</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:6">
       <c r="B35" s="74" t="s">
         <v>208</v>
       </c>
@@ -10998,10 +12097,10 @@
         <v>9.14</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6">
       <c r="D36" s="81"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:6">
       <c r="A37" s="73" t="s">
         <v>220</v>
       </c>
@@ -11011,7 +12110,7 @@
       <c r="C37" s="83"/>
       <c r="D37" s="81"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:6">
       <c r="B38" s="74" t="s">
         <v>200</v>
       </c>
@@ -11022,7 +12121,7 @@
         <v>84093</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:6">
       <c r="B39" s="74" t="s">
         <v>202</v>
       </c>
@@ -11033,7 +12132,7 @@
         <v>73.38</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:6">
       <c r="B40" s="74" t="s">
         <v>204</v>
       </c>
@@ -11043,12 +12142,16 @@
       <c r="D40" s="68">
         <v>3954653723</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="F40" s="65">
+        <f>D40/D38</f>
+        <v>47027.145220172904</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="B41" s="74"/>
       <c r="D41" s="81"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:6">
       <c r="A42" s="73" t="s">
         <v>223</v>
       </c>
@@ -11057,7 +12160,7 @@
       </c>
       <c r="D42" s="81"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:6">
       <c r="B43" s="74" t="s">
         <v>200</v>
       </c>
@@ -11068,136 +12171,143 @@
         <v>224088</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:6">
       <c r="C44" s="84"/>
       <c r="D44" s="85"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75">
-      <c r="A45" s="72" t="s">
+    <row r="45" spans="1:6" ht="15.75">
+      <c r="A45" s="126" t="s">
         <v>225</v>
       </c>
-      <c r="B45" s="72"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="85"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="D46" s="85"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="73" t="s">
+      <c r="B45" s="126"/>
+      <c r="C45" s="126"/>
+      <c r="D45" s="127"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="128"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="128"/>
+      <c r="D46" s="127"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="129" t="s">
         <v>198</v>
       </c>
-      <c r="B47" s="65" t="s">
+      <c r="B47" s="128" t="s">
         <v>162</v>
       </c>
-      <c r="D47" s="85"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="74"/>
-      <c r="B48" s="74" t="s">
+      <c r="C47" s="128"/>
+      <c r="D47" s="127"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="130"/>
+      <c r="B48" s="130" t="s">
         <v>200</v>
       </c>
-      <c r="C48" s="65" t="s">
+      <c r="C48" s="128" t="s">
         <v>199</v>
       </c>
-      <c r="D48" s="79">
+      <c r="D48" s="131">
         <v>39535995292</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="74"/>
-      <c r="B49" s="74" t="s">
+      <c r="A49" s="130"/>
+      <c r="B49" s="130" t="s">
         <v>202</v>
       </c>
-      <c r="C49" s="65" t="s">
+      <c r="C49" s="128" t="s">
         <v>217</v>
       </c>
-      <c r="D49" s="79">
+      <c r="D49" s="131">
         <v>535870232</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="74"/>
-      <c r="B50" s="74" t="s">
+      <c r="A50" s="130"/>
+      <c r="B50" s="130" t="s">
         <v>204</v>
       </c>
-      <c r="C50" s="65" t="s">
+      <c r="C50" s="128" t="s">
         <v>219</v>
       </c>
-      <c r="D50" s="75">
+      <c r="D50" s="132">
         <v>972023664</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="74"/>
-      <c r="B51" s="74" t="s">
+      <c r="A51" s="130"/>
+      <c r="B51" s="130" t="s">
         <v>206</v>
       </c>
-      <c r="C51" s="65" t="s">
+      <c r="C51" s="128" t="s">
         <v>221</v>
       </c>
-      <c r="D51" s="75">
+      <c r="D51" s="132">
         <v>41614466631</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74" t="s">
+      <c r="A52" s="130"/>
+      <c r="B52" s="130" t="s">
         <v>226</v>
       </c>
-      <c r="C52" s="65" t="s">
+      <c r="C52" s="128" t="s">
         <v>227</v>
       </c>
-      <c r="D52" s="75">
+      <c r="D52" s="132">
         <v>37057619</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="74"/>
-      <c r="B53" s="74" t="s">
+      <c r="A53" s="130"/>
+      <c r="B53" s="130" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="65" t="s">
+      <c r="C53" s="128" t="s">
         <v>228</v>
       </c>
-      <c r="D53" s="75">
+      <c r="D53" s="132">
         <v>3066827192</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="74"/>
-      <c r="B54" s="74" t="s">
+      <c r="A54" s="130"/>
+      <c r="B54" s="130" t="s">
         <v>210</v>
       </c>
-      <c r="C54" s="65" t="s">
+      <c r="C54" s="128" t="s">
         <v>224</v>
       </c>
-      <c r="D54" s="75">
+      <c r="D54" s="132">
         <v>85762240630</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="74"/>
-      <c r="B55" s="74"/>
-      <c r="C55" s="86"/>
-      <c r="D55" s="75"/>
+      <c r="A55" s="130"/>
+      <c r="B55" s="130"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="132"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="73">
+      <c r="A56" s="129">
         <v>2</v>
       </c>
-      <c r="B56" s="65" t="s">
+      <c r="B56" s="128" t="s">
         <v>229</v>
       </c>
+      <c r="C56" s="128"/>
+      <c r="D56" s="128"/>
     </row>
     <row r="57" spans="1:4">
-      <c r="B57" s="74" t="s">
+      <c r="A57" s="128"/>
+      <c r="B57" s="130" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="65" t="s">
+      <c r="C57" s="128" t="s">
         <v>199</v>
       </c>
-      <c r="D57" s="34">
+      <c r="D57" s="134">
         <v>23738166660</v>
       </c>
     </row>
@@ -11721,93 +12831,1868 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12C2C70-1D38-4C9C-8A29-A9ED22FEC02C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E4CC7C-9A87-438B-90E6-BB7D13EC56BB}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="1.85546875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="35" customWidth="1"/>
+    <col min="4" max="4" width="3" style="35" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="35" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="35"/>
+    <col min="10" max="10" width="15.42578125" style="35" customWidth="1"/>
+    <col min="11" max="252" width="9.140625" style="35"/>
+    <col min="253" max="253" width="1.85546875" style="35" customWidth="1"/>
+    <col min="254" max="254" width="33.28515625" style="35" customWidth="1"/>
+    <col min="255" max="256" width="20.7109375" style="35" customWidth="1"/>
+    <col min="257" max="257" width="9" style="35" customWidth="1"/>
+    <col min="258" max="258" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="261" max="508" width="9.140625" style="35"/>
+    <col min="509" max="509" width="1.85546875" style="35" customWidth="1"/>
+    <col min="510" max="510" width="33.28515625" style="35" customWidth="1"/>
+    <col min="511" max="512" width="20.7109375" style="35" customWidth="1"/>
+    <col min="513" max="513" width="9" style="35" customWidth="1"/>
+    <col min="514" max="514" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="517" max="764" width="9.140625" style="35"/>
+    <col min="765" max="765" width="1.85546875" style="35" customWidth="1"/>
+    <col min="766" max="766" width="33.28515625" style="35" customWidth="1"/>
+    <col min="767" max="768" width="20.7109375" style="35" customWidth="1"/>
+    <col min="769" max="769" width="9" style="35" customWidth="1"/>
+    <col min="770" max="770" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="772" max="772" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="773" max="1020" width="9.140625" style="35"/>
+    <col min="1021" max="1021" width="1.85546875" style="35" customWidth="1"/>
+    <col min="1022" max="1022" width="33.28515625" style="35" customWidth="1"/>
+    <col min="1023" max="1024" width="20.7109375" style="35" customWidth="1"/>
+    <col min="1025" max="1025" width="9" style="35" customWidth="1"/>
+    <col min="1026" max="1026" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="1029" max="1276" width="9.140625" style="35"/>
+    <col min="1277" max="1277" width="1.85546875" style="35" customWidth="1"/>
+    <col min="1278" max="1278" width="33.28515625" style="35" customWidth="1"/>
+    <col min="1279" max="1280" width="20.7109375" style="35" customWidth="1"/>
+    <col min="1281" max="1281" width="9" style="35" customWidth="1"/>
+    <col min="1282" max="1282" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1284" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="1285" max="1532" width="9.140625" style="35"/>
+    <col min="1533" max="1533" width="1.85546875" style="35" customWidth="1"/>
+    <col min="1534" max="1534" width="33.28515625" style="35" customWidth="1"/>
+    <col min="1535" max="1536" width="20.7109375" style="35" customWidth="1"/>
+    <col min="1537" max="1537" width="9" style="35" customWidth="1"/>
+    <col min="1538" max="1538" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1540" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="1541" max="1788" width="9.140625" style="35"/>
+    <col min="1789" max="1789" width="1.85546875" style="35" customWidth="1"/>
+    <col min="1790" max="1790" width="33.28515625" style="35" customWidth="1"/>
+    <col min="1791" max="1792" width="20.7109375" style="35" customWidth="1"/>
+    <col min="1793" max="1793" width="9" style="35" customWidth="1"/>
+    <col min="1794" max="1794" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1796" max="1796" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="1797" max="2044" width="9.140625" style="35"/>
+    <col min="2045" max="2045" width="1.85546875" style="35" customWidth="1"/>
+    <col min="2046" max="2046" width="33.28515625" style="35" customWidth="1"/>
+    <col min="2047" max="2048" width="20.7109375" style="35" customWidth="1"/>
+    <col min="2049" max="2049" width="9" style="35" customWidth="1"/>
+    <col min="2050" max="2050" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2052" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="2053" max="2300" width="9.140625" style="35"/>
+    <col min="2301" max="2301" width="1.85546875" style="35" customWidth="1"/>
+    <col min="2302" max="2302" width="33.28515625" style="35" customWidth="1"/>
+    <col min="2303" max="2304" width="20.7109375" style="35" customWidth="1"/>
+    <col min="2305" max="2305" width="9" style="35" customWidth="1"/>
+    <col min="2306" max="2306" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2308" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="2309" max="2556" width="9.140625" style="35"/>
+    <col min="2557" max="2557" width="1.85546875" style="35" customWidth="1"/>
+    <col min="2558" max="2558" width="33.28515625" style="35" customWidth="1"/>
+    <col min="2559" max="2560" width="20.7109375" style="35" customWidth="1"/>
+    <col min="2561" max="2561" width="9" style="35" customWidth="1"/>
+    <col min="2562" max="2562" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2564" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="2565" max="2812" width="9.140625" style="35"/>
+    <col min="2813" max="2813" width="1.85546875" style="35" customWidth="1"/>
+    <col min="2814" max="2814" width="33.28515625" style="35" customWidth="1"/>
+    <col min="2815" max="2816" width="20.7109375" style="35" customWidth="1"/>
+    <col min="2817" max="2817" width="9" style="35" customWidth="1"/>
+    <col min="2818" max="2818" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2820" max="2820" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="2821" max="3068" width="9.140625" style="35"/>
+    <col min="3069" max="3069" width="1.85546875" style="35" customWidth="1"/>
+    <col min="3070" max="3070" width="33.28515625" style="35" customWidth="1"/>
+    <col min="3071" max="3072" width="20.7109375" style="35" customWidth="1"/>
+    <col min="3073" max="3073" width="9" style="35" customWidth="1"/>
+    <col min="3074" max="3074" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3076" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="3077" max="3324" width="9.140625" style="35"/>
+    <col min="3325" max="3325" width="1.85546875" style="35" customWidth="1"/>
+    <col min="3326" max="3326" width="33.28515625" style="35" customWidth="1"/>
+    <col min="3327" max="3328" width="20.7109375" style="35" customWidth="1"/>
+    <col min="3329" max="3329" width="9" style="35" customWidth="1"/>
+    <col min="3330" max="3330" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3332" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="3333" max="3580" width="9.140625" style="35"/>
+    <col min="3581" max="3581" width="1.85546875" style="35" customWidth="1"/>
+    <col min="3582" max="3582" width="33.28515625" style="35" customWidth="1"/>
+    <col min="3583" max="3584" width="20.7109375" style="35" customWidth="1"/>
+    <col min="3585" max="3585" width="9" style="35" customWidth="1"/>
+    <col min="3586" max="3586" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3588" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="3589" max="3836" width="9.140625" style="35"/>
+    <col min="3837" max="3837" width="1.85546875" style="35" customWidth="1"/>
+    <col min="3838" max="3838" width="33.28515625" style="35" customWidth="1"/>
+    <col min="3839" max="3840" width="20.7109375" style="35" customWidth="1"/>
+    <col min="3841" max="3841" width="9" style="35" customWidth="1"/>
+    <col min="3842" max="3842" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3844" max="3844" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="3845" max="4092" width="9.140625" style="35"/>
+    <col min="4093" max="4093" width="1.85546875" style="35" customWidth="1"/>
+    <col min="4094" max="4094" width="33.28515625" style="35" customWidth="1"/>
+    <col min="4095" max="4096" width="20.7109375" style="35" customWidth="1"/>
+    <col min="4097" max="4097" width="9" style="35" customWidth="1"/>
+    <col min="4098" max="4098" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4100" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4101" max="4348" width="9.140625" style="35"/>
+    <col min="4349" max="4349" width="1.85546875" style="35" customWidth="1"/>
+    <col min="4350" max="4350" width="33.28515625" style="35" customWidth="1"/>
+    <col min="4351" max="4352" width="20.7109375" style="35" customWidth="1"/>
+    <col min="4353" max="4353" width="9" style="35" customWidth="1"/>
+    <col min="4354" max="4354" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4356" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4357" max="4604" width="9.140625" style="35"/>
+    <col min="4605" max="4605" width="1.85546875" style="35" customWidth="1"/>
+    <col min="4606" max="4606" width="33.28515625" style="35" customWidth="1"/>
+    <col min="4607" max="4608" width="20.7109375" style="35" customWidth="1"/>
+    <col min="4609" max="4609" width="9" style="35" customWidth="1"/>
+    <col min="4610" max="4610" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4612" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4613" max="4860" width="9.140625" style="35"/>
+    <col min="4861" max="4861" width="1.85546875" style="35" customWidth="1"/>
+    <col min="4862" max="4862" width="33.28515625" style="35" customWidth="1"/>
+    <col min="4863" max="4864" width="20.7109375" style="35" customWidth="1"/>
+    <col min="4865" max="4865" width="9" style="35" customWidth="1"/>
+    <col min="4866" max="4866" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4868" max="4868" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4869" max="5116" width="9.140625" style="35"/>
+    <col min="5117" max="5117" width="1.85546875" style="35" customWidth="1"/>
+    <col min="5118" max="5118" width="33.28515625" style="35" customWidth="1"/>
+    <col min="5119" max="5120" width="20.7109375" style="35" customWidth="1"/>
+    <col min="5121" max="5121" width="9" style="35" customWidth="1"/>
+    <col min="5122" max="5122" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5124" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="5125" max="5372" width="9.140625" style="35"/>
+    <col min="5373" max="5373" width="1.85546875" style="35" customWidth="1"/>
+    <col min="5374" max="5374" width="33.28515625" style="35" customWidth="1"/>
+    <col min="5375" max="5376" width="20.7109375" style="35" customWidth="1"/>
+    <col min="5377" max="5377" width="9" style="35" customWidth="1"/>
+    <col min="5378" max="5378" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5380" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="5381" max="5628" width="9.140625" style="35"/>
+    <col min="5629" max="5629" width="1.85546875" style="35" customWidth="1"/>
+    <col min="5630" max="5630" width="33.28515625" style="35" customWidth="1"/>
+    <col min="5631" max="5632" width="20.7109375" style="35" customWidth="1"/>
+    <col min="5633" max="5633" width="9" style="35" customWidth="1"/>
+    <col min="5634" max="5634" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5636" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="5637" max="5884" width="9.140625" style="35"/>
+    <col min="5885" max="5885" width="1.85546875" style="35" customWidth="1"/>
+    <col min="5886" max="5886" width="33.28515625" style="35" customWidth="1"/>
+    <col min="5887" max="5888" width="20.7109375" style="35" customWidth="1"/>
+    <col min="5889" max="5889" width="9" style="35" customWidth="1"/>
+    <col min="5890" max="5890" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5892" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="5893" max="6140" width="9.140625" style="35"/>
+    <col min="6141" max="6141" width="1.85546875" style="35" customWidth="1"/>
+    <col min="6142" max="6142" width="33.28515625" style="35" customWidth="1"/>
+    <col min="6143" max="6144" width="20.7109375" style="35" customWidth="1"/>
+    <col min="6145" max="6145" width="9" style="35" customWidth="1"/>
+    <col min="6146" max="6146" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6148" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="6149" max="6396" width="9.140625" style="35"/>
+    <col min="6397" max="6397" width="1.85546875" style="35" customWidth="1"/>
+    <col min="6398" max="6398" width="33.28515625" style="35" customWidth="1"/>
+    <col min="6399" max="6400" width="20.7109375" style="35" customWidth="1"/>
+    <col min="6401" max="6401" width="9" style="35" customWidth="1"/>
+    <col min="6402" max="6402" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6404" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="6405" max="6652" width="9.140625" style="35"/>
+    <col min="6653" max="6653" width="1.85546875" style="35" customWidth="1"/>
+    <col min="6654" max="6654" width="33.28515625" style="35" customWidth="1"/>
+    <col min="6655" max="6656" width="20.7109375" style="35" customWidth="1"/>
+    <col min="6657" max="6657" width="9" style="35" customWidth="1"/>
+    <col min="6658" max="6658" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6660" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="6661" max="6908" width="9.140625" style="35"/>
+    <col min="6909" max="6909" width="1.85546875" style="35" customWidth="1"/>
+    <col min="6910" max="6910" width="33.28515625" style="35" customWidth="1"/>
+    <col min="6911" max="6912" width="20.7109375" style="35" customWidth="1"/>
+    <col min="6913" max="6913" width="9" style="35" customWidth="1"/>
+    <col min="6914" max="6914" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6916" max="6916" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="6917" max="7164" width="9.140625" style="35"/>
+    <col min="7165" max="7165" width="1.85546875" style="35" customWidth="1"/>
+    <col min="7166" max="7166" width="33.28515625" style="35" customWidth="1"/>
+    <col min="7167" max="7168" width="20.7109375" style="35" customWidth="1"/>
+    <col min="7169" max="7169" width="9" style="35" customWidth="1"/>
+    <col min="7170" max="7170" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7172" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="7173" max="7420" width="9.140625" style="35"/>
+    <col min="7421" max="7421" width="1.85546875" style="35" customWidth="1"/>
+    <col min="7422" max="7422" width="33.28515625" style="35" customWidth="1"/>
+    <col min="7423" max="7424" width="20.7109375" style="35" customWidth="1"/>
+    <col min="7425" max="7425" width="9" style="35" customWidth="1"/>
+    <col min="7426" max="7426" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7428" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="7429" max="7676" width="9.140625" style="35"/>
+    <col min="7677" max="7677" width="1.85546875" style="35" customWidth="1"/>
+    <col min="7678" max="7678" width="33.28515625" style="35" customWidth="1"/>
+    <col min="7679" max="7680" width="20.7109375" style="35" customWidth="1"/>
+    <col min="7681" max="7681" width="9" style="35" customWidth="1"/>
+    <col min="7682" max="7682" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7684" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="7685" max="7932" width="9.140625" style="35"/>
+    <col min="7933" max="7933" width="1.85546875" style="35" customWidth="1"/>
+    <col min="7934" max="7934" width="33.28515625" style="35" customWidth="1"/>
+    <col min="7935" max="7936" width="20.7109375" style="35" customWidth="1"/>
+    <col min="7937" max="7937" width="9" style="35" customWidth="1"/>
+    <col min="7938" max="7938" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7940" max="7940" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="7941" max="8188" width="9.140625" style="35"/>
+    <col min="8189" max="8189" width="1.85546875" style="35" customWidth="1"/>
+    <col min="8190" max="8190" width="33.28515625" style="35" customWidth="1"/>
+    <col min="8191" max="8192" width="20.7109375" style="35" customWidth="1"/>
+    <col min="8193" max="8193" width="9" style="35" customWidth="1"/>
+    <col min="8194" max="8194" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8196" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8197" max="8444" width="9.140625" style="35"/>
+    <col min="8445" max="8445" width="1.85546875" style="35" customWidth="1"/>
+    <col min="8446" max="8446" width="33.28515625" style="35" customWidth="1"/>
+    <col min="8447" max="8448" width="20.7109375" style="35" customWidth="1"/>
+    <col min="8449" max="8449" width="9" style="35" customWidth="1"/>
+    <col min="8450" max="8450" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8452" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8453" max="8700" width="9.140625" style="35"/>
+    <col min="8701" max="8701" width="1.85546875" style="35" customWidth="1"/>
+    <col min="8702" max="8702" width="33.28515625" style="35" customWidth="1"/>
+    <col min="8703" max="8704" width="20.7109375" style="35" customWidth="1"/>
+    <col min="8705" max="8705" width="9" style="35" customWidth="1"/>
+    <col min="8706" max="8706" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8708" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8709" max="8956" width="9.140625" style="35"/>
+    <col min="8957" max="8957" width="1.85546875" style="35" customWidth="1"/>
+    <col min="8958" max="8958" width="33.28515625" style="35" customWidth="1"/>
+    <col min="8959" max="8960" width="20.7109375" style="35" customWidth="1"/>
+    <col min="8961" max="8961" width="9" style="35" customWidth="1"/>
+    <col min="8962" max="8962" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8964" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8965" max="9212" width="9.140625" style="35"/>
+    <col min="9213" max="9213" width="1.85546875" style="35" customWidth="1"/>
+    <col min="9214" max="9214" width="33.28515625" style="35" customWidth="1"/>
+    <col min="9215" max="9216" width="20.7109375" style="35" customWidth="1"/>
+    <col min="9217" max="9217" width="9" style="35" customWidth="1"/>
+    <col min="9218" max="9218" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9220" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9221" max="9468" width="9.140625" style="35"/>
+    <col min="9469" max="9469" width="1.85546875" style="35" customWidth="1"/>
+    <col min="9470" max="9470" width="33.28515625" style="35" customWidth="1"/>
+    <col min="9471" max="9472" width="20.7109375" style="35" customWidth="1"/>
+    <col min="9473" max="9473" width="9" style="35" customWidth="1"/>
+    <col min="9474" max="9474" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9476" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9477" max="9724" width="9.140625" style="35"/>
+    <col min="9725" max="9725" width="1.85546875" style="35" customWidth="1"/>
+    <col min="9726" max="9726" width="33.28515625" style="35" customWidth="1"/>
+    <col min="9727" max="9728" width="20.7109375" style="35" customWidth="1"/>
+    <col min="9729" max="9729" width="9" style="35" customWidth="1"/>
+    <col min="9730" max="9730" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9732" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9733" max="9980" width="9.140625" style="35"/>
+    <col min="9981" max="9981" width="1.85546875" style="35" customWidth="1"/>
+    <col min="9982" max="9982" width="33.28515625" style="35" customWidth="1"/>
+    <col min="9983" max="9984" width="20.7109375" style="35" customWidth="1"/>
+    <col min="9985" max="9985" width="9" style="35" customWidth="1"/>
+    <col min="9986" max="9986" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9988" max="9988" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="9989" max="10236" width="9.140625" style="35"/>
+    <col min="10237" max="10237" width="1.85546875" style="35" customWidth="1"/>
+    <col min="10238" max="10238" width="33.28515625" style="35" customWidth="1"/>
+    <col min="10239" max="10240" width="20.7109375" style="35" customWidth="1"/>
+    <col min="10241" max="10241" width="9" style="35" customWidth="1"/>
+    <col min="10242" max="10242" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10244" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10245" max="10492" width="9.140625" style="35"/>
+    <col min="10493" max="10493" width="1.85546875" style="35" customWidth="1"/>
+    <col min="10494" max="10494" width="33.28515625" style="35" customWidth="1"/>
+    <col min="10495" max="10496" width="20.7109375" style="35" customWidth="1"/>
+    <col min="10497" max="10497" width="9" style="35" customWidth="1"/>
+    <col min="10498" max="10498" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10500" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10501" max="10748" width="9.140625" style="35"/>
+    <col min="10749" max="10749" width="1.85546875" style="35" customWidth="1"/>
+    <col min="10750" max="10750" width="33.28515625" style="35" customWidth="1"/>
+    <col min="10751" max="10752" width="20.7109375" style="35" customWidth="1"/>
+    <col min="10753" max="10753" width="9" style="35" customWidth="1"/>
+    <col min="10754" max="10754" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="10756" max="10756" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10757" max="11004" width="9.140625" style="35"/>
+    <col min="11005" max="11005" width="1.85546875" style="35" customWidth="1"/>
+    <col min="11006" max="11006" width="33.28515625" style="35" customWidth="1"/>
+    <col min="11007" max="11008" width="20.7109375" style="35" customWidth="1"/>
+    <col min="11009" max="11009" width="9" style="35" customWidth="1"/>
+    <col min="11010" max="11010" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11012" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="11013" max="11260" width="9.140625" style="35"/>
+    <col min="11261" max="11261" width="1.85546875" style="35" customWidth="1"/>
+    <col min="11262" max="11262" width="33.28515625" style="35" customWidth="1"/>
+    <col min="11263" max="11264" width="20.7109375" style="35" customWidth="1"/>
+    <col min="11265" max="11265" width="9" style="35" customWidth="1"/>
+    <col min="11266" max="11266" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11268" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="11269" max="11516" width="9.140625" style="35"/>
+    <col min="11517" max="11517" width="1.85546875" style="35" customWidth="1"/>
+    <col min="11518" max="11518" width="33.28515625" style="35" customWidth="1"/>
+    <col min="11519" max="11520" width="20.7109375" style="35" customWidth="1"/>
+    <col min="11521" max="11521" width="9" style="35" customWidth="1"/>
+    <col min="11522" max="11522" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11524" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="11525" max="11772" width="9.140625" style="35"/>
+    <col min="11773" max="11773" width="1.85546875" style="35" customWidth="1"/>
+    <col min="11774" max="11774" width="33.28515625" style="35" customWidth="1"/>
+    <col min="11775" max="11776" width="20.7109375" style="35" customWidth="1"/>
+    <col min="11777" max="11777" width="9" style="35" customWidth="1"/>
+    <col min="11778" max="11778" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11780" max="11780" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="11781" max="12028" width="9.140625" style="35"/>
+    <col min="12029" max="12029" width="1.85546875" style="35" customWidth="1"/>
+    <col min="12030" max="12030" width="33.28515625" style="35" customWidth="1"/>
+    <col min="12031" max="12032" width="20.7109375" style="35" customWidth="1"/>
+    <col min="12033" max="12033" width="9" style="35" customWidth="1"/>
+    <col min="12034" max="12034" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12036" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="12037" max="12284" width="9.140625" style="35"/>
+    <col min="12285" max="12285" width="1.85546875" style="35" customWidth="1"/>
+    <col min="12286" max="12286" width="33.28515625" style="35" customWidth="1"/>
+    <col min="12287" max="12288" width="20.7109375" style="35" customWidth="1"/>
+    <col min="12289" max="12289" width="9" style="35" customWidth="1"/>
+    <col min="12290" max="12290" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12292" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="12293" max="12540" width="9.140625" style="35"/>
+    <col min="12541" max="12541" width="1.85546875" style="35" customWidth="1"/>
+    <col min="12542" max="12542" width="33.28515625" style="35" customWidth="1"/>
+    <col min="12543" max="12544" width="20.7109375" style="35" customWidth="1"/>
+    <col min="12545" max="12545" width="9" style="35" customWidth="1"/>
+    <col min="12546" max="12546" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12548" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="12549" max="12796" width="9.140625" style="35"/>
+    <col min="12797" max="12797" width="1.85546875" style="35" customWidth="1"/>
+    <col min="12798" max="12798" width="33.28515625" style="35" customWidth="1"/>
+    <col min="12799" max="12800" width="20.7109375" style="35" customWidth="1"/>
+    <col min="12801" max="12801" width="9" style="35" customWidth="1"/>
+    <col min="12802" max="12802" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="12804" max="12804" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="12805" max="13052" width="9.140625" style="35"/>
+    <col min="13053" max="13053" width="1.85546875" style="35" customWidth="1"/>
+    <col min="13054" max="13054" width="33.28515625" style="35" customWidth="1"/>
+    <col min="13055" max="13056" width="20.7109375" style="35" customWidth="1"/>
+    <col min="13057" max="13057" width="9" style="35" customWidth="1"/>
+    <col min="13058" max="13058" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13060" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="13061" max="13308" width="9.140625" style="35"/>
+    <col min="13309" max="13309" width="1.85546875" style="35" customWidth="1"/>
+    <col min="13310" max="13310" width="33.28515625" style="35" customWidth="1"/>
+    <col min="13311" max="13312" width="20.7109375" style="35" customWidth="1"/>
+    <col min="13313" max="13313" width="9" style="35" customWidth="1"/>
+    <col min="13314" max="13314" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13316" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13564" width="9.140625" style="35"/>
+    <col min="13565" max="13565" width="1.85546875" style="35" customWidth="1"/>
+    <col min="13566" max="13566" width="33.28515625" style="35" customWidth="1"/>
+    <col min="13567" max="13568" width="20.7109375" style="35" customWidth="1"/>
+    <col min="13569" max="13569" width="9" style="35" customWidth="1"/>
+    <col min="13570" max="13570" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13572" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="13573" max="13820" width="9.140625" style="35"/>
+    <col min="13821" max="13821" width="1.85546875" style="35" customWidth="1"/>
+    <col min="13822" max="13822" width="33.28515625" style="35" customWidth="1"/>
+    <col min="13823" max="13824" width="20.7109375" style="35" customWidth="1"/>
+    <col min="13825" max="13825" width="9" style="35" customWidth="1"/>
+    <col min="13826" max="13826" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13828" max="13828" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="13829" max="14076" width="9.140625" style="35"/>
+    <col min="14077" max="14077" width="1.85546875" style="35" customWidth="1"/>
+    <col min="14078" max="14078" width="33.28515625" style="35" customWidth="1"/>
+    <col min="14079" max="14080" width="20.7109375" style="35" customWidth="1"/>
+    <col min="14081" max="14081" width="9" style="35" customWidth="1"/>
+    <col min="14082" max="14082" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14084" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="14085" max="14332" width="9.140625" style="35"/>
+    <col min="14333" max="14333" width="1.85546875" style="35" customWidth="1"/>
+    <col min="14334" max="14334" width="33.28515625" style="35" customWidth="1"/>
+    <col min="14335" max="14336" width="20.7109375" style="35" customWidth="1"/>
+    <col min="14337" max="14337" width="9" style="35" customWidth="1"/>
+    <col min="14338" max="14338" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14340" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="14341" max="14588" width="9.140625" style="35"/>
+    <col min="14589" max="14589" width="1.85546875" style="35" customWidth="1"/>
+    <col min="14590" max="14590" width="33.28515625" style="35" customWidth="1"/>
+    <col min="14591" max="14592" width="20.7109375" style="35" customWidth="1"/>
+    <col min="14593" max="14593" width="9" style="35" customWidth="1"/>
+    <col min="14594" max="14594" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14596" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="14597" max="14844" width="9.140625" style="35"/>
+    <col min="14845" max="14845" width="1.85546875" style="35" customWidth="1"/>
+    <col min="14846" max="14846" width="33.28515625" style="35" customWidth="1"/>
+    <col min="14847" max="14848" width="20.7109375" style="35" customWidth="1"/>
+    <col min="14849" max="14849" width="9" style="35" customWidth="1"/>
+    <col min="14850" max="14850" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14852" max="14852" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="14853" max="15100" width="9.140625" style="35"/>
+    <col min="15101" max="15101" width="1.85546875" style="35" customWidth="1"/>
+    <col min="15102" max="15102" width="33.28515625" style="35" customWidth="1"/>
+    <col min="15103" max="15104" width="20.7109375" style="35" customWidth="1"/>
+    <col min="15105" max="15105" width="9" style="35" customWidth="1"/>
+    <col min="15106" max="15106" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15108" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="15109" max="15356" width="9.140625" style="35"/>
+    <col min="15357" max="15357" width="1.85546875" style="35" customWidth="1"/>
+    <col min="15358" max="15358" width="33.28515625" style="35" customWidth="1"/>
+    <col min="15359" max="15360" width="20.7109375" style="35" customWidth="1"/>
+    <col min="15361" max="15361" width="9" style="35" customWidth="1"/>
+    <col min="15362" max="15362" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15364" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="15365" max="15612" width="9.140625" style="35"/>
+    <col min="15613" max="15613" width="1.85546875" style="35" customWidth="1"/>
+    <col min="15614" max="15614" width="33.28515625" style="35" customWidth="1"/>
+    <col min="15615" max="15616" width="20.7109375" style="35" customWidth="1"/>
+    <col min="15617" max="15617" width="9" style="35" customWidth="1"/>
+    <col min="15618" max="15618" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15620" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="15621" max="15868" width="9.140625" style="35"/>
+    <col min="15869" max="15869" width="1.85546875" style="35" customWidth="1"/>
+    <col min="15870" max="15870" width="33.28515625" style="35" customWidth="1"/>
+    <col min="15871" max="15872" width="20.7109375" style="35" customWidth="1"/>
+    <col min="15873" max="15873" width="9" style="35" customWidth="1"/>
+    <col min="15874" max="15874" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15876" max="15876" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="15877" max="16124" width="9.140625" style="35"/>
+    <col min="16125" max="16125" width="1.85546875" style="35" customWidth="1"/>
+    <col min="16126" max="16126" width="33.28515625" style="35" customWidth="1"/>
+    <col min="16127" max="16128" width="20.7109375" style="35" customWidth="1"/>
+    <col min="16129" max="16129" width="9" style="35" customWidth="1"/>
+    <col min="16130" max="16130" width="16" style="35" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="15.5703125" style="35" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16132" width="16.7109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16384" width="9.140625" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="14.25">
+      <c r="B1" s="170" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="170"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="150" t="s">
+        <v>284</v>
+      </c>
+      <c r="G1" s="149"/>
+    </row>
+    <row r="2" spans="2:10" ht="15.75">
+      <c r="B2" s="171" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="171"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="152"/>
+    </row>
+    <row r="3" spans="2:10" ht="15">
+      <c r="B3" s="135"/>
+      <c r="C3" s="136">
+        <v>42551</v>
+      </c>
+      <c r="E3" s="153"/>
+      <c r="F3" s="153"/>
+      <c r="G3" s="152"/>
+    </row>
+    <row r="4" spans="2:10" ht="15">
+      <c r="B4" s="137" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="135"/>
+      <c r="E4" s="153" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="153"/>
+      <c r="G4" s="152"/>
+    </row>
+    <row r="5" spans="2:10" ht="15">
+      <c r="B5" s="138" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="139">
+        <v>37667162029</v>
+      </c>
+      <c r="E5" s="154" t="s">
+        <v>200</v>
+      </c>
+      <c r="F5" s="153" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="155">
+        <v>39535995292</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15">
+      <c r="B6" s="138" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="140">
+        <v>828167983</v>
+      </c>
+      <c r="E6" s="154" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" s="153" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="155">
+        <v>535870232</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15">
+      <c r="B7" s="138" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="140">
+        <v>233891569</v>
+      </c>
+      <c r="E7" s="154" t="s">
+        <v>204</v>
+      </c>
+      <c r="F7" s="153" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" s="156">
+        <v>972023664</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15">
+      <c r="B8" s="138" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="140">
+        <v>405896494</v>
+      </c>
+      <c r="E8" s="154" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" s="153" t="s">
+        <v>221</v>
+      </c>
+      <c r="G8" s="156">
+        <v>41614466631</v>
+      </c>
+      <c r="J8" s="140">
+        <v>125975786</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15">
+      <c r="B9" s="138" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="140">
+        <v>0</v>
+      </c>
+      <c r="E9" s="154" t="s">
+        <v>226</v>
+      </c>
+      <c r="F9" s="153" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="156">
+        <v>37057619</v>
+      </c>
+      <c r="J9" s="140">
+        <v>2190015114</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.75">
+      <c r="B10" s="138" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="140">
+        <v>125975786</v>
+      </c>
+      <c r="D10" s="43"/>
+      <c r="E10" s="154" t="s">
+        <v>208</v>
+      </c>
+      <c r="F10" s="153" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="156">
+        <v>3066827192</v>
+      </c>
+      <c r="J10" s="156">
+        <v>972023664</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15">
+      <c r="B11" s="138" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="140">
+        <v>2190015114</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="154" t="s">
+        <v>210</v>
+      </c>
+      <c r="F11" s="153" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" s="156">
+        <v>85762240630</v>
+      </c>
+      <c r="J11" s="159">
+        <f>J8+J9-J10</f>
+        <v>1343967236</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75">
+      <c r="B12" s="138" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="140">
+        <v>2659607405</v>
+      </c>
+      <c r="D12" s="43"/>
+      <c r="E12" s="154"/>
+      <c r="F12" s="157"/>
+      <c r="G12" s="156"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75">
+      <c r="B13" s="138"/>
+      <c r="C13" s="135"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="153" t="s">
+        <v>229</v>
+      </c>
+      <c r="F13" s="153"/>
+      <c r="G13" s="153"/>
+    </row>
+    <row r="14" spans="2:10" ht="15">
+      <c r="B14" s="141" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="142">
+        <v>44110716380</v>
+      </c>
+      <c r="E14" s="154" t="s">
+        <v>200</v>
+      </c>
+      <c r="F14" s="153" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" s="158">
+        <v>23738166660</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="141"/>
+      <c r="C15" s="142"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="141"/>
+      <c r="C16" s="142"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.25">
+      <c r="B17" s="137" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="135"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" s="138" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="139">
+        <v>36908685919</v>
+      </c>
+      <c r="D18" s="124"/>
+      <c r="E18" s="125"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" s="138" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="140">
+        <v>562967821</v>
+      </c>
+      <c r="D19" s="45"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="138" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="140">
+        <v>1079573596</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="138" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="140">
+        <v>286721503</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="138" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="138" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="140">
+        <v>2776517792</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15">
+      <c r="B24" s="138" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="140">
+        <v>37057619</v>
+      </c>
+      <c r="D24" s="52"/>
+    </row>
+    <row r="25" spans="1:5" ht="15">
+      <c r="B25" s="138"/>
+      <c r="C25" s="140"/>
+      <c r="D25" s="52"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="138"/>
+      <c r="C26" s="140"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="138"/>
+      <c r="C27" s="140"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="141" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="143">
+        <v>41651524250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="144" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="142">
+        <v>85762240630</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.25">
+      <c r="B30" s="137" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="145">
+        <v>3083988637</v>
+      </c>
+      <c r="D30" s="58"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="135"/>
+      <c r="C31" s="135"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="59">
+        <v>1</v>
+      </c>
+      <c r="B32" s="146" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="147"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="59">
+        <v>2</v>
+      </c>
+      <c r="B33" s="146" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" s="147"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="59">
+        <v>3</v>
+      </c>
+      <c r="B34" s="146" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="147"/>
+    </row>
+    <row r="35" spans="1:3" ht="13.5">
+      <c r="A35" s="62">
+        <v>4</v>
+      </c>
+      <c r="B35" s="146" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="148"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Present Value of Benefits for prior fiscal year to nearest dollar" sqref="IU5:IV5 SQ5:SR5 ACM5:ACN5 AMI5:AMJ5 AWE5:AWF5 BGA5:BGB5 BPW5:BPX5 BZS5:BZT5 CJO5:CJP5 CTK5:CTL5 DDG5:DDH5 DNC5:DND5 DWY5:DWZ5 EGU5:EGV5 EQQ5:EQR5 FAM5:FAN5 FKI5:FKJ5 FUE5:FUF5 GEA5:GEB5 GNW5:GNX5 GXS5:GXT5 HHO5:HHP5 HRK5:HRL5 IBG5:IBH5 ILC5:ILD5 IUY5:IUZ5 JEU5:JEV5 JOQ5:JOR5 JYM5:JYN5 KII5:KIJ5 KSE5:KSF5 LCA5:LCB5 LLW5:LLX5 LVS5:LVT5 MFO5:MFP5 MPK5:MPL5 MZG5:MZH5 NJC5:NJD5 NSY5:NSZ5 OCU5:OCV5 OMQ5:OMR5 OWM5:OWN5 PGI5:PGJ5 PQE5:PQF5 QAA5:QAB5 QJW5:QJX5 QTS5:QTT5 RDO5:RDP5 RNK5:RNL5 RXG5:RXH5 SHC5:SHD5 SQY5:SQZ5 TAU5:TAV5 TKQ5:TKR5 TUM5:TUN5 UEI5:UEJ5 UOE5:UOF5 UYA5:UYB5 VHW5:VHX5 VRS5:VRT5 WBO5:WBP5 WLK5:WLL5 WVG5:WVH5 IU65535:IV65535 SQ65535:SR65535 ACM65535:ACN65535 AMI65535:AMJ65535 AWE65535:AWF65535 BGA65535:BGB65535 BPW65535:BPX65535 BZS65535:BZT65535 CJO65535:CJP65535 CTK65535:CTL65535 DDG65535:DDH65535 DNC65535:DND65535 DWY65535:DWZ65535 EGU65535:EGV65535 EQQ65535:EQR65535 FAM65535:FAN65535 FKI65535:FKJ65535 FUE65535:FUF65535 GEA65535:GEB65535 GNW65535:GNX65535 GXS65535:GXT65535 HHO65535:HHP65535 HRK65535:HRL65535 IBG65535:IBH65535 ILC65535:ILD65535 IUY65535:IUZ65535 JEU65535:JEV65535 JOQ65535:JOR65535 JYM65535:JYN65535 KII65535:KIJ65535 KSE65535:KSF65535 LCA65535:LCB65535 LLW65535:LLX65535 LVS65535:LVT65535 MFO65535:MFP65535 MPK65535:MPL65535 MZG65535:MZH65535 NJC65535:NJD65535 NSY65535:NSZ65535 OCU65535:OCV65535 OMQ65535:OMR65535 OWM65535:OWN65535 PGI65535:PGJ65535 PQE65535:PQF65535 QAA65535:QAB65535 QJW65535:QJX65535 QTS65535:QTT65535 RDO65535:RDP65535 RNK65535:RNL65535 RXG65535:RXH65535 SHC65535:SHD65535 SQY65535:SQZ65535 TAU65535:TAV65535 TKQ65535:TKR65535 TUM65535:TUN65535 UEI65535:UEJ65535 UOE65535:UOF65535 UYA65535:UYB65535 VHW65535:VHX65535 VRS65535:VRT65535 WBO65535:WBP65535 WLK65535:WLL65535 WVG65535:WVH65535 IU131071:IV131071 SQ131071:SR131071 ACM131071:ACN131071 AMI131071:AMJ131071 AWE131071:AWF131071 BGA131071:BGB131071 BPW131071:BPX131071 BZS131071:BZT131071 CJO131071:CJP131071 CTK131071:CTL131071 DDG131071:DDH131071 DNC131071:DND131071 DWY131071:DWZ131071 EGU131071:EGV131071 EQQ131071:EQR131071 FAM131071:FAN131071 FKI131071:FKJ131071 FUE131071:FUF131071 GEA131071:GEB131071 GNW131071:GNX131071 GXS131071:GXT131071 HHO131071:HHP131071 HRK131071:HRL131071 IBG131071:IBH131071 ILC131071:ILD131071 IUY131071:IUZ131071 JEU131071:JEV131071 JOQ131071:JOR131071 JYM131071:JYN131071 KII131071:KIJ131071 KSE131071:KSF131071 LCA131071:LCB131071 LLW131071:LLX131071 LVS131071:LVT131071 MFO131071:MFP131071 MPK131071:MPL131071 MZG131071:MZH131071 NJC131071:NJD131071 NSY131071:NSZ131071 OCU131071:OCV131071 OMQ131071:OMR131071 OWM131071:OWN131071 PGI131071:PGJ131071 PQE131071:PQF131071 QAA131071:QAB131071 QJW131071:QJX131071 QTS131071:QTT131071 RDO131071:RDP131071 RNK131071:RNL131071 RXG131071:RXH131071 SHC131071:SHD131071 SQY131071:SQZ131071 TAU131071:TAV131071 TKQ131071:TKR131071 TUM131071:TUN131071 UEI131071:UEJ131071 UOE131071:UOF131071 UYA131071:UYB131071 VHW131071:VHX131071 VRS131071:VRT131071 WBO131071:WBP131071 WLK131071:WLL131071 WVG131071:WVH131071 IU196607:IV196607 SQ196607:SR196607 ACM196607:ACN196607 AMI196607:AMJ196607 AWE196607:AWF196607 BGA196607:BGB196607 BPW196607:BPX196607 BZS196607:BZT196607 CJO196607:CJP196607 CTK196607:CTL196607 DDG196607:DDH196607 DNC196607:DND196607 DWY196607:DWZ196607 EGU196607:EGV196607 EQQ196607:EQR196607 FAM196607:FAN196607 FKI196607:FKJ196607 FUE196607:FUF196607 GEA196607:GEB196607 GNW196607:GNX196607 GXS196607:GXT196607 HHO196607:HHP196607 HRK196607:HRL196607 IBG196607:IBH196607 ILC196607:ILD196607 IUY196607:IUZ196607 JEU196607:JEV196607 JOQ196607:JOR196607 JYM196607:JYN196607 KII196607:KIJ196607 KSE196607:KSF196607 LCA196607:LCB196607 LLW196607:LLX196607 LVS196607:LVT196607 MFO196607:MFP196607 MPK196607:MPL196607 MZG196607:MZH196607 NJC196607:NJD196607 NSY196607:NSZ196607 OCU196607:OCV196607 OMQ196607:OMR196607 OWM196607:OWN196607 PGI196607:PGJ196607 PQE196607:PQF196607 QAA196607:QAB196607 QJW196607:QJX196607 QTS196607:QTT196607 RDO196607:RDP196607 RNK196607:RNL196607 RXG196607:RXH196607 SHC196607:SHD196607 SQY196607:SQZ196607 TAU196607:TAV196607 TKQ196607:TKR196607 TUM196607:TUN196607 UEI196607:UEJ196607 UOE196607:UOF196607 UYA196607:UYB196607 VHW196607:VHX196607 VRS196607:VRT196607 WBO196607:WBP196607 WLK196607:WLL196607 WVG196607:WVH196607 IU262143:IV262143 SQ262143:SR262143 ACM262143:ACN262143 AMI262143:AMJ262143 AWE262143:AWF262143 BGA262143:BGB262143 BPW262143:BPX262143 BZS262143:BZT262143 CJO262143:CJP262143 CTK262143:CTL262143 DDG262143:DDH262143 DNC262143:DND262143 DWY262143:DWZ262143 EGU262143:EGV262143 EQQ262143:EQR262143 FAM262143:FAN262143 FKI262143:FKJ262143 FUE262143:FUF262143 GEA262143:GEB262143 GNW262143:GNX262143 GXS262143:GXT262143 HHO262143:HHP262143 HRK262143:HRL262143 IBG262143:IBH262143 ILC262143:ILD262143 IUY262143:IUZ262143 JEU262143:JEV262143 JOQ262143:JOR262143 JYM262143:JYN262143 KII262143:KIJ262143 KSE262143:KSF262143 LCA262143:LCB262143 LLW262143:LLX262143 LVS262143:LVT262143 MFO262143:MFP262143 MPK262143:MPL262143 MZG262143:MZH262143 NJC262143:NJD262143 NSY262143:NSZ262143 OCU262143:OCV262143 OMQ262143:OMR262143 OWM262143:OWN262143 PGI262143:PGJ262143 PQE262143:PQF262143 QAA262143:QAB262143 QJW262143:QJX262143 QTS262143:QTT262143 RDO262143:RDP262143 RNK262143:RNL262143 RXG262143:RXH262143 SHC262143:SHD262143 SQY262143:SQZ262143 TAU262143:TAV262143 TKQ262143:TKR262143 TUM262143:TUN262143 UEI262143:UEJ262143 UOE262143:UOF262143 UYA262143:UYB262143 VHW262143:VHX262143 VRS262143:VRT262143 WBO262143:WBP262143 WLK262143:WLL262143 WVG262143:WVH262143 IU327679:IV327679 SQ327679:SR327679 ACM327679:ACN327679 AMI327679:AMJ327679 AWE327679:AWF327679 BGA327679:BGB327679 BPW327679:BPX327679 BZS327679:BZT327679 CJO327679:CJP327679 CTK327679:CTL327679 DDG327679:DDH327679 DNC327679:DND327679 DWY327679:DWZ327679 EGU327679:EGV327679 EQQ327679:EQR327679 FAM327679:FAN327679 FKI327679:FKJ327679 FUE327679:FUF327679 GEA327679:GEB327679 GNW327679:GNX327679 GXS327679:GXT327679 HHO327679:HHP327679 HRK327679:HRL327679 IBG327679:IBH327679 ILC327679:ILD327679 IUY327679:IUZ327679 JEU327679:JEV327679 JOQ327679:JOR327679 JYM327679:JYN327679 KII327679:KIJ327679 KSE327679:KSF327679 LCA327679:LCB327679 LLW327679:LLX327679 LVS327679:LVT327679 MFO327679:MFP327679 MPK327679:MPL327679 MZG327679:MZH327679 NJC327679:NJD327679 NSY327679:NSZ327679 OCU327679:OCV327679 OMQ327679:OMR327679 OWM327679:OWN327679 PGI327679:PGJ327679 PQE327679:PQF327679 QAA327679:QAB327679 QJW327679:QJX327679 QTS327679:QTT327679 RDO327679:RDP327679 RNK327679:RNL327679 RXG327679:RXH327679 SHC327679:SHD327679 SQY327679:SQZ327679 TAU327679:TAV327679 TKQ327679:TKR327679 TUM327679:TUN327679 UEI327679:UEJ327679 UOE327679:UOF327679 UYA327679:UYB327679 VHW327679:VHX327679 VRS327679:VRT327679 WBO327679:WBP327679 WLK327679:WLL327679 WVG327679:WVH327679 IU393215:IV393215 SQ393215:SR393215 ACM393215:ACN393215 AMI393215:AMJ393215 AWE393215:AWF393215 BGA393215:BGB393215 BPW393215:BPX393215 BZS393215:BZT393215 CJO393215:CJP393215 CTK393215:CTL393215 DDG393215:DDH393215 DNC393215:DND393215 DWY393215:DWZ393215 EGU393215:EGV393215 EQQ393215:EQR393215 FAM393215:FAN393215 FKI393215:FKJ393215 FUE393215:FUF393215 GEA393215:GEB393215 GNW393215:GNX393215 GXS393215:GXT393215 HHO393215:HHP393215 HRK393215:HRL393215 IBG393215:IBH393215 ILC393215:ILD393215 IUY393215:IUZ393215 JEU393215:JEV393215 JOQ393215:JOR393215 JYM393215:JYN393215 KII393215:KIJ393215 KSE393215:KSF393215 LCA393215:LCB393215 LLW393215:LLX393215 LVS393215:LVT393215 MFO393215:MFP393215 MPK393215:MPL393215 MZG393215:MZH393215 NJC393215:NJD393215 NSY393215:NSZ393215 OCU393215:OCV393215 OMQ393215:OMR393215 OWM393215:OWN393215 PGI393215:PGJ393215 PQE393215:PQF393215 QAA393215:QAB393215 QJW393215:QJX393215 QTS393215:QTT393215 RDO393215:RDP393215 RNK393215:RNL393215 RXG393215:RXH393215 SHC393215:SHD393215 SQY393215:SQZ393215 TAU393215:TAV393215 TKQ393215:TKR393215 TUM393215:TUN393215 UEI393215:UEJ393215 UOE393215:UOF393215 UYA393215:UYB393215 VHW393215:VHX393215 VRS393215:VRT393215 WBO393215:WBP393215 WLK393215:WLL393215 WVG393215:WVH393215 IU458751:IV458751 SQ458751:SR458751 ACM458751:ACN458751 AMI458751:AMJ458751 AWE458751:AWF458751 BGA458751:BGB458751 BPW458751:BPX458751 BZS458751:BZT458751 CJO458751:CJP458751 CTK458751:CTL458751 DDG458751:DDH458751 DNC458751:DND458751 DWY458751:DWZ458751 EGU458751:EGV458751 EQQ458751:EQR458751 FAM458751:FAN458751 FKI458751:FKJ458751 FUE458751:FUF458751 GEA458751:GEB458751 GNW458751:GNX458751 GXS458751:GXT458751 HHO458751:HHP458751 HRK458751:HRL458751 IBG458751:IBH458751 ILC458751:ILD458751 IUY458751:IUZ458751 JEU458751:JEV458751 JOQ458751:JOR458751 JYM458751:JYN458751 KII458751:KIJ458751 KSE458751:KSF458751 LCA458751:LCB458751 LLW458751:LLX458751 LVS458751:LVT458751 MFO458751:MFP458751 MPK458751:MPL458751 MZG458751:MZH458751 NJC458751:NJD458751 NSY458751:NSZ458751 OCU458751:OCV458751 OMQ458751:OMR458751 OWM458751:OWN458751 PGI458751:PGJ458751 PQE458751:PQF458751 QAA458751:QAB458751 QJW458751:QJX458751 QTS458751:QTT458751 RDO458751:RDP458751 RNK458751:RNL458751 RXG458751:RXH458751 SHC458751:SHD458751 SQY458751:SQZ458751 TAU458751:TAV458751 TKQ458751:TKR458751 TUM458751:TUN458751 UEI458751:UEJ458751 UOE458751:UOF458751 UYA458751:UYB458751 VHW458751:VHX458751 VRS458751:VRT458751 WBO458751:WBP458751 WLK458751:WLL458751 WVG458751:WVH458751 IU524287:IV524287 SQ524287:SR524287 ACM524287:ACN524287 AMI524287:AMJ524287 AWE524287:AWF524287 BGA524287:BGB524287 BPW524287:BPX524287 BZS524287:BZT524287 CJO524287:CJP524287 CTK524287:CTL524287 DDG524287:DDH524287 DNC524287:DND524287 DWY524287:DWZ524287 EGU524287:EGV524287 EQQ524287:EQR524287 FAM524287:FAN524287 FKI524287:FKJ524287 FUE524287:FUF524287 GEA524287:GEB524287 GNW524287:GNX524287 GXS524287:GXT524287 HHO524287:HHP524287 HRK524287:HRL524287 IBG524287:IBH524287 ILC524287:ILD524287 IUY524287:IUZ524287 JEU524287:JEV524287 JOQ524287:JOR524287 JYM524287:JYN524287 KII524287:KIJ524287 KSE524287:KSF524287 LCA524287:LCB524287 LLW524287:LLX524287 LVS524287:LVT524287 MFO524287:MFP524287 MPK524287:MPL524287 MZG524287:MZH524287 NJC524287:NJD524287 NSY524287:NSZ524287 OCU524287:OCV524287 OMQ524287:OMR524287 OWM524287:OWN524287 PGI524287:PGJ524287 PQE524287:PQF524287 QAA524287:QAB524287 QJW524287:QJX524287 QTS524287:QTT524287 RDO524287:RDP524287 RNK524287:RNL524287 RXG524287:RXH524287 SHC524287:SHD524287 SQY524287:SQZ524287 TAU524287:TAV524287 TKQ524287:TKR524287 TUM524287:TUN524287 UEI524287:UEJ524287 UOE524287:UOF524287 UYA524287:UYB524287 VHW524287:VHX524287 VRS524287:VRT524287 WBO524287:WBP524287 WLK524287:WLL524287 WVG524287:WVH524287 IU589823:IV589823 SQ589823:SR589823 ACM589823:ACN589823 AMI589823:AMJ589823 AWE589823:AWF589823 BGA589823:BGB589823 BPW589823:BPX589823 BZS589823:BZT589823 CJO589823:CJP589823 CTK589823:CTL589823 DDG589823:DDH589823 DNC589823:DND589823 DWY589823:DWZ589823 EGU589823:EGV589823 EQQ589823:EQR589823 FAM589823:FAN589823 FKI589823:FKJ589823 FUE589823:FUF589823 GEA589823:GEB589823 GNW589823:GNX589823 GXS589823:GXT589823 HHO589823:HHP589823 HRK589823:HRL589823 IBG589823:IBH589823 ILC589823:ILD589823 IUY589823:IUZ589823 JEU589823:JEV589823 JOQ589823:JOR589823 JYM589823:JYN589823 KII589823:KIJ589823 KSE589823:KSF589823 LCA589823:LCB589823 LLW589823:LLX589823 LVS589823:LVT589823 MFO589823:MFP589823 MPK589823:MPL589823 MZG589823:MZH589823 NJC589823:NJD589823 NSY589823:NSZ589823 OCU589823:OCV589823 OMQ589823:OMR589823 OWM589823:OWN589823 PGI589823:PGJ589823 PQE589823:PQF589823 QAA589823:QAB589823 QJW589823:QJX589823 QTS589823:QTT589823 RDO589823:RDP589823 RNK589823:RNL589823 RXG589823:RXH589823 SHC589823:SHD589823 SQY589823:SQZ589823 TAU589823:TAV589823 TKQ589823:TKR589823 TUM589823:TUN589823 UEI589823:UEJ589823 UOE589823:UOF589823 UYA589823:UYB589823 VHW589823:VHX589823 VRS589823:VRT589823 WBO589823:WBP589823 WLK589823:WLL589823 WVG589823:WVH589823 IU655359:IV655359 SQ655359:SR655359 ACM655359:ACN655359 AMI655359:AMJ655359 AWE655359:AWF655359 BGA655359:BGB655359 BPW655359:BPX655359 BZS655359:BZT655359 CJO655359:CJP655359 CTK655359:CTL655359 DDG655359:DDH655359 DNC655359:DND655359 DWY655359:DWZ655359 EGU655359:EGV655359 EQQ655359:EQR655359 FAM655359:FAN655359 FKI655359:FKJ655359 FUE655359:FUF655359 GEA655359:GEB655359 GNW655359:GNX655359 GXS655359:GXT655359 HHO655359:HHP655359 HRK655359:HRL655359 IBG655359:IBH655359 ILC655359:ILD655359 IUY655359:IUZ655359 JEU655359:JEV655359 JOQ655359:JOR655359 JYM655359:JYN655359 KII655359:KIJ655359 KSE655359:KSF655359 LCA655359:LCB655359 LLW655359:LLX655359 LVS655359:LVT655359 MFO655359:MFP655359 MPK655359:MPL655359 MZG655359:MZH655359 NJC655359:NJD655359 NSY655359:NSZ655359 OCU655359:OCV655359 OMQ655359:OMR655359 OWM655359:OWN655359 PGI655359:PGJ655359 PQE655359:PQF655359 QAA655359:QAB655359 QJW655359:QJX655359 QTS655359:QTT655359 RDO655359:RDP655359 RNK655359:RNL655359 RXG655359:RXH655359 SHC655359:SHD655359 SQY655359:SQZ655359 TAU655359:TAV655359 TKQ655359:TKR655359 TUM655359:TUN655359 UEI655359:UEJ655359 UOE655359:UOF655359 UYA655359:UYB655359 VHW655359:VHX655359 VRS655359:VRT655359 WBO655359:WBP655359 WLK655359:WLL655359 WVG655359:WVH655359 IU720895:IV720895 SQ720895:SR720895 ACM720895:ACN720895 AMI720895:AMJ720895 AWE720895:AWF720895 BGA720895:BGB720895 BPW720895:BPX720895 BZS720895:BZT720895 CJO720895:CJP720895 CTK720895:CTL720895 DDG720895:DDH720895 DNC720895:DND720895 DWY720895:DWZ720895 EGU720895:EGV720895 EQQ720895:EQR720895 FAM720895:FAN720895 FKI720895:FKJ720895 FUE720895:FUF720895 GEA720895:GEB720895 GNW720895:GNX720895 GXS720895:GXT720895 HHO720895:HHP720895 HRK720895:HRL720895 IBG720895:IBH720895 ILC720895:ILD720895 IUY720895:IUZ720895 JEU720895:JEV720895 JOQ720895:JOR720895 JYM720895:JYN720895 KII720895:KIJ720895 KSE720895:KSF720895 LCA720895:LCB720895 LLW720895:LLX720895 LVS720895:LVT720895 MFO720895:MFP720895 MPK720895:MPL720895 MZG720895:MZH720895 NJC720895:NJD720895 NSY720895:NSZ720895 OCU720895:OCV720895 OMQ720895:OMR720895 OWM720895:OWN720895 PGI720895:PGJ720895 PQE720895:PQF720895 QAA720895:QAB720895 QJW720895:QJX720895 QTS720895:QTT720895 RDO720895:RDP720895 RNK720895:RNL720895 RXG720895:RXH720895 SHC720895:SHD720895 SQY720895:SQZ720895 TAU720895:TAV720895 TKQ720895:TKR720895 TUM720895:TUN720895 UEI720895:UEJ720895 UOE720895:UOF720895 UYA720895:UYB720895 VHW720895:VHX720895 VRS720895:VRT720895 WBO720895:WBP720895 WLK720895:WLL720895 WVG720895:WVH720895 IU786431:IV786431 SQ786431:SR786431 ACM786431:ACN786431 AMI786431:AMJ786431 AWE786431:AWF786431 BGA786431:BGB786431 BPW786431:BPX786431 BZS786431:BZT786431 CJO786431:CJP786431 CTK786431:CTL786431 DDG786431:DDH786431 DNC786431:DND786431 DWY786431:DWZ786431 EGU786431:EGV786431 EQQ786431:EQR786431 FAM786431:FAN786431 FKI786431:FKJ786431 FUE786431:FUF786431 GEA786431:GEB786431 GNW786431:GNX786431 GXS786431:GXT786431 HHO786431:HHP786431 HRK786431:HRL786431 IBG786431:IBH786431 ILC786431:ILD786431 IUY786431:IUZ786431 JEU786431:JEV786431 JOQ786431:JOR786431 JYM786431:JYN786431 KII786431:KIJ786431 KSE786431:KSF786431 LCA786431:LCB786431 LLW786431:LLX786431 LVS786431:LVT786431 MFO786431:MFP786431 MPK786431:MPL786431 MZG786431:MZH786431 NJC786431:NJD786431 NSY786431:NSZ786431 OCU786431:OCV786431 OMQ786431:OMR786431 OWM786431:OWN786431 PGI786431:PGJ786431 PQE786431:PQF786431 QAA786431:QAB786431 QJW786431:QJX786431 QTS786431:QTT786431 RDO786431:RDP786431 RNK786431:RNL786431 RXG786431:RXH786431 SHC786431:SHD786431 SQY786431:SQZ786431 TAU786431:TAV786431 TKQ786431:TKR786431 TUM786431:TUN786431 UEI786431:UEJ786431 UOE786431:UOF786431 UYA786431:UYB786431 VHW786431:VHX786431 VRS786431:VRT786431 WBO786431:WBP786431 WLK786431:WLL786431 WVG786431:WVH786431 IU851967:IV851967 SQ851967:SR851967 ACM851967:ACN851967 AMI851967:AMJ851967 AWE851967:AWF851967 BGA851967:BGB851967 BPW851967:BPX851967 BZS851967:BZT851967 CJO851967:CJP851967 CTK851967:CTL851967 DDG851967:DDH851967 DNC851967:DND851967 DWY851967:DWZ851967 EGU851967:EGV851967 EQQ851967:EQR851967 FAM851967:FAN851967 FKI851967:FKJ851967 FUE851967:FUF851967 GEA851967:GEB851967 GNW851967:GNX851967 GXS851967:GXT851967 HHO851967:HHP851967 HRK851967:HRL851967 IBG851967:IBH851967 ILC851967:ILD851967 IUY851967:IUZ851967 JEU851967:JEV851967 JOQ851967:JOR851967 JYM851967:JYN851967 KII851967:KIJ851967 KSE851967:KSF851967 LCA851967:LCB851967 LLW851967:LLX851967 LVS851967:LVT851967 MFO851967:MFP851967 MPK851967:MPL851967 MZG851967:MZH851967 NJC851967:NJD851967 NSY851967:NSZ851967 OCU851967:OCV851967 OMQ851967:OMR851967 OWM851967:OWN851967 PGI851967:PGJ851967 PQE851967:PQF851967 QAA851967:QAB851967 QJW851967:QJX851967 QTS851967:QTT851967 RDO851967:RDP851967 RNK851967:RNL851967 RXG851967:RXH851967 SHC851967:SHD851967 SQY851967:SQZ851967 TAU851967:TAV851967 TKQ851967:TKR851967 TUM851967:TUN851967 UEI851967:UEJ851967 UOE851967:UOF851967 UYA851967:UYB851967 VHW851967:VHX851967 VRS851967:VRT851967 WBO851967:WBP851967 WLK851967:WLL851967 WVG851967:WVH851967 IU917503:IV917503 SQ917503:SR917503 ACM917503:ACN917503 AMI917503:AMJ917503 AWE917503:AWF917503 BGA917503:BGB917503 BPW917503:BPX917503 BZS917503:BZT917503 CJO917503:CJP917503 CTK917503:CTL917503 DDG917503:DDH917503 DNC917503:DND917503 DWY917503:DWZ917503 EGU917503:EGV917503 EQQ917503:EQR917503 FAM917503:FAN917503 FKI917503:FKJ917503 FUE917503:FUF917503 GEA917503:GEB917503 GNW917503:GNX917503 GXS917503:GXT917503 HHO917503:HHP917503 HRK917503:HRL917503 IBG917503:IBH917503 ILC917503:ILD917503 IUY917503:IUZ917503 JEU917503:JEV917503 JOQ917503:JOR917503 JYM917503:JYN917503 KII917503:KIJ917503 KSE917503:KSF917503 LCA917503:LCB917503 LLW917503:LLX917503 LVS917503:LVT917503 MFO917503:MFP917503 MPK917503:MPL917503 MZG917503:MZH917503 NJC917503:NJD917503 NSY917503:NSZ917503 OCU917503:OCV917503 OMQ917503:OMR917503 OWM917503:OWN917503 PGI917503:PGJ917503 PQE917503:PQF917503 QAA917503:QAB917503 QJW917503:QJX917503 QTS917503:QTT917503 RDO917503:RDP917503 RNK917503:RNL917503 RXG917503:RXH917503 SHC917503:SHD917503 SQY917503:SQZ917503 TAU917503:TAV917503 TKQ917503:TKR917503 TUM917503:TUN917503 UEI917503:UEJ917503 UOE917503:UOF917503 UYA917503:UYB917503 VHW917503:VHX917503 VRS917503:VRT917503 WBO917503:WBP917503 WLK917503:WLL917503 WVG917503:WVH917503 IU983039:IV983039 SQ983039:SR983039 ACM983039:ACN983039 AMI983039:AMJ983039 AWE983039:AWF983039 BGA983039:BGB983039 BPW983039:BPX983039 BZS983039:BZT983039 CJO983039:CJP983039 CTK983039:CTL983039 DDG983039:DDH983039 DNC983039:DND983039 DWY983039:DWZ983039 EGU983039:EGV983039 EQQ983039:EQR983039 FAM983039:FAN983039 FKI983039:FKJ983039 FUE983039:FUF983039 GEA983039:GEB983039 GNW983039:GNX983039 GXS983039:GXT983039 HHO983039:HHP983039 HRK983039:HRL983039 IBG983039:IBH983039 ILC983039:ILD983039 IUY983039:IUZ983039 JEU983039:JEV983039 JOQ983039:JOR983039 JYM983039:JYN983039 KII983039:KIJ983039 KSE983039:KSF983039 LCA983039:LCB983039 LLW983039:LLX983039 LVS983039:LVT983039 MFO983039:MFP983039 MPK983039:MPL983039 MZG983039:MZH983039 NJC983039:NJD983039 NSY983039:NSZ983039 OCU983039:OCV983039 OMQ983039:OMR983039 OWM983039:OWN983039 PGI983039:PGJ983039 PQE983039:PQF983039 QAA983039:QAB983039 QJW983039:QJX983039 QTS983039:QTT983039 RDO983039:RDP983039 RNK983039:RNL983039 RXG983039:RXH983039 SHC983039:SHD983039 SQY983039:SQZ983039 TAU983039:TAV983039 TKQ983039:TKR983039 TUM983039:TUN983039 UEI983039:UEJ983039 UOE983039:UOF983039 UYA983039:UYB983039 VHW983039:VHX983039 VRS983039:VRT983039 WBO983039:WBP983039 WLK983039:WLL983039 WVG983039:WVH983039 C983039 C917503 C851967 C786431 C720895 C655359 C589823 C524287 C458751 C393215 C327679 C262143 C196607 C131071 C65535 C5" xr:uid="{FC8C5A74-6D93-453B-B734-4B441F9815E5}">
+      <formula1>-1000000000000</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Benefit type; e.g., Service Retirement, Ordinary Disability" sqref="B5 IT5 SP5 ACL5 AMH5 AWD5 BFZ5 BPV5 BZR5 CJN5 CTJ5 DDF5 DNB5 DWX5 EGT5 EQP5 FAL5 FKH5 FUD5 GDZ5 GNV5 GXR5 HHN5 HRJ5 IBF5 ILB5 IUX5 JET5 JOP5 JYL5 KIH5 KSD5 LBZ5 LLV5 LVR5 MFN5 MPJ5 MZF5 NJB5 NSX5 OCT5 OMP5 OWL5 PGH5 PQD5 PZZ5 QJV5 QTR5 RDN5 RNJ5 RXF5 SHB5 SQX5 TAT5 TKP5 TUL5 UEH5 UOD5 UXZ5 VHV5 VRR5 WBN5 WLJ5 WVF5 B65535 IT65535 SP65535 ACL65535 AMH65535 AWD65535 BFZ65535 BPV65535 BZR65535 CJN65535 CTJ65535 DDF65535 DNB65535 DWX65535 EGT65535 EQP65535 FAL65535 FKH65535 FUD65535 GDZ65535 GNV65535 GXR65535 HHN65535 HRJ65535 IBF65535 ILB65535 IUX65535 JET65535 JOP65535 JYL65535 KIH65535 KSD65535 LBZ65535 LLV65535 LVR65535 MFN65535 MPJ65535 MZF65535 NJB65535 NSX65535 OCT65535 OMP65535 OWL65535 PGH65535 PQD65535 PZZ65535 QJV65535 QTR65535 RDN65535 RNJ65535 RXF65535 SHB65535 SQX65535 TAT65535 TKP65535 TUL65535 UEH65535 UOD65535 UXZ65535 VHV65535 VRR65535 WBN65535 WLJ65535 WVF65535 B131071 IT131071 SP131071 ACL131071 AMH131071 AWD131071 BFZ131071 BPV131071 BZR131071 CJN131071 CTJ131071 DDF131071 DNB131071 DWX131071 EGT131071 EQP131071 FAL131071 FKH131071 FUD131071 GDZ131071 GNV131071 GXR131071 HHN131071 HRJ131071 IBF131071 ILB131071 IUX131071 JET131071 JOP131071 JYL131071 KIH131071 KSD131071 LBZ131071 LLV131071 LVR131071 MFN131071 MPJ131071 MZF131071 NJB131071 NSX131071 OCT131071 OMP131071 OWL131071 PGH131071 PQD131071 PZZ131071 QJV131071 QTR131071 RDN131071 RNJ131071 RXF131071 SHB131071 SQX131071 TAT131071 TKP131071 TUL131071 UEH131071 UOD131071 UXZ131071 VHV131071 VRR131071 WBN131071 WLJ131071 WVF131071 B196607 IT196607 SP196607 ACL196607 AMH196607 AWD196607 BFZ196607 BPV196607 BZR196607 CJN196607 CTJ196607 DDF196607 DNB196607 DWX196607 EGT196607 EQP196607 FAL196607 FKH196607 FUD196607 GDZ196607 GNV196607 GXR196607 HHN196607 HRJ196607 IBF196607 ILB196607 IUX196607 JET196607 JOP196607 JYL196607 KIH196607 KSD196607 LBZ196607 LLV196607 LVR196607 MFN196607 MPJ196607 MZF196607 NJB196607 NSX196607 OCT196607 OMP196607 OWL196607 PGH196607 PQD196607 PZZ196607 QJV196607 QTR196607 RDN196607 RNJ196607 RXF196607 SHB196607 SQX196607 TAT196607 TKP196607 TUL196607 UEH196607 UOD196607 UXZ196607 VHV196607 VRR196607 WBN196607 WLJ196607 WVF196607 B262143 IT262143 SP262143 ACL262143 AMH262143 AWD262143 BFZ262143 BPV262143 BZR262143 CJN262143 CTJ262143 DDF262143 DNB262143 DWX262143 EGT262143 EQP262143 FAL262143 FKH262143 FUD262143 GDZ262143 GNV262143 GXR262143 HHN262143 HRJ262143 IBF262143 ILB262143 IUX262143 JET262143 JOP262143 JYL262143 KIH262143 KSD262143 LBZ262143 LLV262143 LVR262143 MFN262143 MPJ262143 MZF262143 NJB262143 NSX262143 OCT262143 OMP262143 OWL262143 PGH262143 PQD262143 PZZ262143 QJV262143 QTR262143 RDN262143 RNJ262143 RXF262143 SHB262143 SQX262143 TAT262143 TKP262143 TUL262143 UEH262143 UOD262143 UXZ262143 VHV262143 VRR262143 WBN262143 WLJ262143 WVF262143 B327679 IT327679 SP327679 ACL327679 AMH327679 AWD327679 BFZ327679 BPV327679 BZR327679 CJN327679 CTJ327679 DDF327679 DNB327679 DWX327679 EGT327679 EQP327679 FAL327679 FKH327679 FUD327679 GDZ327679 GNV327679 GXR327679 HHN327679 HRJ327679 IBF327679 ILB327679 IUX327679 JET327679 JOP327679 JYL327679 KIH327679 KSD327679 LBZ327679 LLV327679 LVR327679 MFN327679 MPJ327679 MZF327679 NJB327679 NSX327679 OCT327679 OMP327679 OWL327679 PGH327679 PQD327679 PZZ327679 QJV327679 QTR327679 RDN327679 RNJ327679 RXF327679 SHB327679 SQX327679 TAT327679 TKP327679 TUL327679 UEH327679 UOD327679 UXZ327679 VHV327679 VRR327679 WBN327679 WLJ327679 WVF327679 B393215 IT393215 SP393215 ACL393215 AMH393215 AWD393215 BFZ393215 BPV393215 BZR393215 CJN393215 CTJ393215 DDF393215 DNB393215 DWX393215 EGT393215 EQP393215 FAL393215 FKH393215 FUD393215 GDZ393215 GNV393215 GXR393215 HHN393215 HRJ393215 IBF393215 ILB393215 IUX393215 JET393215 JOP393215 JYL393215 KIH393215 KSD393215 LBZ393215 LLV393215 LVR393215 MFN393215 MPJ393215 MZF393215 NJB393215 NSX393215 OCT393215 OMP393215 OWL393215 PGH393215 PQD393215 PZZ393215 QJV393215 QTR393215 RDN393215 RNJ393215 RXF393215 SHB393215 SQX393215 TAT393215 TKP393215 TUL393215 UEH393215 UOD393215 UXZ393215 VHV393215 VRR393215 WBN393215 WLJ393215 WVF393215 B458751 IT458751 SP458751 ACL458751 AMH458751 AWD458751 BFZ458751 BPV458751 BZR458751 CJN458751 CTJ458751 DDF458751 DNB458751 DWX458751 EGT458751 EQP458751 FAL458751 FKH458751 FUD458751 GDZ458751 GNV458751 GXR458751 HHN458751 HRJ458751 IBF458751 ILB458751 IUX458751 JET458751 JOP458751 JYL458751 KIH458751 KSD458751 LBZ458751 LLV458751 LVR458751 MFN458751 MPJ458751 MZF458751 NJB458751 NSX458751 OCT458751 OMP458751 OWL458751 PGH458751 PQD458751 PZZ458751 QJV458751 QTR458751 RDN458751 RNJ458751 RXF458751 SHB458751 SQX458751 TAT458751 TKP458751 TUL458751 UEH458751 UOD458751 UXZ458751 VHV458751 VRR458751 WBN458751 WLJ458751 WVF458751 B524287 IT524287 SP524287 ACL524287 AMH524287 AWD524287 BFZ524287 BPV524287 BZR524287 CJN524287 CTJ524287 DDF524287 DNB524287 DWX524287 EGT524287 EQP524287 FAL524287 FKH524287 FUD524287 GDZ524287 GNV524287 GXR524287 HHN524287 HRJ524287 IBF524287 ILB524287 IUX524287 JET524287 JOP524287 JYL524287 KIH524287 KSD524287 LBZ524287 LLV524287 LVR524287 MFN524287 MPJ524287 MZF524287 NJB524287 NSX524287 OCT524287 OMP524287 OWL524287 PGH524287 PQD524287 PZZ524287 QJV524287 QTR524287 RDN524287 RNJ524287 RXF524287 SHB524287 SQX524287 TAT524287 TKP524287 TUL524287 UEH524287 UOD524287 UXZ524287 VHV524287 VRR524287 WBN524287 WLJ524287 WVF524287 B589823 IT589823 SP589823 ACL589823 AMH589823 AWD589823 BFZ589823 BPV589823 BZR589823 CJN589823 CTJ589823 DDF589823 DNB589823 DWX589823 EGT589823 EQP589823 FAL589823 FKH589823 FUD589823 GDZ589823 GNV589823 GXR589823 HHN589823 HRJ589823 IBF589823 ILB589823 IUX589823 JET589823 JOP589823 JYL589823 KIH589823 KSD589823 LBZ589823 LLV589823 LVR589823 MFN589823 MPJ589823 MZF589823 NJB589823 NSX589823 OCT589823 OMP589823 OWL589823 PGH589823 PQD589823 PZZ589823 QJV589823 QTR589823 RDN589823 RNJ589823 RXF589823 SHB589823 SQX589823 TAT589823 TKP589823 TUL589823 UEH589823 UOD589823 UXZ589823 VHV589823 VRR589823 WBN589823 WLJ589823 WVF589823 B655359 IT655359 SP655359 ACL655359 AMH655359 AWD655359 BFZ655359 BPV655359 BZR655359 CJN655359 CTJ655359 DDF655359 DNB655359 DWX655359 EGT655359 EQP655359 FAL655359 FKH655359 FUD655359 GDZ655359 GNV655359 GXR655359 HHN655359 HRJ655359 IBF655359 ILB655359 IUX655359 JET655359 JOP655359 JYL655359 KIH655359 KSD655359 LBZ655359 LLV655359 LVR655359 MFN655359 MPJ655359 MZF655359 NJB655359 NSX655359 OCT655359 OMP655359 OWL655359 PGH655359 PQD655359 PZZ655359 QJV655359 QTR655359 RDN655359 RNJ655359 RXF655359 SHB655359 SQX655359 TAT655359 TKP655359 TUL655359 UEH655359 UOD655359 UXZ655359 VHV655359 VRR655359 WBN655359 WLJ655359 WVF655359 B720895 IT720895 SP720895 ACL720895 AMH720895 AWD720895 BFZ720895 BPV720895 BZR720895 CJN720895 CTJ720895 DDF720895 DNB720895 DWX720895 EGT720895 EQP720895 FAL720895 FKH720895 FUD720895 GDZ720895 GNV720895 GXR720895 HHN720895 HRJ720895 IBF720895 ILB720895 IUX720895 JET720895 JOP720895 JYL720895 KIH720895 KSD720895 LBZ720895 LLV720895 LVR720895 MFN720895 MPJ720895 MZF720895 NJB720895 NSX720895 OCT720895 OMP720895 OWL720895 PGH720895 PQD720895 PZZ720895 QJV720895 QTR720895 RDN720895 RNJ720895 RXF720895 SHB720895 SQX720895 TAT720895 TKP720895 TUL720895 UEH720895 UOD720895 UXZ720895 VHV720895 VRR720895 WBN720895 WLJ720895 WVF720895 B786431 IT786431 SP786431 ACL786431 AMH786431 AWD786431 BFZ786431 BPV786431 BZR786431 CJN786431 CTJ786431 DDF786431 DNB786431 DWX786431 EGT786431 EQP786431 FAL786431 FKH786431 FUD786431 GDZ786431 GNV786431 GXR786431 HHN786431 HRJ786431 IBF786431 ILB786431 IUX786431 JET786431 JOP786431 JYL786431 KIH786431 KSD786431 LBZ786431 LLV786431 LVR786431 MFN786431 MPJ786431 MZF786431 NJB786431 NSX786431 OCT786431 OMP786431 OWL786431 PGH786431 PQD786431 PZZ786431 QJV786431 QTR786431 RDN786431 RNJ786431 RXF786431 SHB786431 SQX786431 TAT786431 TKP786431 TUL786431 UEH786431 UOD786431 UXZ786431 VHV786431 VRR786431 WBN786431 WLJ786431 WVF786431 B851967 IT851967 SP851967 ACL851967 AMH851967 AWD851967 BFZ851967 BPV851967 BZR851967 CJN851967 CTJ851967 DDF851967 DNB851967 DWX851967 EGT851967 EQP851967 FAL851967 FKH851967 FUD851967 GDZ851967 GNV851967 GXR851967 HHN851967 HRJ851967 IBF851967 ILB851967 IUX851967 JET851967 JOP851967 JYL851967 KIH851967 KSD851967 LBZ851967 LLV851967 LVR851967 MFN851967 MPJ851967 MZF851967 NJB851967 NSX851967 OCT851967 OMP851967 OWL851967 PGH851967 PQD851967 PZZ851967 QJV851967 QTR851967 RDN851967 RNJ851967 RXF851967 SHB851967 SQX851967 TAT851967 TKP851967 TUL851967 UEH851967 UOD851967 UXZ851967 VHV851967 VRR851967 WBN851967 WLJ851967 WVF851967 B917503 IT917503 SP917503 ACL917503 AMH917503 AWD917503 BFZ917503 BPV917503 BZR917503 CJN917503 CTJ917503 DDF917503 DNB917503 DWX917503 EGT917503 EQP917503 FAL917503 FKH917503 FUD917503 GDZ917503 GNV917503 GXR917503 HHN917503 HRJ917503 IBF917503 ILB917503 IUX917503 JET917503 JOP917503 JYL917503 KIH917503 KSD917503 LBZ917503 LLV917503 LVR917503 MFN917503 MPJ917503 MZF917503 NJB917503 NSX917503 OCT917503 OMP917503 OWL917503 PGH917503 PQD917503 PZZ917503 QJV917503 QTR917503 RDN917503 RNJ917503 RXF917503 SHB917503 SQX917503 TAT917503 TKP917503 TUL917503 UEH917503 UOD917503 UXZ917503 VHV917503 VRR917503 WBN917503 WLJ917503 WVF917503 B983039 IT983039 SP983039 ACL983039 AMH983039 AWD983039 BFZ983039 BPV983039 BZR983039 CJN983039 CTJ983039 DDF983039 DNB983039 DWX983039 EGT983039 EQP983039 FAL983039 FKH983039 FUD983039 GDZ983039 GNV983039 GXR983039 HHN983039 HRJ983039 IBF983039 ILB983039 IUX983039 JET983039 JOP983039 JYL983039 KIH983039 KSD983039 LBZ983039 LLV983039 LVR983039 MFN983039 MPJ983039 MZF983039 NJB983039 NSX983039 OCT983039 OMP983039 OWL983039 PGH983039 PQD983039 PZZ983039 QJV983039 QTR983039 RDN983039 RNJ983039 RXF983039 SHB983039 SQX983039 TAT983039 TKP983039 TUL983039 UEH983039 UOD983039 UXZ983039 VHV983039 VRR983039 WBN983039 WLJ983039 WVF983039" xr:uid="{EFAD6EF3-883A-4668-AAC1-A42340E2A7BF}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4FDDF8-106A-47EA-BD4C-5B4A1371B873}">
-  <dimension ref="B2:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E10804-3FBF-4684-9424-690AFBFFB981}">
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="8" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B1">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="27">
-        <v>70000777</v>
-      </c>
-      <c r="D4" s="27">
-        <v>43629545</v>
-      </c>
-      <c r="G4">
-        <v>20292733</v>
-      </c>
-      <c r="I4" s="29">
-        <f>G4/D4</f>
-        <v>0.46511447689862456</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9">
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="27">
-        <v>73323430</v>
-      </c>
-      <c r="D5" s="27">
-        <v>50095723</v>
+        <v>285</v>
+      </c>
+      <c r="C4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G4" t="s">
+        <v>287</v>
+      </c>
+      <c r="H4" t="s">
+        <v>288</v>
+      </c>
+      <c r="I4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <f>B1</f>
+        <v>47000</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>SUM(D4:D$5)</f>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>22004183</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
-      <c r="C6" s="28"/>
+        <f>$B$1</f>
+        <v>47000</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>SUM(H4:H$5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6">
+        <v>61</v>
+      </c>
+      <c r="C6" s="160">
+        <f t="shared" ref="C6:C14" si="0">C5+D5</f>
+        <v>47000</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>SUM(D$5:D5)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="160">
+        <f t="shared" ref="G6:G14" si="1">G5+H5</f>
+        <v>47000</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>SUM(H$5:H5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7">
+        <v>62</v>
+      </c>
+      <c r="C7" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>SUM(D$5:D6)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>SUM(H$5:H6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8">
+        <v>63</v>
+      </c>
+      <c r="C8" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>SUM(D$5:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>SUM(H$5:H7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>SUM(D$5:D8)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>SUM(H$5:H8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10">
+        <v>65</v>
+      </c>
+      <c r="C10" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>SUM(D$5:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUM(H$5:H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11">
+        <v>66</v>
+      </c>
+      <c r="C11" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>SUM(D$5:D10)</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>SUM(H$5:H10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12">
+        <v>67</v>
+      </c>
+      <c r="C12" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>SUM(D$5:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f>SUM(H$5:H11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13">
+        <v>68</v>
+      </c>
+      <c r="C13" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>SUM(D$5:D12)</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>SUM(H$5:H12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14">
+        <v>69</v>
+      </c>
+      <c r="C14" s="160">
+        <f t="shared" si="0"/>
+        <v>47000</v>
+      </c>
+      <c r="D14">
+        <f>(MIN($B$1, $B$2) +E14) *(0.015)</f>
+        <v>270</v>
+      </c>
+      <c r="E14">
+        <f>SUM(D$5:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="160">
+        <f t="shared" si="1"/>
+        <v>47000</v>
+      </c>
+      <c r="H14">
+        <f>MIN($B$1, $B$2)  *(0.015)</f>
+        <v>270</v>
+      </c>
+      <c r="I14">
+        <f>SUM(H$5:H13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="C15" s="160">
+        <f>C14+D14</f>
+        <v>47270</v>
+      </c>
+      <c r="D15" s="160">
+        <f>(MIN($B$1, $B$2) +E15) *(0.015)</f>
+        <v>274.05</v>
+      </c>
+      <c r="E15" s="160">
+        <f>SUM(D$5:D14)</f>
+        <v>270</v>
+      </c>
+      <c r="G15" s="160">
+        <f>G14+H14</f>
+        <v>47270</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:H35" si="2">MIN($B$1, $B$2)  *(0.015)</f>
+        <v>270</v>
+      </c>
+      <c r="I15" s="160">
+        <f>SUM(H$5:H14)</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16">
+        <v>71</v>
+      </c>
+      <c r="C16" s="160">
+        <f t="shared" ref="C16:C35" si="3">C15+D15</f>
+        <v>47544.05</v>
+      </c>
+      <c r="D16" s="160">
+        <f t="shared" ref="D16:D35" si="4">(MIN($B$1, $B$2) +E16) *(0.015)</f>
+        <v>278.16074999999995</v>
+      </c>
+      <c r="E16" s="160">
+        <f>SUM(D$5:D15)</f>
+        <v>544.04999999999995</v>
+      </c>
+      <c r="G16" s="160">
+        <f t="shared" ref="G16:G35" si="5">G15+H15</f>
+        <v>47540</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I16" s="160">
+        <f>SUM(H$5:H15)</f>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17">
+        <v>72</v>
+      </c>
+      <c r="C17" s="160">
+        <f t="shared" si="3"/>
+        <v>47822.210750000006</v>
+      </c>
+      <c r="D17" s="160">
+        <f t="shared" si="4"/>
+        <v>282.33316124999999</v>
+      </c>
+      <c r="E17" s="160">
+        <f>SUM(D$5:D16)</f>
+        <v>822.21074999999996</v>
+      </c>
+      <c r="G17" s="160">
+        <f t="shared" si="5"/>
+        <v>47810</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I17" s="160">
+        <f>SUM(H$5:H16)</f>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18">
+        <v>73</v>
+      </c>
+      <c r="C18" s="160">
+        <f t="shared" si="3"/>
+        <v>48104.543911250003</v>
+      </c>
+      <c r="D18" s="160">
+        <f t="shared" si="4"/>
+        <v>286.56815866874996</v>
+      </c>
+      <c r="E18" s="160">
+        <f>SUM(D$5:D17)</f>
+        <v>1104.5439112499998</v>
+      </c>
+      <c r="G18" s="160">
+        <f t="shared" si="5"/>
+        <v>48080</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I18" s="160">
+        <f>SUM(H$5:H17)</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19">
+        <v>74</v>
+      </c>
+      <c r="C19" s="160">
+        <f t="shared" si="3"/>
+        <v>48391.112069918752</v>
+      </c>
+      <c r="D19" s="160">
+        <f t="shared" si="4"/>
+        <v>290.86668104878123</v>
+      </c>
+      <c r="E19" s="160">
+        <f>SUM(D$5:D18)</f>
+        <v>1391.1120699187497</v>
+      </c>
+      <c r="G19" s="160">
+        <f t="shared" si="5"/>
+        <v>48350</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I19" s="160">
+        <f>SUM(H$5:H18)</f>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20">
+        <v>75</v>
+      </c>
+      <c r="C20" s="160">
+        <f t="shared" si="3"/>
+        <v>48681.978750967537</v>
+      </c>
+      <c r="D20" s="160">
+        <f t="shared" si="4"/>
+        <v>295.22968126451292</v>
+      </c>
+      <c r="E20" s="160">
+        <f>SUM(D$5:D19)</f>
+        <v>1681.9787509675309</v>
+      </c>
+      <c r="G20" s="160">
+        <f t="shared" si="5"/>
+        <v>48620</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I20" s="160">
+        <f>SUM(H$5:H19)</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21">
+        <v>76</v>
+      </c>
+      <c r="C21" s="160">
+        <f t="shared" si="3"/>
+        <v>48977.208432232052</v>
+      </c>
+      <c r="D21" s="160">
+        <f t="shared" si="4"/>
+        <v>299.65812648348066</v>
+      </c>
+      <c r="E21" s="160">
+        <f>SUM(D$5:D20)</f>
+        <v>1977.2084322320438</v>
+      </c>
+      <c r="G21" s="160">
+        <f t="shared" si="5"/>
+        <v>48890</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I21" s="160">
+        <f>SUM(H$5:H20)</f>
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22">
+        <v>77</v>
+      </c>
+      <c r="C22" s="160">
+        <f t="shared" si="3"/>
+        <v>49276.866558715534</v>
+      </c>
+      <c r="D22" s="160">
+        <f t="shared" si="4"/>
+        <v>304.15299838073287</v>
+      </c>
+      <c r="E22" s="160">
+        <f>SUM(D$5:D21)</f>
+        <v>2276.8665587155247</v>
+      </c>
+      <c r="G22" s="160">
+        <f t="shared" si="5"/>
+        <v>49160</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I22" s="160">
+        <f>SUM(H$5:H21)</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23">
+        <v>78</v>
+      </c>
+      <c r="C23" s="160">
+        <f t="shared" si="3"/>
+        <v>49581.019557096268</v>
+      </c>
+      <c r="D23" s="160">
+        <f t="shared" si="4"/>
+        <v>308.71529335644385</v>
+      </c>
+      <c r="E23" s="160">
+        <f>SUM(D$5:D22)</f>
+        <v>2581.0195570962574</v>
+      </c>
+      <c r="G23" s="160">
+        <f t="shared" si="5"/>
+        <v>49430</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I23" s="160">
+        <f>SUM(H$5:H22)</f>
+        <v>2430</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24">
+        <v>79</v>
+      </c>
+      <c r="C24" s="160">
+        <f t="shared" si="3"/>
+        <v>49889.734850452711</v>
+      </c>
+      <c r="D24" s="160">
+        <f t="shared" si="4"/>
+        <v>313.34602275679049</v>
+      </c>
+      <c r="E24" s="160">
+        <f>SUM(D$5:D23)</f>
+        <v>2889.7348504527013</v>
+      </c>
+      <c r="G24" s="160">
+        <f t="shared" si="5"/>
+        <v>49700</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I24" s="160">
+        <f>SUM(H$5:H23)</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25">
+        <v>80</v>
+      </c>
+      <c r="C25" s="160">
+        <f t="shared" si="3"/>
+        <v>50203.080873209503</v>
+      </c>
+      <c r="D25" s="160">
+        <f t="shared" si="4"/>
+        <v>318.04621309814235</v>
+      </c>
+      <c r="E25" s="160">
+        <f>SUM(D$5:D24)</f>
+        <v>3203.080873209492</v>
+      </c>
+      <c r="G25" s="160">
+        <f t="shared" si="5"/>
+        <v>49970</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I25" s="160">
+        <f>SUM(H$5:H24)</f>
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26">
+        <v>81</v>
+      </c>
+      <c r="C26" s="160">
+        <f t="shared" si="3"/>
+        <v>50521.127086307642</v>
+      </c>
+      <c r="D26" s="160">
+        <f t="shared" si="4"/>
+        <v>322.81690629461451</v>
+      </c>
+      <c r="E26" s="160">
+        <f>SUM(D$5:D25)</f>
+        <v>3521.1270863076343</v>
+      </c>
+      <c r="G26" s="160">
+        <f t="shared" si="5"/>
+        <v>50240</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I26" s="160">
+        <f>SUM(H$5:H25)</f>
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27">
+        <v>82</v>
+      </c>
+      <c r="C27" s="160">
+        <f t="shared" si="3"/>
+        <v>50843.943992602261</v>
+      </c>
+      <c r="D27" s="160">
+        <f t="shared" si="4"/>
+        <v>327.65915988903373</v>
+      </c>
+      <c r="E27" s="160">
+        <f>SUM(D$5:D26)</f>
+        <v>3843.9439926022487</v>
+      </c>
+      <c r="G27" s="160">
+        <f t="shared" si="5"/>
+        <v>50510</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I27" s="160">
+        <f>SUM(H$5:H26)</f>
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28">
+        <v>83</v>
+      </c>
+      <c r="C28" s="160">
+        <f t="shared" si="3"/>
+        <v>51171.603152491298</v>
+      </c>
+      <c r="D28" s="160">
+        <f t="shared" si="4"/>
+        <v>332.57404728736924</v>
+      </c>
+      <c r="E28" s="160">
+        <f>SUM(D$5:D27)</f>
+        <v>4171.6031524912823</v>
+      </c>
+      <c r="G28" s="160">
+        <f t="shared" si="5"/>
+        <v>50780</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I28" s="160">
+        <f>SUM(H$5:H27)</f>
+        <v>3780</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29">
+        <v>84</v>
+      </c>
+      <c r="C29" s="160">
+        <f t="shared" si="3"/>
+        <v>51504.177199778664</v>
+      </c>
+      <c r="D29" s="160">
+        <f t="shared" si="4"/>
+        <v>337.56265799667977</v>
+      </c>
+      <c r="E29" s="160">
+        <f>SUM(D$5:D28)</f>
+        <v>4504.1771997786518</v>
+      </c>
+      <c r="G29" s="160">
+        <f t="shared" si="5"/>
+        <v>51050</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I29" s="160">
+        <f>SUM(H$5:H28)</f>
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30">
+        <v>85</v>
+      </c>
+      <c r="C30" s="160">
+        <f t="shared" si="3"/>
+        <v>51841.739857775341</v>
+      </c>
+      <c r="D30" s="160">
+        <f t="shared" si="4"/>
+        <v>342.62609786663</v>
+      </c>
+      <c r="E30" s="160">
+        <f>SUM(D$5:D29)</f>
+        <v>4841.739857775332</v>
+      </c>
+      <c r="G30" s="160">
+        <f t="shared" si="5"/>
+        <v>51320</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I30" s="160">
+        <f>SUM(H$5:H29)</f>
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31">
+        <v>86</v>
+      </c>
+      <c r="C31" s="160">
+        <f t="shared" si="3"/>
+        <v>52184.365955641973</v>
+      </c>
+      <c r="D31" s="160">
+        <f t="shared" si="4"/>
+        <v>347.76548933462942</v>
+      </c>
+      <c r="E31" s="160">
+        <f>SUM(D$5:D30)</f>
+        <v>5184.3659556419616</v>
+      </c>
+      <c r="G31" s="160">
+        <f t="shared" si="5"/>
+        <v>51590</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I31" s="160">
+        <f>SUM(H$5:H30)</f>
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32">
+        <v>87</v>
+      </c>
+      <c r="C32" s="160">
+        <f t="shared" si="3"/>
+        <v>52532.1314449766</v>
+      </c>
+      <c r="D32" s="160">
+        <f t="shared" si="4"/>
+        <v>352.98197167464889</v>
+      </c>
+      <c r="E32" s="160">
+        <f>SUM(D$5:D31)</f>
+        <v>5532.1314449765914</v>
+      </c>
+      <c r="G32" s="160">
+        <f t="shared" si="5"/>
+        <v>51860</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I32" s="160">
+        <f>SUM(H$5:H31)</f>
+        <v>4860</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33">
+        <v>88</v>
+      </c>
+      <c r="C33" s="160">
+        <f t="shared" si="3"/>
+        <v>52885.113416651249</v>
+      </c>
+      <c r="D33" s="160">
+        <f t="shared" si="4"/>
+        <v>358.27670124976862</v>
+      </c>
+      <c r="E33" s="160">
+        <f>SUM(D$5:D32)</f>
+        <v>5885.1134166512402</v>
+      </c>
+      <c r="G33" s="160">
+        <f t="shared" si="5"/>
+        <v>52130</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I33" s="160">
+        <f>SUM(H$5:H32)</f>
+        <v>5130</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34">
+        <v>89</v>
+      </c>
+      <c r="C34" s="160">
+        <f t="shared" si="3"/>
+        <v>53243.390117901021</v>
+      </c>
+      <c r="D34" s="160">
+        <f t="shared" si="4"/>
+        <v>363.65085176851511</v>
+      </c>
+      <c r="E34" s="160">
+        <f>SUM(D$5:D33)</f>
+        <v>6243.390117901009</v>
+      </c>
+      <c r="G34" s="160">
+        <f t="shared" si="5"/>
+        <v>52400</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I34" s="160">
+        <f>SUM(H$5:H33)</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35">
+        <v>90</v>
+      </c>
+      <c r="C35" s="160">
+        <f t="shared" si="3"/>
+        <v>53607.040969669535</v>
+      </c>
+      <c r="D35" s="160">
+        <f t="shared" si="4"/>
+        <v>369.10561454504284</v>
+      </c>
+      <c r="E35" s="160">
+        <f>SUM(D$5:D34)</f>
+        <v>6607.0409696695242</v>
+      </c>
+      <c r="G35" s="160">
+        <f t="shared" si="5"/>
+        <v>52670</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="I35" s="160">
+        <f>SUM(H$5:H34)</f>
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" t="s">
+        <v>290</v>
+      </c>
+      <c r="C37" s="161">
+        <f>NPV(0.07,C5:C35)</f>
+        <v>602958.80571988749</v>
+      </c>
+      <c r="G37" s="161">
+        <f>NPV(0.07,G5:G35)</f>
+        <v>601783.9164313064</v>
+      </c>
+      <c r="J37" t="s">
+        <v>291</v>
+      </c>
+      <c r="K37" s="6">
+        <f>C37/G37 - 1</f>
+        <v>1.9523441163871169E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test steady state demographic
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6BFA98-EF50-4033-B508-BA1482AA768F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F87502-8A9F-4810-889B-C21779F7083B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1530" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -52,7 +52,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Skip the year-1 amort. payment for new amortization basis. 
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -78,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 20292733/43629545 = 46.5%</t>
@@ -118,7 +118,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -127,7 +127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 AL_pct; AA0, noSmoothing</t>
@@ -747,7 +747,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,19 +790,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1467,11 +1454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:BE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,7 +1769,7 @@
         <v>138</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0.3</v>
@@ -2261,7 +2248,7 @@
         <v>161</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0.3</v>
@@ -6030,7 +6017,7 @@
   <dimension ref="A3:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6079,7 +6066,7 @@
         <v>2000</v>
       </c>
       <c r="C4">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -6112,8 +6099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6235,7 +6222,7 @@
         <v>0.12</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update figures and calibrations for TRS
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36281236-8B6A-443B-AB14-AEB31FB23958}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A923CFE-CF6E-4C4A-BE64-95A32BC5A9D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2462,10 +2462,10 @@
   <dimension ref="A3:BH46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="AQ8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="AW16" sqref="AW16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3985,7 +3985,7 @@
         <v>115</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0.3</v>
@@ -4152,7 +4152,7 @@
         <v>115</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0.3</v>
@@ -4319,7 +4319,7 @@
         <v>115</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>0.3</v>
@@ -4486,7 +4486,7 @@
         <v>115</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0.3</v>
@@ -4653,7 +4653,7 @@
         <v>115</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0.3</v>
@@ -4820,7 +4820,7 @@
         <v>114</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <v>0.3</v>
@@ -8259,7 +8259,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8313,7 +8313,7 @@
         <v>0.13</v>
       </c>
       <c r="F2" s="6">
-        <f t="shared" ref="F2:F10" si="1">B2 - C2^2/2</f>
+        <f t="shared" ref="F2:F3" si="1">B2 - C2^2/2</f>
         <v>0.13</v>
       </c>
       <c r="G2" t="s">
@@ -8363,7 +8363,6 @@
         <v>0.02</v>
       </c>
       <c r="F4" s="6">
-        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="G4" t="s">
@@ -8388,7 +8387,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F2:F10" si="2">B5 - C5^2/2</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G5" t="s">
@@ -8413,7 +8412,7 @@
         <v>0.13</v>
       </c>
       <c r="F6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.13</v>
       </c>
       <c r="G6" t="s">
@@ -8438,7 +8437,7 @@
         <v>0.128</v>
       </c>
       <c r="F7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.128</v>
       </c>
       <c r="G7" t="s">
@@ -8463,7 +8462,6 @@
         <v>0.02</v>
       </c>
       <c r="F8" s="6">
-        <f t="shared" si="1"/>
         <v>0.02</v>
       </c>
       <c r="G8" t="s">
@@ -8488,7 +8486,7 @@
         <v>0.05</v>
       </c>
       <c r="F9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.05</v>
       </c>
       <c r="G9" t="s">
@@ -8513,7 +8511,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G10" t="s">
@@ -8538,7 +8536,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" ref="F11:F20" si="2">B11 - C11^2/2</f>
+        <f t="shared" ref="F11:F20" si="3">B11 - C11^2/2</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G11" t="s">
@@ -8563,7 +8561,7 @@
         <v>0.13</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13</v>
       </c>
       <c r="G12" t="s">
@@ -8588,7 +8586,7 @@
         <v>0.128</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.128</v>
       </c>
       <c r="G13" t="s">
@@ -8613,7 +8611,6 @@
         <v>0.02</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="G14" t="s">
@@ -8638,7 +8635,7 @@
         <v>0.05</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
       <c r="G15" t="s">
@@ -8663,7 +8660,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="G16" t="s">
@@ -8688,7 +8685,7 @@
         <v>0.13</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.13</v>
       </c>
       <c r="G17" t="s">
@@ -8713,7 +8710,7 @@
         <v>0.128</v>
       </c>
       <c r="F18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.128</v>
       </c>
       <c r="G18" t="s">
@@ -8738,7 +8735,6 @@
         <v>0.02</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" si="2"/>
         <v>0.02</v>
       </c>
       <c r="G19" t="s">
@@ -8763,7 +8759,7 @@
         <v>-0.24</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.24</v>
       </c>
       <c r="G20" t="s">
@@ -8788,7 +8784,7 @@
         <v>0.12</v>
       </c>
       <c r="F21" s="6">
-        <f t="shared" ref="F21:F28" si="3">B21 - C21^2/2</f>
+        <f t="shared" ref="F21:F28" si="4">B21 - C21^2/2</f>
         <v>0.12</v>
       </c>
       <c r="G21" t="s">
@@ -8813,7 +8809,7 @@
         <v>0.13</v>
       </c>
       <c r="F22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13</v>
       </c>
       <c r="G22" t="s">
@@ -8838,7 +8834,7 @@
         <v>0.11</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
       <c r="G23" t="s">
@@ -8863,7 +8859,7 @@
         <v>0.05</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="G24" t="s">
@@ -8888,7 +8884,7 @@
         <v>0.13</v>
       </c>
       <c r="F25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13</v>
       </c>
       <c r="G25" t="s">
@@ -8909,11 +8905,11 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" ref="E26:E32" si="4">F26</f>
+        <f t="shared" ref="E26:E32" si="5">F26</f>
         <v>0.128</v>
       </c>
       <c r="F26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.128</v>
       </c>
       <c r="G26" t="s">
@@ -8934,11 +8930,10 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
       <c r="F27" s="6">
-        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
       <c r="G27" t="s">
@@ -8959,11 +8954,11 @@
         <v>1</v>
       </c>
       <c r="E28" s="4">
+        <f t="shared" si="5"/>
+        <v>-0.24</v>
+      </c>
+      <c r="F28" s="6">
         <f t="shared" si="4"/>
-        <v>-0.24</v>
-      </c>
-      <c r="F28" s="6">
-        <f t="shared" si="3"/>
         <v>-0.24</v>
       </c>
       <c r="G28" t="s">
@@ -8984,7 +8979,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.12</v>
       </c>
       <c r="F29" s="6">
@@ -9009,7 +9004,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.13</v>
       </c>
       <c r="F30" s="6">
@@ -9034,7 +9029,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.11</v>
       </c>
       <c r="F31" s="6">
@@ -9059,7 +9054,7 @@
         <v>26</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F32" s="6">

</xml_diff>

<commit_message>
update for symp 2
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB7E480-B4F4-4C68-889F-BB6A7763D8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D11B1F-B296-481D-B0A9-12EA312BBAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2535,10 +2537,10 @@
   <dimension ref="A3:BK59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4497,7 +4499,7 @@
         <v>344</v>
       </c>
       <c r="D20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0.3</v>
@@ -4678,7 +4680,7 @@
         <v>340</v>
       </c>
       <c r="D22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
         <v>0.3</v>
@@ -4738,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="Y22">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="Z22">
         <v>40</v>
@@ -4854,7 +4856,7 @@
         <v>341</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>0.3</v>
@@ -4914,7 +4916,7 @@
         <v>0</v>
       </c>
       <c r="Y23">
-        <v>0.15</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="Z23">
         <v>40</v>
@@ -5090,7 +5092,7 @@
         <v>0</v>
       </c>
       <c r="Y24">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
       <c r="Z24">
         <v>40</v>

</xml_diff>

<commit_message>
add figures for the final report
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D11B1F-B296-481D-B0A9-12EA312BBAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3782E033-A372-49DB-BEE5-D14832304808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -2537,10 +2537,10 @@
   <dimension ref="A3:BK59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="R5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4680,7 +4680,7 @@
         <v>340</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0.3</v>
@@ -4856,7 +4856,7 @@
         <v>341</v>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0.3</v>
@@ -5385,11 +5385,11 @@
       <c r="A27" s="167" t="s">
         <v>262</v>
       </c>
-      <c r="C27" s="167" t="s">
-        <v>130</v>
+      <c r="C27" t="s">
+        <v>344</v>
       </c>
       <c r="D27" s="167" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="167">
         <v>0.3</v>
@@ -10768,7 +10768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -11215,13 +11215,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6BF394-4CD7-4BCB-B328-ED95773294C9}">
   <dimension ref="B2:M44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" style="105" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="105" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="106" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="106" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="106" customWidth="1"/>

</xml_diff>